<commit_message>
run and update the excel
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -1100,25 +1100,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.04361083053488459</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.152259667467783</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>1.730736173241318</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.2088320629953279</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>35.10665008416099</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>0.04726521039170312</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>0.1608162633132601</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>1.876846892054885</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>0.217405635602445</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>36.55802913864838</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -1126,25 +1162,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.08399010310308568</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.2113187903242607</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>2.145265106764904</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.2898104606515881</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>40.98046976307042</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.08116345128157965</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.2069797492216358</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>2.296600666795835</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0.2848919993288327</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>40.19132040945326</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -1152,25 +1224,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.05237721390149574</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.1510755082777625</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>1.705198101452275</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.228860686666574</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>33.0516606476717</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.05516637829350945</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.1639225303051357</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>1.778948721274245</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0.234875239847689</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>35.46271918707125</v>
+      </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -2146,25 +2254,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>192.2762521125019</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>13.54307598179339</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>54.48326724911767</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>13.86637126693577</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>183.632550132453</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>165.0306622255378</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>12.55647366606213</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>50.92338674385622</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>12.84642604873191</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>182.652874380205</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -2172,25 +2316,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearRegression()}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>148.6116808240873</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>11.30694095599458</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>63.59851264640785</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>12.19063906545048</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>175.3274273786684</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>245.8592272192249</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>15.27411941473676</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>58.92915732946842</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>15.67989882681725</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>185.5180064732139</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -2198,25 +2378,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>181.2794340607661</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>13.44813636208137</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>60.36193658564193</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>13.46400512703282</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>183.5912080460261</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>195.3286086321815</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>13.93139020905613</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>62.73564751569906</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>13.97600116743632</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>184.0927527968756</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -3190,25 +3406,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>111.0213766172669</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>10.26383430783124</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>5.168401719429726</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>10.53666819337436</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>135.0008356871378</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>125.2387344669246</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>10.97396441931363</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>5.514657073939576</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>11.19101132458209</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>138.3296180687961</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -3216,25 +3468,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearRegression()}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>160.1426419695156</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>11.83947404910845</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>6.426702303041881</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>12.65474780347343</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>137.0959953914537</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>198.8904317540341</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>13.91618710504955</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>7.038071097381223</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>14.10285190144299</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>148.034817926583</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -3242,25 +3530,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>127.6320179538618</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>11.2533859497944</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>5.78778588882778</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>11.29743413142391</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>139.9883088153425</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>117.662586465981</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>10.74676729136119</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>5.437805454337338</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>10.84723865626552</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>137.9769009985856</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -4234,25 +4558,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>225.2219984690273</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>13.67475941230423</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.9144478121423754</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>15.00739812455934</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>173.2290789877207</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>225.6055514663967</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>13.6901020893697</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>0.9120029695156455</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>15.02017148591842</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>173.9011859584534</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -4260,25 +4620,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>222.4764756379618</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>13.5542118291853</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.9058657184211895</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>14.91564533092557</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>168.8623020400715</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>222.180312386199</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>13.55767510378079</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0.9266571333684611</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>14.90571408508157</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>169.9367457912961</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -4286,25 +4682,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>224.7899486449594</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>13.6526482367092</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.921287147866131</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>14.9929966532698</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>172.78951349507</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>224.7899486449594</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>13.6526482367092</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>0.921287147866131</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>14.9929966532698</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>172.78951349507</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -5276,25 +5708,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.05641594815704015</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.1761178338003387</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>20794897960969.17</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.2375204162951896</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>37.56236843279562</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>0.05641594815704015</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>0.1761178338003387</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>20794897960969.17</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>0.2375204162951896</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>37.56236843279562</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -5302,25 +5770,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.06079647329963422</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.1893892234855264</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>22481624472142.79</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.2465694086857375</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>39.35514479529489</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.06079647329963422</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.1893892234855264</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>22481624472142.79</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0.2465694086857375</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>39.35514479529489</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -5328,25 +5832,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.06795889771421494</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.1987242050508918</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>22069759901682.35</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.2606892742600181</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>41.22524476203199</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.06795889771421494</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.1987242050508918</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>22069759901682.35</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0.2606892742600181</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>41.22524476203199</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -6318,25 +6858,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>1.047588904092994</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.5859830227709439</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.6585066244636306</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>1.023517906092998</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>27.52132700130401</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>1.047588904092994</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>0.5859830227709439</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>0.6585066244636306</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>1.023517906092998</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>27.52132700130401</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -6344,25 +6920,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearRegression()}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>1.136575428094937</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.7008268560793711</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.6701065975371003</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>1.066102916277287</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>32.52689390998577</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearRegression()}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>1.136575428094937</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.7008268560793711</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0.6701065975371003</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>1.066102916277287</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>32.52689390998577</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -6370,25 +6982,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>1.034466283655863</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.6021847499277053</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.6300232566230564</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>1.017087156371499</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>28.13447459432926</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>1.034466283655863</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.6021847499277053</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>0.6300232566230564</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>1.017087156371499</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>28.13447459432926</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -7268,13 +7916,31 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.09736240869423027</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.2336080265182465</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>2.553395417997963</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.3120294997179437</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>44.0045332024833</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
@@ -7294,13 +7960,31 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.07989360955708616</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.213986169680463</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>2.427001931401164</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.2826545763950872</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>41.5600271337884</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
@@ -7320,13 +8004,31 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.06503124013457584</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.1860654772402059</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>2.359128422994464</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.2550122352644591</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>38.48154805038671</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
@@ -8146,13 +8848,31 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>1.734151076300294</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.8622584100892295</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.6907921906062401</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>1.316871700774337</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>38.31853571218099</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
@@ -8172,13 +8892,31 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.8929316923296909</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.4900667682577249</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.4883044999543502</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.94495062957262</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>24.4248324790963</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
@@ -8198,13 +8936,31 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.8345416247294862</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.6159076689970492</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.4822294738452215</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.9135324979055131</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>30.41621742985091</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
@@ -9096,25 +9852,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.05004410033828557</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.1517910197271224</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>1.540624600600262</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.2237053873698297</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>32.85276638023121</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>0.0492178532509725</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>0.1544079944156327</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>1.584324042802247</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>0.2218509708136805</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>33.01067277145971</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -9122,25 +9914,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.08359994475608624</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.2315220015110875</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>2.013967271202212</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.289136550363468</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>44.61751383155751</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.1038846064347096</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.264372105648231</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>2.094533209408047</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0.3223113501487492</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>50.15766734266793</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -9148,25 +9976,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.05319738039984293</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.1718979120342271</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>1.679792578048122</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.2306455731199776</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>36.50884421291477</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.05471926758680111</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.1766236371270891</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>1.734968601326935</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0.2339214987699957</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>36.71227582865131</v>
+      </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -10118,25 +10982,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0.04353373594887233</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0.1467893457761121</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>1.814889016605119</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.2086473962187698</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>32.62342469885509</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>0.04877119688664654</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>0.1565277963512166</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>1.912991647321364</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>0.2208420179373629</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>34.08851870319486</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -10144,25 +11044,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.08620517726681132</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.2422027420273067</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>2.356274916347361</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.2936071819060483</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>46.55229071735872</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.07868982005901613</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.2291585368008477</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>2.264008501423303</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0.2805170584100299</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>44.55972323886865</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -10170,25 +11106,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.0544965361078763</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.1567771709649858</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>1.870272243483558</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.2334449316388692</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>34.12981131062897</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.04672944159407549</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.1534962677700555</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>1.735817138793481</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0.2161699368415402</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>33.8084599886319</v>
+      </c>
     </row>
     <row r="16" ht="121.5" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -11143,25 +12115,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.800778029232982</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.5276992810432793</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.4424792978410539</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.8948620168679537</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>27.03837156993348</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.76623490418525</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.573010279535794</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0.4341017733885329</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0.8753484472969892</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>29.67386566157197</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -11169,25 +12177,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.7740036635110037</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.4954687260375205</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.4400928114430226</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.8797747799925864</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>25.458718904941</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.8009404985107926</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.4864442413617613</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>0.4420418794325146</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0.8949527912190635</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>25.0221612072595</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -11195,25 +12239,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n"/>
-      <c r="C16" s="5" t="n"/>
-      <c r="D16" s="5" t="n"/>
-      <c r="E16" s="5" t="n"/>
-      <c r="F16" s="5" t="n"/>
-      <c r="G16" s="5" t="n"/>
-      <c r="H16" s="5" t="n"/>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>0.9167982938451932</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0.6082090843875482</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0.4801197979694892</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0.9574958453409567</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>29.58617021469036</v>
+      </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J16" s="8" t="n"/>
-      <c r="K16" s="8" t="n"/>
-      <c r="L16" s="8" t="n"/>
-      <c r="M16" s="8" t="n"/>
-      <c r="N16" s="8" t="n"/>
-      <c r="O16" s="8" t="n"/>
-      <c r="P16" s="8" t="n"/>
+      <c r="J16" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K16" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
+        </is>
+      </c>
+      <c r="L16" s="8" t="n">
+        <v>0.8960020466533004</v>
+      </c>
+      <c r="M16" s="8" t="n">
+        <v>0.5994270290849186</v>
+      </c>
+      <c r="N16" s="8" t="n">
+        <v>0.4622802578521346</v>
+      </c>
+      <c r="O16" s="8" t="n">
+        <v>0.9465738463814117</v>
+      </c>
+      <c r="P16" s="8" t="n">
+        <v>29.51141083010795</v>
+      </c>
     </row>
     <row r="17" ht="60.75" customHeight="1">
       <c r="A17" s="6" t="inlineStr">
@@ -12168,25 +13248,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.6626170659601728</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.5151033657254422</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.4457786952589812</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.8140129396761288</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>26.55682590630345</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.8429000344772248</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.5633931428170731</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0.470249357765031</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0.9180958743384183</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>30.0017771918978</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -12194,25 +13310,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.7600549759745411</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.4695381177076497</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.4781118131199529</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.871811319021806</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>23.85663915986686</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.7365982107783461</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.4231269955855145</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>0.463689919512996</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0.8582529992830471</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>22.13258082574935</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -12220,25 +13372,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n"/>
-      <c r="C16" s="5" t="n"/>
-      <c r="D16" s="5" t="n"/>
-      <c r="E16" s="5" t="n"/>
-      <c r="F16" s="5" t="n"/>
-      <c r="G16" s="5" t="n"/>
-      <c r="H16" s="5" t="n"/>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>0.777453684037718</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0.5950249735707045</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0.4959576739828901</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0.881733340663558</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>29.33639131600205</v>
+      </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J16" s="8" t="n"/>
-      <c r="K16" s="8" t="n"/>
-      <c r="L16" s="8" t="n"/>
-      <c r="M16" s="8" t="n"/>
-      <c r="N16" s="8" t="n"/>
-      <c r="O16" s="8" t="n"/>
-      <c r="P16" s="8" t="n"/>
+      <c r="J16" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K16" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L16" s="8" t="n">
+        <v>0.7629493733225143</v>
+      </c>
+      <c r="M16" s="8" t="n">
+        <v>0.5840707899764573</v>
+      </c>
+      <c r="N16" s="8" t="n">
+        <v>0.4921110943194993</v>
+      </c>
+      <c r="O16" s="8" t="n">
+        <v>0.8734697323448102</v>
+      </c>
+      <c r="P16" s="8" t="n">
+        <v>28.88021649054867</v>
+      </c>
     </row>
     <row r="17" ht="60.75" customHeight="1">
       <c r="A17" s="6" t="inlineStr">
@@ -13193,25 +14381,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.7805909050741481</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.5330130488948146</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.4582542155941546</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.8835105574208766</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>27.36138813766305</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>0.8187816827305214</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>0.5690303422838872</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0.4554235844819229</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0.9048655605837375</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>29.83827327062981</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
@@ -13219,25 +14443,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>0.857400264819111</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>0.4577205626813853</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.4706255460361808</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>0.9259591053708102</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>23.24729719627171</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>0.8479665416834432</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0.4626270198380099</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>0.4713226750533187</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0.9208509877735068</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>23.48915373154582</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -13245,25 +14505,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n"/>
-      <c r="C16" s="5" t="n"/>
-      <c r="D16" s="5" t="n"/>
-      <c r="E16" s="5" t="n"/>
-      <c r="F16" s="5" t="n"/>
-      <c r="G16" s="5" t="n"/>
-      <c r="H16" s="5" t="n"/>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>0.799833318916699</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0.5737772453101366</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0.4655795174959742</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>0.8943340085877864</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>28.7136418165221</v>
+      </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J16" s="8" t="n"/>
-      <c r="K16" s="8" t="n"/>
-      <c r="L16" s="8" t="n"/>
-      <c r="M16" s="8" t="n"/>
-      <c r="N16" s="8" t="n"/>
-      <c r="O16" s="8" t="n"/>
-      <c r="P16" s="8" t="n"/>
+      <c r="J16" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K16" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L16" s="8" t="n">
+        <v>0.8130570470303361</v>
+      </c>
+      <c r="M16" s="8" t="n">
+        <v>0.5865424832187879</v>
+      </c>
+      <c r="N16" s="8" t="n">
+        <v>0.4757191984887919</v>
+      </c>
+      <c r="O16" s="8" t="n">
+        <v>0.9016967600198728</v>
+      </c>
+      <c r="P16" s="8" t="n">
+        <v>29.17759743838515</v>
+      </c>
     </row>
     <row r="17" ht="60.75" customHeight="1">
       <c r="A17" s="6" t="inlineStr">
@@ -14237,25 +15533,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>225.5477101849752</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>13.68383102913718</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.9079235671735688</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>15.01824590905926</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>173.1259242776922</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>224.876921707674</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>13.6638187281175</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>0.9168008811041889</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>14.99589682905541</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>173.2437250732445</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -14263,25 +15595,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>223.0518785930658</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>13.5884938356678</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0.9350791802723485</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>14.93492144582843</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>170.9411587467795</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>223.4012794426272</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>13.58659424970684</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0.9153848039904513</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>14.9466143137042</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>169.961726888576</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -14289,25 +15657,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>224.7899486449594</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>13.6526482367092</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0.921287147866131</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>14.9929966532698</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>172.78951349507</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>224.7899486449594</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>13.6526482367092</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>0.921287147866131</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>14.9929966532698</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>172.78951349507</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -15283,25 +16687,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>172.494531274657</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>12.91901581177114</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>56.00499028049325</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>13.13371734409786</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>183.1515521943148</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 200}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>164.0562667907667</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>12.29572927167462</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>48.24461346851991</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>12.80844513556453</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>181.565067072978</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -15309,25 +16749,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>209.3577514391281</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>14.23460009359095</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>63.41178715739733</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>14.46920009672712</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>184.2106164107108</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearRegression()}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>165.7655167788964</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>11.74709006815314</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>67.41054314122432</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>12.87499579723801</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>175.3013952298899</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -15335,25 +16811,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>188.8010979219683</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>13.66373234036774</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>63.31831316366728</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>13.74049118197629</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>183.7739422809657</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>184.38714840905</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>13.50077711458334</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>60.53768062414295</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>13.5789229473125</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>183.7025283879853</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">
@@ -16327,25 +17839,61 @@
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
-      <c r="D13" s="5" t="n"/>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
-      <c r="H13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>125.9485770583523</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>11.04590824860999</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>5.499150984071545</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>11.22268136669452</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>138.9630160795865</v>
+      </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
           <t>Voting Regressor</t>
         </is>
       </c>
-      <c r="J13" s="8" t="n"/>
-      <c r="K13" s="8" t="n"/>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
-      <c r="P13" s="8" t="n"/>
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="inlineStr">
+        <is>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+        </is>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>118.7069701200986</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>10.69279433478641</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>5.279967138717829</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>10.89527283366959</v>
+      </c>
+      <c r="P13" s="8" t="n">
+        <v>137.7460750645692</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
@@ -16353,25 +17901,61 @@
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearRegression()}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>113.1509966361781</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>9.988700966326487</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>5.47331077521501</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>10.63724572604102</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>130.1583684656321</v>
+      </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
           <t>Stacking Regressor</t>
         </is>
       </c>
-      <c r="J14" s="8" t="n"/>
-      <c r="K14" s="8" t="n"/>
-      <c r="L14" s="8" t="n"/>
-      <c r="M14" s="8" t="n"/>
-      <c r="N14" s="8" t="n"/>
-      <c r="O14" s="8" t="n"/>
-      <c r="P14" s="8" t="n"/>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>145.8441246753081</v>
+      </c>
+      <c r="M14" s="8" t="n">
+        <v>12.0316605442504</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>6.139596774032428</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>12.07659408423203</v>
+      </c>
+      <c r="P14" s="8" t="n">
+        <v>142.7612197618481</v>
+      </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
       <c r="A15" s="6" t="inlineStr">
@@ -16379,25 +17963,61 @@
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="B15" s="5" t="n"/>
-      <c r="C15" s="5" t="n"/>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="5" t="n"/>
-      <c r="G15" s="5" t="n"/>
-      <c r="H15" s="5" t="n"/>
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>129.4585869269867</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>11.32940585468695</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>5.785575401389575</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <v>11.37798694528108</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <v>140.2759760292652</v>
+      </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
           <t>Gradient Boosting Regressor</t>
         </is>
       </c>
-      <c r="J15" s="8" t="n"/>
-      <c r="K15" s="8" t="n"/>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
-      <c r="P15" s="8" t="n"/>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>139.2742201764383</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>11.75203331009096</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>6.060149711916241</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>11.80144991839724</v>
+      </c>
+      <c r="P15" s="8" t="n">
+        <v>141.6609125972374</v>
+      </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
       <c r="A16" s="6" t="inlineStr">

</xml_diff>

<commit_message>
update result for adabosst
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -1348,25 +1348,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.05133368341445282</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.1651034353832049</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>2.239136661475503</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0.2265693788102285</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>35.15038612352898</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>0.05120525718238492</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>0.1606677460568164</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>2.223428807349505</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>0.2262857865231153</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>34.71974123106379</v>
+      </c>
     </row>
     <row r="18" ht="56" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -2502,25 +2538,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>185.4142371194634</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>13.5447441952645</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>61.42654128171799</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>13.61668965349006</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>183.6372972217531</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>176.5978626037236</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>13.04754572656535</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>55.80796655210585</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>13.28901285286923</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>182.9207971898298</v>
+      </c>
     </row>
     <row r="18" ht="28" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -3654,25 +3726,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>112.1397331729322</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>10.38577611414401</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>5.345266419501679</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>10.58960495830379</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>135.6896745821867</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 50, 'loss': 'linear', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>112.9603765933375</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>10.52524816753306</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>5.259894291950213</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>10.62828192105091</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>137.2911285399592</v>
+      </c>
     </row>
     <row r="18" ht="42" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -4806,25 +4914,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>224.7056127506848</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>13.65605126040622</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0.9285363549858882</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>14.99018387981564</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>173.2832862864289</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>224.8832373306709</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>13.66463256302335</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>0.923264033337865</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>14.99610740594608</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>173.6363267716511</v>
+      </c>
     </row>
     <row r="18" ht="56" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -5956,25 +6100,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 50, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.05851591976532541</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.1745337953102407</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>19665830818956.19</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0.2419006402747322</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>36.95896371775796</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 50, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>0.05851591976532541</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>0.1745337953102407</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>19665830818956.19</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>0.2419006402747322</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>36.95896371775796</v>
+      </c>
     </row>
     <row r="18" ht="42" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -7106,25 +7286,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 300, 'loss': 'exponential', 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>1.095564342962908</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.5442014133626787</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0.664642900026665</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>1.046692095586332</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>25.62284556156876</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 300, 'loss': 'exponential', 'learning_rate': 0.05}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>1.095564342962908</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>0.5442014133626787</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>0.664642900026665</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>1.046692095586332</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>25.62284556156876</v>
+      </c>
     </row>
     <row r="18" ht="42" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -8092,13 +8308,31 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.06194606875428836</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.1679493884227006</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>2.547318089279239</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0.2488896718513815</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>33.89431278675</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
@@ -9024,13 +9258,31 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.8602006447923788</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.4943774276226495</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0.4495336526081964</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0.9274700236624248</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>25.0402860336859</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
@@ -10100,25 +10352,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.05772291600081485</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.176992925192152</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>1.564684684741948</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0.2402559385339202</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>36.41469485531299</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 200, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>0.05819278115104796</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>0.1756666749800065</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>1.87924345769138</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>0.2412317996265168</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>35.87310981994763</v>
+      </c>
     </row>
     <row r="18" ht="42" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -11230,25 +11518,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.05672008610435777</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.1670138588136524</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>1.966522360897971</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0.2381597911158762</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>34.9333269255115</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>0.06222770305510863</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>0.1741268946637178</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>2.117770472749085</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>0.2494548116495423</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>35.54875016046574</v>
+      </c>
     </row>
     <row r="18" ht="42" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -12363,25 +12687,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.9857003547059051</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.5239328072220621</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0.4939599463435503</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.992824432971865</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>25.41051108615162</v>
+      </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J18" s="8" t="n"/>
-      <c r="K18" s="8" t="n"/>
-      <c r="L18" s="8" t="n"/>
-      <c r="M18" s="8" t="n"/>
-      <c r="N18" s="8" t="n"/>
-      <c r="O18" s="8" t="n"/>
-      <c r="P18" s="8" t="n"/>
+      <c r="J18" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="L18" s="8" t="n">
+        <v>0.9602393913429583</v>
+      </c>
+      <c r="M18" s="8" t="n">
+        <v>0.5183342315710838</v>
+      </c>
+      <c r="N18" s="8" t="n">
+        <v>0.4906317919934912</v>
+      </c>
+      <c r="O18" s="8" t="n">
+        <v>0.9799180533814847</v>
+      </c>
+      <c r="P18" s="8" t="n">
+        <v>25.31664377700406</v>
+      </c>
     </row>
     <row r="19" ht="42" customHeight="1">
       <c r="A19" s="6" t="inlineStr">
@@ -13496,25 +13856,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.8686468802038639</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.4997667529084262</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0.5178115819982123</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.9320122747066499</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>24.59483079678612</v>
+      </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J18" s="8" t="n"/>
-      <c r="K18" s="8" t="n"/>
-      <c r="L18" s="8" t="n"/>
-      <c r="M18" s="8" t="n"/>
-      <c r="N18" s="8" t="n"/>
-      <c r="O18" s="8" t="n"/>
-      <c r="P18" s="8" t="n"/>
+      <c r="J18" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="L18" s="8" t="n">
+        <v>0.8784103897013205</v>
+      </c>
+      <c r="M18" s="8" t="n">
+        <v>0.5132829883883131</v>
+      </c>
+      <c r="N18" s="8" t="n">
+        <v>0.5228411345714549</v>
+      </c>
+      <c r="O18" s="8" t="n">
+        <v>0.9372355038629941</v>
+      </c>
+      <c r="P18" s="8" t="n">
+        <v>25.1052199623789</v>
+      </c>
     </row>
     <row r="19" ht="42" customHeight="1">
       <c r="A19" s="6" t="inlineStr">
@@ -14629,25 +15025,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="5" t="n"/>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
-      <c r="H18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>0.9144438987047983</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.4993077249817766</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0.4939129757919268</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>0.9562656005027046</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>24.69096067914505</v>
+      </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J18" s="8" t="n"/>
-      <c r="K18" s="8" t="n"/>
-      <c r="L18" s="8" t="n"/>
-      <c r="M18" s="8" t="n"/>
-      <c r="N18" s="8" t="n"/>
-      <c r="O18" s="8" t="n"/>
-      <c r="P18" s="8" t="n"/>
+      <c r="J18" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="L18" s="8" t="n">
+        <v>0.938794687777585</v>
+      </c>
+      <c r="M18" s="8" t="n">
+        <v>0.5163865870553167</v>
+      </c>
+      <c r="N18" s="8" t="n">
+        <v>0.5056595857986339</v>
+      </c>
+      <c r="O18" s="8" t="n">
+        <v>0.9689141797793988</v>
+      </c>
+      <c r="P18" s="8" t="n">
+        <v>25.22943117244068</v>
+      </c>
     </row>
     <row r="19" ht="42" customHeight="1">
       <c r="A19" s="6" t="inlineStr">
@@ -15781,25 +16213,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>223.4342044569902</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>13.62016492467195</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0.9177416095990379</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>14.94771569360985</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>172.6546174454353</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>224.2512272359723</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>13.64128794978036</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>0.9213330043121857</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>14.97502010803232</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>172.6054501967378</v>
+      </c>
     </row>
     <row r="18" ht="42" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -16935,25 +17403,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'linear', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>173.2607485762262</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>13.10980668850248</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>60.41793197782881</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>13.16285487940311</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>183.2559811458397</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 50, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>150.1079608429256</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>12.1033868890715</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>52.88966070007036</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>12.25185540409801</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>181.6400837838315</v>
+      </c>
     </row>
     <row r="18" ht="28" customHeight="1">
       <c r="A18" s="6" t="inlineStr">
@@ -18087,25 +18591,61 @@
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
-      <c r="C17" s="5" t="n"/>
-      <c r="D17" s="5" t="n"/>
-      <c r="E17" s="5" t="n"/>
-      <c r="F17" s="5" t="n"/>
-      <c r="G17" s="5" t="n"/>
-      <c r="H17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 50, 'loss': 'linear', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>126.7749298083672</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>11.12154799306095</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>5.702124351294703</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>11.25943736642143</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>139.0066724549143</v>
+      </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
           <t>AdaBoostRegressor</t>
         </is>
       </c>
-      <c r="J17" s="8" t="n"/>
-      <c r="K17" s="8" t="n"/>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
-      <c r="P17" s="8" t="n"/>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
+          <t>{'n_estimators': 400, 'loss': 'linear', 'learning_rate': 0.01}</t>
+        </is>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>120.7181582392292</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>10.9214830315794</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>5.583839654009876</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>10.98718154210757</v>
+      </c>
+      <c r="P17" s="8" t="n">
+        <v>138.7494674485191</v>
+      </c>
     </row>
     <row r="18" ht="56" customHeight="1">
       <c r="A18" s="6" t="inlineStr">

</xml_diff>

<commit_message>
add MLP and changed read_train
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -1678,25 +1678,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.07838523387908936</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.215093806385994</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>2.577588558197021</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2799736306852654</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>40.89487195014954</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.08215077221393585</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2195072770118713</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>2.674199819564819</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2866195600686315</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>40.85392653942108</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -2904,25 +2940,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>220.8598022460938</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>14.85894680023193</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>67.21656799316406</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>14.86135263850817</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>185.0137591362</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': Tanh(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>238.7121276855469</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>15.44793796539307</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>69.78421783447266</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>15.45031157244238</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>185.5399012565613</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -4128,25 +4200,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>225.9319763183594</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>15.00244426727295</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>7.622591495513916</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>15.03103377410747</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>151.177179813385</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>133.8338623046875</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>11.53218555450439</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>5.922179222106934</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>11.56865862166775</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>140.9954428672791</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -5352,25 +5460,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>221.8839416503906</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>13.55358409881592</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.919352650642395</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>14.89576925339509</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>170.1185345649719</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>221.9650421142578</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>13.55808067321777</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.9219601154327393</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>14.89849126973123</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>170.1954245567322</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -6574,25 +6718,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.08294864743947983</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2235938757658005</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>29775519285248</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2880080683583011</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>43.07083785533905</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.08614324778318405</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2296033203601837</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>30235582005248</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2935016997960728</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>43.15841794013977</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -7796,25 +7976,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>1.209032416343689</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.5945903062820435</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.7156850695610046</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>1.099560101287642</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>26.51034593582153</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>1.169228196144104</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.6135646104812622</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.706624448299408</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>1.081308557324922</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>30.0974428653717</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -8782,13 +8998,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.08387590944766998</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2306056022644043</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>2.468596935272217</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2896133792621984</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>41.43242239952087</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -9750,13 +9984,31 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.9527064561843872</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.5113569498062134</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.5067695379257202</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.9760668297736519</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>25.04952549934387</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
@@ -10934,25 +11186,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.07530313730239868</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2082056403160095</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>2.210495471954346</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2744141711034594</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>41.23804569244385</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.07020536065101624</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2018416970968246</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>2.061851263046265</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2649629420334403</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>41.15466177463531</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -12136,25 +12424,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>0.07684499770402908</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>0.2159523963928223</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>2.456914663314819</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>0.2772093030618364</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>40.13096690177917</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>0.07276012003421783</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>0.2020772397518158</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>2.508364915847778</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>0.2697408386474281</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>40.30642807483673</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -13341,25 +13665,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.9624125957489014</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.5236716270446777</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.4887340068817139</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.9810262971750051</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>25.3871887922287</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.9571841955184937</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.5163381695747375</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.4868794977664948</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.9783579076792366</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>25.36321878433228</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -14546,25 +14906,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.8795596361160278</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.5047705173492432</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.5202772617340088</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.9378484078549304</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>25.02793967723846</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.8720538020133972</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.5051361918449402</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.5180037021636963</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.9338382097630173</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>24.99433308839798</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -15751,25 +16147,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B23" s="5" t="n"/>
-      <c r="C23" s="5" t="n"/>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="5" t="n"/>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.9536649584770203</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.5118158459663391</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.5077627897262573</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.9765577087284808</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>24.98691529035568</v>
+      </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J23" s="8" t="n"/>
-      <c r="K23" s="8" t="n"/>
-      <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
-      <c r="N23" s="8" t="n"/>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="8" t="n"/>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>0.9326292276382446</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>0.5089412331581116</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <v>0.502464771270752</v>
+      </c>
+      <c r="O23" s="8" t="n">
+        <v>0.9657273050081191</v>
+      </c>
+      <c r="P23" s="8" t="n">
+        <v>24.97279196977615</v>
+      </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
       <c r="A24" s="6" t="inlineStr">
@@ -16975,25 +17407,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>221.9242401123047</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>13.55620574951172</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0.9227257370948792</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>14.89712187344605</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>170.1274991035461</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>221.9751586914062</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>13.55815315246582</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>0.9227643609046936</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>14.89883078269588</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>170.1757669448853</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -18201,25 +18669,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': Tanh(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>239.0968475341797</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>15.46049022674561</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>69.87956237792969</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>15.46275678959543</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>185.5507731437683</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>167.5979766845703</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>12.94260406494141</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>58.66448211669922</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>12.94596372173854</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>182.9998135566711</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">
@@ -19425,25 +19929,61 @@
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="5" t="n"/>
-      <c r="G22" s="5" t="n"/>
-      <c r="H22" s="5" t="n"/>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': Tanh(), 'lr': 0.02}</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="n">
+        <v>190.3064880371094</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>13.7652006149292</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>7.015673637390137</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <v>13.7951617619044</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <v>147.9785799980164</v>
+      </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
           <t>Multilayer Perceptron</t>
         </is>
       </c>
-      <c r="J22" s="8" t="n"/>
-      <c r="K22" s="8" t="n"/>
-      <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
-      <c r="N22" s="8" t="n"/>
-      <c r="O22" s="8" t="n"/>
-      <c r="P22" s="8" t="n"/>
+      <c r="J22" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K22" s="8" t="inlineStr">
+        <is>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
+        </is>
+      </c>
+      <c r="L22" s="8" t="n">
+        <v>179.9839782714844</v>
+      </c>
+      <c r="M22" s="8" t="n">
+        <v>13.38486957550049</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <v>6.830113410949707</v>
+      </c>
+      <c r="O22" s="8" t="n">
+        <v>13.41581075714339</v>
+      </c>
+      <c r="P22" s="8" t="n">
+        <v>146.9086766242981</v>
+      </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
       <c r="A23" s="6" t="inlineStr">

</xml_diff>

<commit_message>
add CNN, cant run on KPCA data
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="805" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Option 1 - LR1 - DN1 (80-20)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Option 1 - LR1 - DN1 (60-40)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Option 1 - LR1 - DN1 (70-30)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Option 1 - LR1 - DN2 (80-20)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Option 1 - LR1 - DN2 (60-40)" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Option 1 - LR1 - DN2 (70-30)" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Option 1 - LR2 - DN1 (80-20)" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Option 1 - LR2 - DN1 (60-40)" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Option 1 - LR2 - DN1 (70-30)" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Option 1 - LR2 - DN2 (60-40)" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Option 1 - LR2 - DN2 (70-30)" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Option 1 - LR2 - DN2 (80-20)" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Option 1 - NLR1 - DN1 (70-30)" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Option 1 - NLR1 - DN2 (70-30)" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Option 1 - NLR2 - DN1 (70-30)" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Option 1 - NLR2 - DN2 (70-30)" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN1 (80-20)" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN1 (60-40)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN1 (70-30)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN2 (80-20)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN2 (60-40)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR1 - DN2 (70-30)" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN1 (80-20)" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN1 (60-40)" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN1 (70-30)" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN2 (60-40)" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN2 (70-30)" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - LR2 - DN2 (80-20)" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR1 - DN1 (70-30)" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR1 - DN2 (70-30)" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR2 - DN1 (70-30)" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Option 1 - NLR2 - DN2 (70-30)" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1838,25 +1838,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.06672632694244385</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.1865313649177551</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>2.241897106170654</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0.258314395538545</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>37.19305694103241</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>0.07476578652858734</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>0.2113934755325317</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>2.270585775375366</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>0.2734333310490646</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>41.74971282482147</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3116,25 +3152,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>493.8932189941406</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>22.20759391784668</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>99.38224792480469</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>22.22370848877704</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>189.666736125946</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>405.25927734375</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>20.10616683959961</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>89.31976318359375</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>20.13105256422898</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>188.6757493019104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4392,25 +4464,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>231.982177734375</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>15.19534015655518</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>7.710440158843994</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>15.23096115596041</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>151.6064405441284</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>298.8934936523438</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>17.25723075866699</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>8.698757171630859</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>17.288536480927</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>156.100857257843</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5668,25 +5776,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>223.1090240478516</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>13.59994029998779</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>0.9138834476470947</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>14.93683447213135</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>171.2110042572021</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>218.0384216308594</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>13.42439651489258</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>0.9199987649917603</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>14.76612412350849</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>166.641902923584</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9220,13 +9364,31 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.204253762960434</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.3202943801879883</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>3.557053327560425</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0.4519444246369613</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>47.6514995098114</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
@@ -10224,13 +10386,31 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>2.105569839477539</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.9695848226547241</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>0.8032482266426086</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>1.451058179218717</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>37.03500330448151</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
@@ -11498,25 +11678,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.08108207583427429</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.1826180219650269</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>2.268268346786499</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0.2847491454495945</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>35.57400107383728</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>0.06733357906341553</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>0.1812693327665329</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>2.118668079376221</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>0.2594871462392994</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>36.37834191322327</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12772,25 +12988,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.06867791712284088</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.1685656309127808</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>2.543929815292358</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0.2620647193401677</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>33.71310532093048</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>0.07128681987524033</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>0.1777063310146332</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>2.52039909362793</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>0.2669959173381502</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>35.10835766792297</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14049,25 +14301,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n"/>
-      <c r="C25" s="5" t="n"/>
-      <c r="D25" s="5" t="n"/>
-      <c r="E25" s="5" t="n"/>
-      <c r="F25" s="5" t="n"/>
-      <c r="G25" s="5" t="n"/>
-      <c r="H25" s="5" t="n"/>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>1.198211789131165</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>0.6169342994689941</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>0.5674945712089539</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>1.094628607853442</v>
+      </c>
+      <c r="H25" s="5" t="n">
+        <v>28.00677120685577</v>
+      </c>
       <c r="I25" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J25" s="8" t="n"/>
-      <c r="K25" s="8" t="n"/>
-      <c r="L25" s="8" t="n"/>
-      <c r="M25" s="8" t="n"/>
-      <c r="N25" s="8" t="n"/>
-      <c r="O25" s="8" t="n"/>
-      <c r="P25" s="8" t="n"/>
+      <c r="J25" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K25" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L25" s="8" t="n">
+        <v>0.9754546880722046</v>
+      </c>
+      <c r="M25" s="8" t="n">
+        <v>0.5227827429771423</v>
+      </c>
+      <c r="N25" s="8" t="n">
+        <v>0.4932146966457367</v>
+      </c>
+      <c r="O25" s="8" t="n">
+        <v>0.9876510963251165</v>
+      </c>
+      <c r="P25" s="8" t="n">
+        <v>25.44384002685547</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15326,25 +15614,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n"/>
-      <c r="C25" s="5" t="n"/>
-      <c r="D25" s="5" t="n"/>
-      <c r="E25" s="5" t="n"/>
-      <c r="F25" s="5" t="n"/>
-      <c r="G25" s="5" t="n"/>
-      <c r="H25" s="5" t="n"/>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>1.003121137619019</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>0.543346643447876</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>0.555172860622406</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>1.001559353018591</v>
+      </c>
+      <c r="H25" s="5" t="n">
+        <v>25.7503479719162</v>
+      </c>
       <c r="I25" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J25" s="8" t="n"/>
-      <c r="K25" s="8" t="n"/>
-      <c r="L25" s="8" t="n"/>
-      <c r="M25" s="8" t="n"/>
-      <c r="N25" s="8" t="n"/>
-      <c r="O25" s="8" t="n"/>
-      <c r="P25" s="8" t="n"/>
+      <c r="J25" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K25" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L25" s="8" t="n">
+        <v>0.8401133418083191</v>
+      </c>
+      <c r="M25" s="8" t="n">
+        <v>0.5114778280258179</v>
+      </c>
+      <c r="N25" s="8" t="n">
+        <v>0.5073946714401245</v>
+      </c>
+      <c r="O25" s="8" t="n">
+        <v>0.9165769699312323</v>
+      </c>
+      <c r="P25" s="8" t="n">
+        <v>25.28231739997864</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16603,25 +16927,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B25" s="5" t="n"/>
-      <c r="C25" s="5" t="n"/>
-      <c r="D25" s="5" t="n"/>
-      <c r="E25" s="5" t="n"/>
-      <c r="F25" s="5" t="n"/>
-      <c r="G25" s="5" t="n"/>
-      <c r="H25" s="5" t="n"/>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>0.810571551322937</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>0.635327935218811</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>0.4800490736961365</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <v>0.9003174725189649</v>
+      </c>
+      <c r="H25" s="5" t="n">
+        <v>31.66752755641937</v>
+      </c>
       <c r="I25" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J25" s="8" t="n"/>
-      <c r="K25" s="8" t="n"/>
-      <c r="L25" s="8" t="n"/>
-      <c r="M25" s="8" t="n"/>
-      <c r="N25" s="8" t="n"/>
-      <c r="O25" s="8" t="n"/>
-      <c r="P25" s="8" t="n"/>
+      <c r="J25" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K25" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L25" s="8" t="n">
+        <v>0.8663380742073059</v>
+      </c>
+      <c r="M25" s="8" t="n">
+        <v>0.6241239905357361</v>
+      </c>
+      <c r="N25" s="8" t="n">
+        <v>0.500713586807251</v>
+      </c>
+      <c r="O25" s="8" t="n">
+        <v>0.9307728370592396</v>
+      </c>
+      <c r="P25" s="8" t="n">
+        <v>30.59184551239014</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17879,25 +18239,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>220.3426361083984</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>13.50227165222168</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>0.9207553863525391</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>14.84394274134734</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>168.6696887016296</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>218.9997406005859</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>13.45299339294434</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>0.9174178838729858</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>14.79863982265215</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>167.0999884605408</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19157,25 +19553,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>380.690673828125</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>19.49611473083496</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>87.18663024902344</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>19.51129605710818</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>188.3451461791992</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>164.0846862792969</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>12.80196952819824</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>57.43050003051758</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>12.80955449183526</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>182.8518509864807</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20433,25 +20865,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>345.32080078125</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>18.54377937316895</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>9.379693984985352</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>18.58280928119454</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>158.4026098251343</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>161.2060241699219</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>12.64818000793457</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>6.481948852539062</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>12.69669343450971</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>144.6035146713257</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
re run the LR for option 1, fill new sheets for different datasets
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -770,19 +770,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.07170309606401425</v>
+        <v>0.07170309606401419</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>0.186292336975765</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.456033923310312</v>
+        <v>1.456033923310313</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2677743379489794</v>
+        <v>0.2677743379489793</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>41.18218322329804</v>
+        <v>41.18218322329802</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.08189086093339405</v>
+        <v>0.081890860933394</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.2045413624390392</v>
+        <v>0.2045413624390393</v>
       </c>
       <c r="N7" s="8" t="n">
         <v>1.72274655042239</v>
@@ -812,7 +812,7 @@
         <v>0.2861657927380455</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>44.16749192075862</v>
+        <v>44.16749192075866</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -2084,16 +2084,16 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>224.1674839411998</v>
+        <v>224.1674839412</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>13.68001563405001</v>
+        <v>13.68001563405002</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>42.34785977017865</v>
+        <v>42.34785977017866</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>14.97222374736631</v>
+        <v>14.97222374736632</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>182.9974054215934</v>
@@ -2114,16 +2114,16 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>229.0288486751149</v>
+        <v>229.0288486751145</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>13.60253792883092</v>
+        <v>13.60253792883091</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>40.87184629998021</v>
+        <v>40.87184629998013</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>15.13369910745932</v>
+        <v>15.1336991074593</v>
       </c>
       <c r="P7" s="8" t="n">
         <v>179.8795705216952</v>
@@ -3396,13 +3396,13 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>155.1159635610918</v>
+        <v>155.1159635610919</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>11.25363907279669</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>5.292135772446135</v>
+        <v>5.292135772446131</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>12.45455593592529</v>
@@ -3426,19 +3426,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>145.5107082302829</v>
+        <v>145.510708230283</v>
       </c>
       <c r="M7" s="8" t="n">
         <v>10.6674178031528</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>4.904539737636824</v>
+        <v>4.904539737636826</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>12.06278194407422</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>128.4071917291414</v>
+        <v>128.4071917291415</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -4714,13 +4714,13 @@
         <v>13.64991077201485</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.9204451719720371</v>
+        <v>0.9204451719720375</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>14.96260446636914</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>174.3664989276996</v>
+        <v>174.3664989276997</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -4744,13 +4744,13 @@
         <v>13.66895480473618</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.943431768184124</v>
+        <v>0.9434317681841236</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>14.97246538186103</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>179.483085501089</v>
+        <v>179.4830855010889</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -6007,25 +6007,61 @@
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.05842016526623228</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.1814459625699927</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>20722139914727.48</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.2417026381035844</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>37.66921234585003</v>
+      </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="J7" s="8" t="n"/>
-      <c r="K7" s="8" t="n"/>
-      <c r="L7" s="8" t="n"/>
-      <c r="M7" s="8" t="n"/>
-      <c r="N7" s="8" t="n"/>
-      <c r="O7" s="8" t="n"/>
-      <c r="P7" s="8" t="n"/>
+      <c r="J7" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K7" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>0.05842016526623228</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <v>0.1814459625699927</v>
+      </c>
+      <c r="N7" s="8" t="n">
+        <v>20722139914727.48</v>
+      </c>
+      <c r="O7" s="8" t="n">
+        <v>0.2417026381035844</v>
+      </c>
+      <c r="P7" s="8" t="n">
+        <v>37.66921234585003</v>
+      </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
@@ -7256,7 +7292,7 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0564659096743711</v>
+        <v>0.05646590967437108</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>0.1806374684935386</v>
@@ -7286,7 +7322,7 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0564659096743711</v>
+        <v>0.05646590967437108</v>
       </c>
       <c r="M7" s="8" t="n">
         <v>0.1806374684935386</v>
@@ -8530,19 +8566,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0564659096743711</v>
+        <v>0.05922356432069868</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1806374684935386</v>
+        <v>0.1858861652413798</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>22972839564223.58</v>
+        <v>24801660827758.78</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2376255661210954</v>
+        <v>0.2433589207748479</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>37.8091717418089</v>
+        <v>38.69262186983138</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -8560,19 +8596,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.0564659096743711</v>
+        <v>0.05660950470877726</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1806374684935386</v>
+        <v>0.1814901079323312</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>22972839564223.58</v>
+        <v>24656179578374.99</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2376255661210954</v>
+        <v>0.2379275198643008</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>37.8091717418089</v>
+        <v>38.19255996742378</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -9793,25 +9829,61 @@
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.9972854966527085</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.6083726915747472</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.5965976040668238</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.9986418260080581</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>29.23314770596295</v>
+      </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="J7" s="8" t="n"/>
-      <c r="K7" s="8" t="n"/>
-      <c r="L7" s="8" t="n"/>
-      <c r="M7" s="8" t="n"/>
-      <c r="N7" s="8" t="n"/>
-      <c r="O7" s="8" t="n"/>
-      <c r="P7" s="8" t="n"/>
+      <c r="J7" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K7" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>0.9994900133592056</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <v>0.6103894270354667</v>
+      </c>
+      <c r="N7" s="8" t="n">
+        <v>0.5971204879126394</v>
+      </c>
+      <c r="O7" s="8" t="n">
+        <v>0.9997449741605134</v>
+      </c>
+      <c r="P7" s="8" t="n">
+        <v>29.3415993157885</v>
+      </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
@@ -12305,25 +12377,61 @@
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>1.098046403166383</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.6181445844567487</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.6208096847378437</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>1.04787709354026</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>28.94298347310742</v>
+      </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="J7" s="8" t="n"/>
-      <c r="K7" s="8" t="n"/>
-      <c r="L7" s="8" t="n"/>
-      <c r="M7" s="8" t="n"/>
-      <c r="N7" s="8" t="n"/>
-      <c r="O7" s="8" t="n"/>
-      <c r="P7" s="8" t="n"/>
+      <c r="J7" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K7" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>1.098046403166383</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <v>0.6181445844567487</v>
+      </c>
+      <c r="N7" s="8" t="n">
+        <v>0.6208096847378437</v>
+      </c>
+      <c r="O7" s="8" t="n">
+        <v>1.04787709354026</v>
+      </c>
+      <c r="P7" s="8" t="n">
+        <v>28.94298347310742</v>
+      </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
@@ -13543,13 +13651,31 @@
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.09032232363439829</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.2434390558764038</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>1.30555807670287</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.3005367259327856</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>47.83910315568752</v>
+      </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Linear Regressor</t>
@@ -14570,7 +14696,7 @@
         <v>0.2282994639332527</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>33.128422439755</v>
+        <v>33.12842243975501</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -14588,13 +14714,13 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.05372609952304652</v>
+        <v>0.05372609952304654</v>
       </c>
       <c r="M7" s="8" t="n">
         <v>0.1657192252358889</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>1.411404403341891</v>
+        <v>1.41140440334189</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>0.2317889115618919</v>
@@ -15868,19 +15994,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.4294384111078768</v>
+        <v>0.4294384111078816</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.5187946743211793</v>
+        <v>0.5187946743211823</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>3.876475190047705</v>
+        <v>3.87647519004772</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.6553155050110419</v>
+        <v>0.6553155050110455</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>77.23363865710085</v>
+        <v>77.23363865710112</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -16879,13 +17005,31 @@
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>1.933087785218292</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>1.071452301097999</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>4.404460161408686</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>1.390355273021357</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>108.9582795732013</v>
+      </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Linear Regressor</t>
@@ -17883,13 +18027,31 @@
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>2.068307251458357</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.9191153329814845</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.7028178625532929</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>1.438161065895735</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>43.06246236397043</v>
+      </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Linear Regressor</t>
@@ -18898,7 +19060,7 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>7.37069434997466</v>
+        <v>7.370694349974656</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>1.536193477550144</v>
@@ -18910,7 +19072,7 @@
         <v>2.714902272637941</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>47.25990391674981</v>
+        <v>47.25990391674979</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -19909,13 +20071,31 @@
           <t>Linear Regressor</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
-      <c r="C7" s="5" t="n"/>
-      <c r="D7" s="5" t="n"/>
-      <c r="E7" s="5" t="n"/>
-      <c r="F7" s="5" t="n"/>
-      <c r="G7" s="5" t="n"/>
-      <c r="H7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>12.38513793352731</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>2.517627051576155</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>1.650520298717122</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>3.519252468000457</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>82.36634663912197</v>
+      </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
           <t>Linear Regressor</t>
@@ -20924,16 +21104,16 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.05107518501818602</v>
+        <v>0.05107518501818605</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>0.1411135151931689</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.629103238468468</v>
+        <v>1.629103238468466</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2259981969356968</v>
+        <v>0.2259981969356969</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>32.75030408043421</v>
@@ -20960,13 +21140,13 @@
         <v>0.1599121708056201</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>1.805127560762998</v>
+        <v>1.805127560762999</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>0.2424658769607383</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>35.48766046527</v>
+        <v>35.48766046527004</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -22237,19 +22417,19 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.7251027128430018</v>
+        <v>0.7251027128430022</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.5854098318913584</v>
+        <v>0.585409831891359</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.4325432641101764</v>
+        <v>0.4325432641101767</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.8515296312184337</v>
+        <v>0.8515296312184339</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>30.60342864762472</v>
+        <v>30.60342864762473</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -22267,16 +22447,16 @@
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>0.6133607290226011</v>
+        <v>0.6133607290226015</v>
       </c>
       <c r="M8" s="8" t="n">
         <v>0.5839077175462739</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>0.3805789482373465</v>
+        <v>0.3805789482373467</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>0.7831734986722936</v>
+        <v>0.7831734986722939</v>
       </c>
       <c r="P8" s="8" t="n">
         <v>31.9284412239871</v>
@@ -23550,19 +23730,19 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.6612258207487424</v>
+        <v>0.6612258207487418</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>0.5600757950868516</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.4480600826031109</v>
+        <v>0.448060082603111</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.8131579310003331</v>
+        <v>0.8131579310003327</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>28.87149778622366</v>
+        <v>28.87149778622365</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -23580,10 +23760,10 @@
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>0.8683025062912475</v>
+        <v>0.8683025062912474</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.7040932480537432</v>
+        <v>0.704093248053743</v>
       </c>
       <c r="N8" s="8" t="n">
         <v>0.480864130196735</v>
@@ -23592,7 +23772,7 @@
         <v>0.9318275088723489</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>35.24670787676123</v>
+        <v>35.24670787676127</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -24863,19 +25043,19 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.7245242636518847</v>
+        <v>0.7245242636518846</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.553589665257585</v>
+        <v>0.5535896652575847</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.4481368171205169</v>
+        <v>0.4481368171205167</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.8511899104500034</v>
+        <v>0.8511899104500033</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>28.78373952402107</v>
+        <v>28.78373952402106</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -24893,19 +25073,19 @@
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>0.7398949711337037</v>
+        <v>0.7398949711337043</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.5977392290146721</v>
+        <v>0.597739229014673</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>0.4195608739169494</v>
+        <v>0.4195608739169495</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>0.8601714777494681</v>
+        <v>0.8601714777494684</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>32.8196775600078</v>
+        <v>32.81967756000784</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -26181,13 +26361,13 @@
         <v>13.64745995574642</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.913588348989489</v>
+        <v>0.9135883489894892</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>14.96448038142695</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>173.3034872293751</v>
+        <v>173.3034872293752</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -26208,10 +26388,10 @@
         <v>223.8058861443396</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>13.64354821182386</v>
+        <v>13.64354821182387</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.9136043920115666</v>
+        <v>0.913604392011567</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>14.96014325280141</v>
@@ -27489,16 +27669,16 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>208.0932959243308</v>
+        <v>208.0932959243306</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>13.31867999251359</v>
+        <v>13.31867999251358</v>
       </c>
       <c r="F7" s="5" t="n">
         <v>46.55228556417578</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>14.42543919346412</v>
+        <v>14.42543919346411</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>182.2698618253632</v>
@@ -27519,19 +27699,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>220.8066486399369</v>
+        <v>220.806648639937</v>
       </c>
       <c r="M7" s="8" t="n">
         <v>13.46330233097094</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>41.95065002947821</v>
+        <v>41.95065002947818</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>14.85956421433472</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>181.7230175726124</v>
+        <v>181.7230175726125</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -28801,13 +28981,13 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>168.6872491478568</v>
+        <v>168.6872491478569</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>12.0801770609241</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>5.80141004897118</v>
+        <v>5.801410048971181</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>12.98796555076494</v>
@@ -28837,13 +29017,13 @@
         <v>12.1362341986298</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>5.650894614402512</v>
+        <v>5.650894614402508</v>
       </c>
       <c r="O7" s="8" t="n">
         <v>13.24340046772151</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>140.0434783690048</v>
+        <v>140.0434783690042</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">

</xml_diff>

<commit_message>
updates CNN for all datasets
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -7101,25 +7101,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.1014032140374184</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.2450904548168182</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>27880381743104</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0.3184387131575216</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>44.83312666416168</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>0.1102476418018341</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>0.2558545470237732</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>29177996640256</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>0.3320356032142248</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>45.93763649463654</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8375,25 +8411,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>0.07501772046089172</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>0.1971401125192642</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>26607699886080</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>0.2738936298289752</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>39.19986486434937</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>0.07061392068862915</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>0.2048145830631256</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>26526863065088</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>0.2657327994219553</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>41.04349613189697</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9649,25 +9721,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>1335200.375</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>884.6502075195312</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>6.286405333208269e+16</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>1155.508708318548</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>197.805392742157</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>0.08269235491752625</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>0.2210704982280731</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>32996390338560</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>0.2875627843054908</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>42.59116053581238</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10923,25 +11031,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>3.017023324966431</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>1.413211822509766</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>0.7693153023719788</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>1.736958066553833</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>68.37573051452637</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>4.010422229766846</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>1.706381797790527</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>0.956902027130127</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>2.00260386241684</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>84.01063680648804</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12197,25 +12341,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>4.31737232208252</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>1.782651305198669</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>0.9417372941970825</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>2.077828751866361</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>102.4152159690857</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>3.605465650558472</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>1.441632509231567</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>0.7818022966384888</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>1.898806375215354</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>60.18291711807251</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13471,25 +13651,61 @@
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
-      <c r="C24" s="5" t="n"/>
-      <c r="D24" s="5" t="n"/>
-      <c r="E24" s="5" t="n"/>
-      <c r="F24" s="5" t="n"/>
-      <c r="G24" s="5" t="n"/>
-      <c r="H24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>24.74347305297852</v>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>3.979507207870483</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>2.548369169235229</v>
+      </c>
+      <c r="G24" s="5" t="n">
+        <v>4.974281159421783</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>137.6319408416748</v>
+      </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
           <t>Convolutional neural network</t>
         </is>
       </c>
-      <c r="J24" s="8" t="n"/>
-      <c r="K24" s="8" t="n"/>
-      <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
-      <c r="N24" s="8" t="n"/>
-      <c r="O24" s="8" t="n"/>
-      <c r="P24" s="8" t="n"/>
+      <c r="J24" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K24" s="8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>3.568130970001221</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>1.415134429931641</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <v>1.059643030166626</v>
+      </c>
+      <c r="O24" s="8" t="n">
+        <v>1.888949700230586</v>
+      </c>
+      <c r="P24" s="8" t="n">
+        <v>56.30818605422974</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rerun option 1 for kpca
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -6018,19 +6018,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.05842016526623228</v>
+        <v>0.04934490442668437</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1814459625699927</v>
+        <v>0.1597061771726322</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>20722139914727.48</v>
+        <v>24703286042772.77</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2417026381035844</v>
+        <v>0.2221371297795224</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>37.66921234585003</v>
+        <v>34.26087042431212</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -6048,19 +6048,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.05842016526623228</v>
+        <v>0.04933841524590248</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1814459625699927</v>
+        <v>0.1587443171447075</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>20722139914727.48</v>
+        <v>24705183363896.26</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2417026381035844</v>
+        <v>0.2221225230495604</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>37.66921234585003</v>
+        <v>34.08336849254361</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -6076,23 +6076,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.070011206202778</v>
+        <v>0.05129250578218996</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.2080945798859079</v>
+        <v>0.1620744040834298</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>23309998460419.51</v>
+        <v>31029211527340.41</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.2645963079915856</v>
+        <v>0.226478488563903</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>41.62498215635366</v>
+        <v>35.96810689809151</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -6106,23 +6106,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>0.070011206202778</v>
+        <v>0.05279037341160148</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.2080945798859079</v>
+        <v>0.1663257440163751</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>23309998460419.51</v>
+        <v>31059593192428.9</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>0.2645963079915856</v>
+        <v>0.2297615577323619</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>41.62498215635366</v>
+        <v>36.64988662356566</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -6138,23 +6138,23 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>{'splitter': 'best', 'min_samples_split': 5, 'min_samples_leaf': 4, 'min_impurity_decrease': 0.1, 'max_leaf_nodes': 90, 'max_features': None, 'max_depth': 26, 'criterion': 'mae', 'ccp_alpha': 0.0}</t>
+          <t>{'splitter': 'best', 'min_samples_split': 2, 'min_samples_leaf': 1, 'min_impurity_decrease': 0.1, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': 7, 'criterion': 'friedman_mse', 'ccp_alpha': 0.0}</t>
         </is>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0.0712915219945261</v>
+        <v>0.07182882690808208</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>0.2091504123057637</v>
+        <v>0.1999718188871933</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>23820157658679.84</v>
+        <v>27003821152313.93</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>0.267004722794422</v>
+        <v>0.2680090052742297</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>41.61081967385951</v>
+        <v>40.49291951229772</v>
       </c>
       <c r="I9" s="9" t="inlineStr">
         <is>
@@ -6168,23 +6168,23 @@
       </c>
       <c r="K9" s="8" t="inlineStr">
         <is>
-          <t>{'splitter': 'best', 'min_samples_split': 5, 'min_samples_leaf': 4, 'min_impurity_decrease': 0.1, 'max_leaf_nodes': 90, 'max_features': None, 'max_depth': 26, 'criterion': 'mae', 'ccp_alpha': 0.0}</t>
+          <t>{'splitter': 'best', 'min_samples_split': 2, 'min_samples_leaf': 1, 'min_impurity_decrease': 0.1, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': 7, 'criterion': 'friedman_mse', 'ccp_alpha': 0.0}</t>
         </is>
       </c>
       <c r="L9" s="8" t="n">
-        <v>0.0712915219945261</v>
+        <v>0.07856640140243044</v>
       </c>
       <c r="M9" s="8" t="n">
-        <v>0.2091504123057637</v>
+        <v>0.2113196769567876</v>
       </c>
       <c r="N9" s="8" t="n">
-        <v>23820157658679.84</v>
+        <v>29966146605498.22</v>
       </c>
       <c r="O9" s="8" t="n">
-        <v>0.267004722794422</v>
+        <v>0.2802969878582901</v>
       </c>
       <c r="P9" s="8" t="n">
-        <v>41.61081967385951</v>
+        <v>41.26798569794828</v>
       </c>
     </row>
     <row r="10" ht="27.95" customHeight="1">
@@ -6200,23 +6200,23 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 2}</t>
+          <t>{'weights': 'distance', 'n_neighbors': 2}</t>
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0.06323856106945384</v>
+        <v>0.0684605369619242</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.1888433729421327</v>
+        <v>0.1724776075314736</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>19077989185279.11</v>
+        <v>26686048014663.68</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.2514727839537588</v>
+        <v>0.2616496454458217</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>40.69533945439992</v>
+        <v>34.17891686634869</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -6230,23 +6230,23 @@
       </c>
       <c r="K10" s="8" t="inlineStr">
         <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 2}</t>
+          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>0.06323856106945384</v>
+        <v>0.06087330246559607</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.1888433729421327</v>
+        <v>0.1638957781719567</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>19077989185279.11</v>
+        <v>30159887898440.89</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>0.2514727839537588</v>
+        <v>0.2467251557210899</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>40.69533945439992</v>
+        <v>34.06793441427384</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -6262,23 +6262,23 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>{'tol': 0.0001, 'power_t': 0.25, 'penalty': 'elasticnet', 'max_iter': 3000, 'loss': 'squared_loss', 'learning_rate': 'optimal', 'l1_ratio': 0, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 1}</t>
+          <t>{'tol': 0.0001, 'power_t': 0.5, 'penalty': 'l1', 'max_iter': 1000, 'loss': 'squared_loss', 'learning_rate': 'adaptive', 'l1_ratio': 0.15, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 0.001}</t>
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>0.068694679844423</v>
+        <v>0.1008476339381634</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>0.2075769179532206</v>
+        <v>0.2797587799467701</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>22574139692305.95</v>
+        <v>14806811800935.56</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>0.2620966994153552</v>
+        <v>0.317565164868824</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>41.7922548346248</v>
+        <v>63.21919905887252</v>
       </c>
       <c r="I11" s="9" t="inlineStr">
         <is>
@@ -6292,23 +6292,23 @@
       </c>
       <c r="K11" s="8" t="inlineStr">
         <is>
-          <t>{'tol': 0.0001, 'power_t': 0.25, 'penalty': 'elasticnet', 'max_iter': 3000, 'loss': 'squared_loss', 'learning_rate': 'optimal', 'l1_ratio': 0, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 1}</t>
+          <t>{'tol': 0.0001, 'power_t': 0.5, 'penalty': 'l1', 'max_iter': 1000, 'loss': 'squared_loss', 'learning_rate': 'adaptive', 'l1_ratio': 0.15, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 0.001}</t>
         </is>
       </c>
       <c r="L11" s="8" t="n">
-        <v>0.068694679844423</v>
+        <v>0.1087758623433754</v>
       </c>
       <c r="M11" s="8" t="n">
-        <v>0.2075769179532206</v>
+        <v>0.2932749384635216</v>
       </c>
       <c r="N11" s="8" t="n">
-        <v>22574139692305.95</v>
+        <v>14394575375713.41</v>
       </c>
       <c r="O11" s="8" t="n">
-        <v>0.2620966994153552</v>
+        <v>0.3298118590096109</v>
       </c>
       <c r="P11" s="8" t="n">
-        <v>41.7922548346248</v>
+        <v>68.08927144620176</v>
       </c>
     </row>
     <row r="12" ht="45.75" customHeight="1">
@@ -6406,23 +6406,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.0573943957492737</v>
+        <v>0.05648577145223542</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1817784585087612</v>
+        <v>0.1698174640905329</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>21114290799805.62</v>
+        <v>26396464820531.27</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2395712748834336</v>
+        <v>0.2376673546203505</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>38.03032954173963</v>
+        <v>35.54728312959153</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -6436,23 +6436,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.0573943957492737</v>
+        <v>0.05847506791838772</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1817784585087612</v>
+        <v>0.1739426891288433</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>21114290799805.62</v>
+        <v>26332785771740.23</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2395712748834336</v>
+        <v>0.2418161862208312</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>38.03032954173963</v>
+        <v>36.12539160730516</v>
       </c>
     </row>
     <row r="14">
@@ -6468,23 +6468,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.0691583530842363</v>
+        <v>0.1176834511250729</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.2061805742620788</v>
+        <v>0.2929721245787036</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>23894835702273.01</v>
+        <v>20174543863335</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2629797579363025</v>
+        <v>0.3430502166229791</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>41.32452055065748</v>
+        <v>54.10695771819847</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -6498,23 +6498,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.0691583530842363</v>
+        <v>0.1023774884475761</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2061805742620788</v>
+        <v>0.2647457785138173</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>23894835702273.01</v>
+        <v>26010333386601.05</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2629797579363025</v>
+        <v>0.319964823765951</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>41.32452055065748</v>
+        <v>49.4603558170823</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -6530,23 +6530,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.0688623761327956</v>
+        <v>0.0655568138632792</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.2079522524602403</v>
+        <v>0.1793851654657052</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>22599858394903.36</v>
+        <v>22648374414305.41</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2624164174223778</v>
+        <v>0.2560406488495122</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>41.85046965851177</v>
+        <v>36.72324741461622</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -6560,23 +6560,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'sqrt', 'max_depth': 30, 'learning_rate': 0.5}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0688623761327956</v>
+        <v>0.06817263944818992</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.2079522524602403</v>
+        <v>0.1809171594590156</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>22599858394903.36</v>
+        <v>27190220413998.47</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2624164174223778</v>
+        <v>0.2610989074052014</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>41.85046965851177</v>
+        <v>36.36746826341344</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -6592,23 +6592,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0.0554585516550583</v>
+        <v>0.06287394183536452</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0.1726933538966199</v>
+        <v>0.1856420274603999</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>20140584043979.84</v>
+        <v>25213254597002.24</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>0.2354963941444929</v>
+        <v>0.2507467683448074</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>36.42517805501596</v>
+        <v>37.8209378739172</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -6622,23 +6622,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>0.0554585516550583</v>
+        <v>0.06030372161262379</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>0.1726933538966199</v>
+        <v>0.1762975444386184</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>20140584043979.84</v>
+        <v>25196203402449.32</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>0.2354963941444929</v>
+        <v>0.245568160828361</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>36.42517805501596</v>
+        <v>36.35026539049743</v>
       </c>
     </row>
     <row r="17">
@@ -6716,23 +6716,23 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'max_samples': 1.0, 'max_features': 0.6}</t>
+          <t>{'n_estimators': 30, 'max_samples': 0.9, 'max_features': 0.7000000000000001}</t>
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.06515119974124876</v>
+        <v>0.06476128476488952</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.2039758285700859</v>
+        <v>0.183652973685979</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>25368295152635.13</v>
+        <v>25828300551712.71</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2552473305271747</v>
+        <v>0.2544823859619552</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>42.07209078276708</v>
+        <v>37.26051876644975</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -6746,23 +6746,23 @@
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'max_samples': 1.0, 'max_features': 0.6}</t>
+          <t>{'n_estimators': 30, 'max_samples': 0.9, 'max_features': 0.7000000000000001}</t>
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.06515119974124876</v>
+        <v>0.062540021141131</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.2039758285700859</v>
+        <v>0.1765332935711301</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>25368295152635.13</v>
+        <v>26483291288731.57</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2552473305271747</v>
+        <v>0.2500800294728289</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>42.07209078276708</v>
+        <v>36.15385580145526</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -6778,23 +6778,23 @@
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 2, 'max_depth': None}</t>
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0.0584156604097701</v>
+        <v>0.05927410083148792</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0.1851065613647936</v>
+        <v>0.1715590389129592</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>20276262581739.96</v>
+        <v>26559541120608.65</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>0.241693318918356</v>
+        <v>0.2434627298612416</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>38.52570195329248</v>
+        <v>35.59136890259921</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -6808,23 +6808,23 @@
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
+          <t>{'n_estimators': 200, 'min_samples_split': 5, 'min_samples_leaf': 2, 'max_depth': None}</t>
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>0.0584156604097701</v>
+        <v>0.05970823928400489</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>0.1851065613647936</v>
+        <v>0.1716579513199675</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>20276262581739.96</v>
+        <v>25554487370965.74</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>0.241693318918356</v>
+        <v>0.2443526944480148</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>38.52570195329248</v>
+        <v>35.5299817580095</v>
       </c>
     </row>
     <row r="20">
@@ -6840,23 +6840,23 @@
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>{'subsample': 1.0, 'reg_lambda': 0, 'reg_alpha': 1.0, 'n_estimators': 700, 'min_child_weight': 1, 'max_depth': 9, 'learning_rate': 0.01, 'gamma': 0.3, 'colsample_bytree': 0.8}</t>
+          <t>{'subsample': 0.9, 'reg_lambda': 0, 'reg_alpha': 0.1, 'n_estimators': 400, 'min_child_weight': 5, 'max_depth': 9, 'learning_rate': 0.01, 'gamma': 0.2, 'colsample_bytree': 0.9}</t>
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>0.0688623760829622</v>
+        <v>0.0664663595480311</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>0.2079522524901536</v>
+        <v>0.1973120351979616</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>22599858349997.61</v>
+        <v>24602597606867.85</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>0.2624164173274269</v>
+        <v>0.2578107048747804</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>41.85046967891</v>
+        <v>39.82150397607875</v>
       </c>
       <c r="I20" s="9" t="inlineStr">
         <is>
@@ -6870,23 +6870,23 @@
       </c>
       <c r="K20" s="8" t="inlineStr">
         <is>
-          <t>{'subsample': 1.0, 'reg_lambda': 0, 'reg_alpha': 1.0, 'n_estimators': 700, 'min_child_weight': 1, 'max_depth': 9, 'learning_rate': 0.01, 'gamma': 0.3, 'colsample_bytree': 0.8}</t>
+          <t>{'subsample': 0.9, 'reg_lambda': 0, 'reg_alpha': 0.1, 'n_estimators': 400, 'min_child_weight': 5, 'max_depth': 9, 'learning_rate': 0.01, 'gamma': 0.2, 'colsample_bytree': 0.9}</t>
         </is>
       </c>
       <c r="L20" s="8" t="n">
-        <v>0.0688623760829622</v>
+        <v>0.06753651014562737</v>
       </c>
       <c r="M20" s="8" t="n">
-        <v>0.2079522524901536</v>
+        <v>0.1989535841901319</v>
       </c>
       <c r="N20" s="8" t="n">
-        <v>22599858349997.61</v>
+        <v>25043803446689.09</v>
       </c>
       <c r="O20" s="8" t="n">
-        <v>0.2624164173274269</v>
+        <v>0.2598778754446545</v>
       </c>
       <c r="P20" s="8" t="n">
-        <v>41.85046967891</v>
+        <v>40.01489275772015</v>
       </c>
     </row>
     <row r="21" ht="45.75" customHeight="1">
@@ -6984,23 +6984,23 @@
       </c>
       <c r="C22" s="5" t="inlineStr">
         <is>
-          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>0.08194797500000001</v>
+        <v>0.07063674181699753</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0.21995957</v>
+        <v>0.200381338596344</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>26290810000000</v>
+        <v>23440241197056</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>0.2862655670189277</v>
+        <v>0.2657757359447953</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>42.82346665859222</v>
+        <v>42.36835539340973</v>
       </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
@@ -7014,23 +7014,23 @@
       </c>
       <c r="K22" s="8" t="inlineStr">
         <is>
-          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
         </is>
       </c>
       <c r="L22" s="8" t="n">
-        <v>0.082835846</v>
+        <v>0.08467613905668259</v>
       </c>
       <c r="M22" s="8" t="n">
-        <v>0.22171035</v>
+        <v>0.2282557040452957</v>
       </c>
       <c r="N22" s="8" t="n">
-        <v>26141283000000</v>
+        <v>24808832106496</v>
       </c>
       <c r="O22" s="8" t="n">
-        <v>0.2878121707802545</v>
+        <v>0.2909916477438529</v>
       </c>
       <c r="P22" s="8" t="n">
-        <v>42.79095232486725</v>
+        <v>42.42106974124908</v>
       </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
@@ -7046,53 +7046,53 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>0.08007480204105377</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.2168893665075302</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>27547752464384</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>0.2829749141550427</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>51.01410150527954</v>
+      </c>
+      <c r="I23" s="9" t="inlineStr">
+        <is>
+          <t>Long Short-Term Memory Network</t>
+        </is>
+      </c>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
           <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
         </is>
       </c>
-      <c r="D23" s="5" t="n">
-        <v>0.095250875</v>
-      </c>
-      <c r="E23" s="5" t="n">
-        <v>0.24006736</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>29687141000000</v>
-      </c>
-      <c r="G23" s="5" t="n">
-        <v>0.3086274044179595</v>
-      </c>
-      <c r="H23" s="5" t="n">
-        <v>41.90779030323029</v>
-      </c>
-      <c r="I23" s="9" t="inlineStr">
-        <is>
-          <t>Long Short-Term Memory Network</t>
-        </is>
-      </c>
-      <c r="J23" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K23" s="8" t="inlineStr">
-        <is>
-          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
-        </is>
-      </c>
       <c r="L23" s="8" t="n">
-        <v>0.09393493</v>
+        <v>0.07745779305696487</v>
       </c>
       <c r="M23" s="8" t="n">
-        <v>0.23721074</v>
+        <v>0.2092974483966827</v>
       </c>
       <c r="N23" s="8" t="n">
-        <v>29786154000000</v>
+        <v>29230731624448</v>
       </c>
       <c r="O23" s="8" t="n">
-        <v>0.3064880598995599</v>
+        <v>0.2783124019100925</v>
       </c>
       <c r="P23" s="8" t="n">
-        <v>41.88181161880493</v>
+        <v>44.93624567985535</v>
       </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
@@ -7112,19 +7112,19 @@
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>0.1014032140374184</v>
+        <v>0.2743563055992126</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>0.2450904548168182</v>
+        <v>0.4052923917770386</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>27880381743104</v>
+        <v>23272215281664</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>0.3184387131575216</v>
+        <v>0.5237903259885702</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>44.83312666416168</v>
+        <v>71.97405695915222</v>
       </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
@@ -7142,19 +7142,19 @@
         </is>
       </c>
       <c r="L24" s="8" t="n">
-        <v>0.1102476418018341</v>
+        <v>0.1061076000332832</v>
       </c>
       <c r="M24" s="8" t="n">
-        <v>0.2558545470237732</v>
+        <v>0.2636534869670868</v>
       </c>
       <c r="N24" s="8" t="n">
-        <v>29177996640256</v>
+        <v>23856723001344</v>
       </c>
       <c r="O24" s="8" t="n">
-        <v>0.3320356032142248</v>
+        <v>0.3257416154458672</v>
       </c>
       <c r="P24" s="8" t="n">
-        <v>45.93763649463654</v>
+        <v>56.72944188117981</v>
       </c>
     </row>
   </sheetData>
@@ -7328,19 +7328,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.05646590967437108</v>
+        <v>0.05506920285095059</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1806374684935386</v>
+        <v>0.1765173031004875</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>22972839564223.58</v>
+        <v>23920696396865.79</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2376255661210954</v>
+        <v>0.2346682825840565</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>37.8091717418089</v>
+        <v>37.03661936461267</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -7358,19 +7358,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.05646590967437108</v>
+        <v>0.05597977948111193</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1806374684935386</v>
+        <v>0.1805274616729948</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>22972839564223.58</v>
+        <v>22784068091883.64</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2376255661210954</v>
+        <v>0.2366004638226898</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>37.8091717418089</v>
+        <v>37.80121370886107</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -7386,23 +7386,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.1, 'C': 1}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.06963867239717809</v>
+        <v>0.06934928439299419</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.2084047864069103</v>
+        <v>0.2112551733707201</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>26191986564144.98</v>
+        <v>24983337332075.05</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.2638914026587037</v>
+        <v>0.2633425229487145</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>41.88893716494003</v>
+        <v>42.73745139731462</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -7416,23 +7416,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>0.06963867239717809</v>
+        <v>0.05376149483468623</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.2084047864069103</v>
+        <v>0.1711116961735539</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>26191986564144.98</v>
+        <v>24110809155642.21</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>0.2638914026587037</v>
+        <v>0.2318652514601665</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>41.88893716494003</v>
+        <v>36.45778124379989</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -7448,11 +7448,11 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>{'splitter': 'best', 'min_samples_split': 5, 'min_samples_leaf': 4, 'min_impurity_decrease': 0.1, 'max_leaf_nodes': 90, 'max_features': None, 'max_depth': 26, 'criterion': 'mae', 'ccp_alpha': 0.0}</t>
+          <t>{'splitter': 'best', 'min_samples_split': 5, 'min_samples_leaf': 2, 'min_impurity_decrease': 1.0, 'max_leaf_nodes': 50, 'max_features': 'auto', 'max_depth': 32, 'criterion': 'mae', 'ccp_alpha': 1.0}</t>
         </is>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0.07119163127258921</v>
+        <v>0.07119163127258926</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>0.21065697591085</v>
@@ -7478,11 +7478,11 @@
       </c>
       <c r="K9" s="8" t="inlineStr">
         <is>
-          <t>{'splitter': 'best', 'min_samples_split': 5, 'min_samples_leaf': 4, 'min_impurity_decrease': 0.1, 'max_leaf_nodes': 90, 'max_features': None, 'max_depth': 26, 'criterion': 'mae', 'ccp_alpha': 0.0}</t>
+          <t>{'splitter': 'best', 'min_samples_split': 5, 'min_samples_leaf': 2, 'min_impurity_decrease': 1.0, 'max_leaf_nodes': 50, 'max_features': 'auto', 'max_depth': 32, 'criterion': 'mae', 'ccp_alpha': 1.0}</t>
         </is>
       </c>
       <c r="L9" s="8" t="n">
-        <v>0.07119163127258921</v>
+        <v>0.07119163127258926</v>
       </c>
       <c r="M9" s="8" t="n">
         <v>0.21065697591085</v>
@@ -7514,19 +7514,19 @@
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0.05826691756827131</v>
+        <v>0.05938038453845324</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.1824877495837984</v>
+        <v>0.1822027604259327</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>22490669117788.94</v>
+        <v>24953578667350.85</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.2413854129152615</v>
+        <v>0.243680907209517</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>38.45264245217578</v>
+        <v>37.83445351255985</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -7544,19 +7544,19 @@
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>0.05826691756827131</v>
+        <v>0.05861475607285566</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.1824877495837984</v>
+        <v>0.1804554818286656</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>22490669117788.94</v>
+        <v>26439595229634.39</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>0.2413854129152615</v>
+        <v>0.2421048452073103</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>38.45264245217578</v>
+        <v>37.67969133766655</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -7572,23 +7572,23 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>{'tol': 0.0001, 'power_t': 0.25, 'penalty': 'elasticnet', 'max_iter': 3000, 'loss': 'squared_loss', 'learning_rate': 'optimal', 'l1_ratio': 0, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 1}</t>
+          <t>{'tol': 0.001, 'power_t': 0.25, 'penalty': 'none', 'max_iter': 1000, 'loss': 'huber', 'learning_rate': 'adaptive', 'l1_ratio': 0.7, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 0.01}</t>
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>0.0693604267958287</v>
+        <v>31.80009093728438</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>0.2099141854928262</v>
+        <v>4.460804498336811</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>25535344544115.46</v>
+        <v>160287488162644.6</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>0.2633636778218074</v>
+        <v>5.639156934975687</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>42.34414356709601</v>
+        <v>163.7443627224724</v>
       </c>
       <c r="I11" s="9" t="inlineStr">
         <is>
@@ -7602,23 +7602,23 @@
       </c>
       <c r="K11" s="8" t="inlineStr">
         <is>
-          <t>{'tol': 0.0001, 'power_t': 0.25, 'penalty': 'elasticnet', 'max_iter': 3000, 'loss': 'squared_loss', 'learning_rate': 'optimal', 'l1_ratio': 0, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 1}</t>
+          <t>{'tol': 1e-05, 'power_t': 0.5, 'penalty': 'l2', 'max_iter': 3000, 'loss': 'squared_epsilon_insensitive', 'learning_rate': 'adaptive', 'l1_ratio': 1, 'fit_intercept': False, 'eta0': 0.1, 'alpha': 1}</t>
         </is>
       </c>
       <c r="L11" s="8" t="n">
-        <v>0.0693604267958287</v>
+        <v>0.4211402598848671</v>
       </c>
       <c r="M11" s="8" t="n">
-        <v>0.2099141854928262</v>
+        <v>0.6052499650359917</v>
       </c>
       <c r="N11" s="8" t="n">
-        <v>25535344544115.46</v>
+        <v>2855861606214.893</v>
       </c>
       <c r="O11" s="8" t="n">
-        <v>0.2633636778218074</v>
+        <v>0.6489532031547938</v>
       </c>
       <c r="P11" s="8" t="n">
-        <v>42.34414356709601</v>
+        <v>184.163829539131</v>
       </c>
     </row>
     <row r="12" ht="45.75" customHeight="1">
@@ -7716,23 +7716,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.0564159481570401</v>
+        <v>0.04945933520229624</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1761178338003387</v>
+        <v>0.1674971170068324</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>20794897960969.17</v>
+        <v>23656231193879.87</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.2375204162951895</v>
+        <v>0.2223945484994995</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>37.56236843279562</v>
+        <v>35.4624460614015</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -7746,23 +7746,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.0564159481570401</v>
+        <v>0.04908946581707793</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1761178338003387</v>
+        <v>0.1703676837637862</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>20794897960969.17</v>
+        <v>23347411203166.96</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2375204162951895</v>
+        <v>0.2215614267355172</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>37.56236843279562</v>
+        <v>36.235367711255</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -7778,53 +7778,53 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>0.09022842320629142</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>0.2364134597618383</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>28338666745182.21</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>0.3003804640889474</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <v>45.77110704173516</v>
+      </c>
+      <c r="I14" s="9" t="inlineStr">
+        <is>
+          <t>Stacking Regressor</t>
+        </is>
+      </c>
+      <c r="J14" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K14" s="8" t="inlineStr">
+        <is>
           <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
-      <c r="D14" s="5" t="n">
-        <v>0.0607964732996342</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>0.1893892234855264</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>22481624472142.8</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <v>0.2465694086857374</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <v>39.35514479529489</v>
-      </c>
-      <c r="I14" s="9" t="inlineStr">
-        <is>
-          <t>Stacking Regressor</t>
-        </is>
-      </c>
-      <c r="J14" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K14" s="8" t="inlineStr">
-        <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
-        </is>
-      </c>
       <c r="L14" s="8" t="n">
-        <v>0.0607964732996342</v>
+        <v>0.07033006396237493</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.1893892234855264</v>
+        <v>0.2028654246449865</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>22481624472142.8</v>
+        <v>26127891314604.59</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2465694086857374</v>
+        <v>0.2651981598020147</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>39.35514479529489</v>
+        <v>40.64580319191941</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -7840,23 +7840,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.0679588977142149</v>
+        <v>0.06960230689516862</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.1987242050508918</v>
+        <v>0.2104138311503264</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>22069759901682.35</v>
+        <v>25566740450964.13</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2606892742600181</v>
+        <v>0.2638224912610155</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>41.22524476203199</v>
+        <v>42.42072550665512</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -7870,23 +7870,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 5, 'max_features': 'log2', 'max_depth': 30, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0679588977142149</v>
+        <v>0.06960230689516862</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.1987242050508918</v>
+        <v>0.2104138311503264</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>22069759901682.35</v>
+        <v>25566740450964.13</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2606892742600181</v>
+        <v>0.2638224912610155</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>41.22524476203199</v>
+        <v>42.42072550665512</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -7902,23 +7902,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0.0589820876068267</v>
+        <v>0.05184423167013936</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0.1776065746524728</v>
+        <v>0.1746700858409219</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>19016817830663.01</v>
+        <v>23095409642854.23</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>0.2428622811529751</v>
+        <v>0.2276932842007848</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>37.704707810329</v>
+        <v>37.35259461409189</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -7932,23 +7932,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 2, 'max_depth': None}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>0.0589820876068267</v>
+        <v>0.04945431467988452</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>0.1776065746524728</v>
+        <v>0.1683549538185005</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>19016817830663.01</v>
+        <v>21921892031361.27</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>0.2428622811529751</v>
+        <v>0.2223832607906551</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>37.704707810329</v>
+        <v>36.03778428587271</v>
       </c>
     </row>
     <row r="17" ht="42.75" customHeight="1">
@@ -8030,19 +8030,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.06068035059434203</v>
+        <v>0.06552320320015612</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.1879509119332573</v>
+        <v>0.19876716949384</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>23627561244459.81</v>
+        <v>25641682162811.25</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2463338194287216</v>
+        <v>0.255975005030093</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>38.82995165234105</v>
+        <v>40.40499752486321</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -8060,19 +8060,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.06068035059434203</v>
+        <v>0.06462090091538875</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.1879509119332573</v>
+        <v>0.1984209408963854</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>23627561244459.81</v>
+        <v>25920824503009.91</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2463338194287216</v>
+        <v>0.2542064139934096</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>38.82995165234105</v>
+        <v>40.39701956428086</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -8088,23 +8088,23 @@
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0.0588453912227243</v>
+        <v>0.05240969522165263</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0.1893136330658788</v>
+        <v>0.1780712815667265</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>21900432631099.29</v>
+        <v>24109656740367.25</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>0.2425806901274797</v>
+        <v>0.2289316387519485</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>39.36377331542993</v>
+        <v>38.13238737128543</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -8118,23 +8118,23 @@
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 2, 'max_depth': None}</t>
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>0.0588453912227243</v>
+        <v>0.05071715570834319</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>0.1893136330658788</v>
+        <v>0.1773104132494211</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>21900432631099.29</v>
+        <v>20319950768350.11</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>0.2425806901274797</v>
+        <v>0.2252046973496405</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>39.36377331542993</v>
+        <v>38.35956983507885</v>
       </c>
     </row>
     <row r="20" ht="128.25" customHeight="1">
@@ -8150,23 +8150,23 @@
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>{'subsample': 0.9, 'reg_lambda': 0.1, 'reg_alpha': 0.5, 'n_estimators': 600, 'min_child_weight': 5, 'max_depth': 10, 'learning_rate': 0.1, 'gamma': 0.1, 'colsample_bytree': 0.7}</t>
+          <t>{'subsample': 0.9, 'reg_lambda': 0.1, 'reg_alpha': 0.5, 'n_estimators': 200, 'min_child_weight': 1, 'max_depth': 10, 'learning_rate': 0.1, 'gamma': 0.3, 'colsample_bytree': 0.9}</t>
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>0.0599142796681522</v>
+        <v>0.06184873249408603</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>0.1922070109386474</v>
+        <v>0.197787906331553</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>22718176331584.95</v>
+        <v>25239570310513.27</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>0.2447739358431617</v>
+        <v>0.2486940539982531</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>39.80811383623279</v>
+        <v>40.58025161178524</v>
       </c>
       <c r="I20" s="9" t="inlineStr">
         <is>
@@ -8180,23 +8180,23 @@
       </c>
       <c r="K20" s="8" t="inlineStr">
         <is>
-          <t>{'subsample': 0.9, 'reg_lambda': 0.1, 'reg_alpha': 0.5, 'n_estimators': 600, 'min_child_weight': 5, 'max_depth': 10, 'learning_rate': 0.1, 'gamma': 0.1, 'colsample_bytree': 0.7}</t>
+          <t>{'subsample': 0.9, 'reg_lambda': 0.1, 'reg_alpha': 0.5, 'n_estimators': 200, 'min_child_weight': 1, 'max_depth': 10, 'learning_rate': 0.1, 'gamma': 0.3, 'colsample_bytree': 0.9}</t>
         </is>
       </c>
       <c r="L20" s="8" t="n">
-        <v>0.0599142796681522</v>
+        <v>0.06402620111538673</v>
       </c>
       <c r="M20" s="8" t="n">
-        <v>0.1922070109386474</v>
+        <v>0.2014253019604962</v>
       </c>
       <c r="N20" s="8" t="n">
-        <v>22718176331584.95</v>
+        <v>25618945582140.18</v>
       </c>
       <c r="O20" s="8" t="n">
-        <v>0.2447739358431617</v>
+        <v>0.2530339920156712</v>
       </c>
       <c r="P20" s="8" t="n">
-        <v>39.80811383623279</v>
+        <v>41.06152573297317</v>
       </c>
     </row>
     <row r="21" ht="45.75" customHeight="1">
@@ -8294,23 +8294,23 @@
       </c>
       <c r="C22" s="5" t="inlineStr">
         <is>
-          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>0.08294865</v>
+        <v>0.08482728898525238</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0.22359388</v>
+        <v>0.2327423691749573</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>29775520000000</v>
+        <v>28384780353536</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>0.288008068358301</v>
+        <v>0.2912512471823123</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>43.07083785533905</v>
+        <v>43.51461231708527</v>
       </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
@@ -8324,23 +8324,23 @@
       </c>
       <c r="K22" s="8" t="inlineStr">
         <is>
-          <t>{'module__num_units': 50, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
         </is>
       </c>
       <c r="L22" s="8" t="n">
-        <v>0.08614325</v>
+        <v>0.09172665327787399</v>
       </c>
       <c r="M22" s="8" t="n">
-        <v>0.22960332</v>
+        <v>0.23125821352005</v>
       </c>
       <c r="N22" s="8" t="n">
-        <v>30235582000000</v>
+        <v>34735491383296</v>
       </c>
       <c r="O22" s="8" t="n">
-        <v>0.2935016997960728</v>
+        <v>0.3028640838360898</v>
       </c>
       <c r="P22" s="8" t="n">
-        <v>43.15841794013977</v>
+        <v>46.05624675750732</v>
       </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
@@ -8356,23 +8356,23 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
         </is>
       </c>
       <c r="D23" s="5" t="n">
-        <v>0.08599666</v>
+        <v>0.1111845821142197</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>0.22661445</v>
+        <v>0.2497399002313614</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>33222476000000</v>
+        <v>25662742069248</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>0.2932518671891785</v>
+        <v>0.3334435216258065</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>40.77632129192352</v>
+        <v>64.33287262916565</v>
       </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
@@ -8390,19 +8390,19 @@
         </is>
       </c>
       <c r="L23" s="8" t="n">
-        <v>0.08550727</v>
+        <v>0.05191219598054886</v>
       </c>
       <c r="M23" s="8" t="n">
-        <v>0.22598037</v>
+        <v>0.172699823975563</v>
       </c>
       <c r="N23" s="8" t="n">
-        <v>33220626000000</v>
+        <v>29153604665344</v>
       </c>
       <c r="O23" s="8" t="n">
-        <v>0.2924162677998801</v>
+        <v>0.2278424806320122</v>
       </c>
       <c r="P23" s="8" t="n">
-        <v>40.74816703796387</v>
+        <v>48.13580811023712</v>
       </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
@@ -8422,19 +8422,19 @@
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>0.07501772046089172</v>
+        <v>3807.388916015625</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>0.1971401125192642</v>
+        <v>44.56591796875</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>26607699886080</v>
+        <v>805874914295808</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>0.2738936298289752</v>
+        <v>61.70404294708431</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>39.19986486434937</v>
+        <v>190.6166911125183</v>
       </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
@@ -8452,19 +8452,19 @@
         </is>
       </c>
       <c r="L24" s="8" t="n">
-        <v>0.07061392068862915</v>
+        <v>0.1638609170913696</v>
       </c>
       <c r="M24" s="8" t="n">
-        <v>0.2048145830631256</v>
+        <v>0.3003096580505371</v>
       </c>
       <c r="N24" s="8" t="n">
-        <v>26526863065088</v>
+        <v>17196006768640</v>
       </c>
       <c r="O24" s="8" t="n">
-        <v>0.2657327994219553</v>
+        <v>0.4047973778217562</v>
       </c>
       <c r="P24" s="8" t="n">
-        <v>41.04349613189697</v>
+        <v>59.75452065467834</v>
       </c>
     </row>
   </sheetData>
@@ -8638,19 +8638,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.05922356432069868</v>
+        <v>0.04698528612772342</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.1858861652413798</v>
+        <v>0.1522323554377048</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>24801660827758.78</v>
+        <v>29901067812994.32</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.2433589207748479</v>
+        <v>0.2167608962145235</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>38.69262186983138</v>
+        <v>33.18918625025464</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -8668,19 +8668,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.05660950470877726</v>
+        <v>0.05432397895885679</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.1814901079323312</v>
+        <v>0.173798013155719</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>24656179578374.99</v>
+        <v>25903446188832.43</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.2379275198643008</v>
+        <v>0.2330750500565361</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>38.19255996742378</v>
+        <v>36.68824980009423</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -8696,23 +8696,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.1, 'C': 1}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.0685195201860918</v>
+        <v>0.06704204778750833</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.209449034824606</v>
+        <v>0.2068595657458495</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>28773471740342.18</v>
+        <v>28747010075998.53</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.2617623353083706</v>
+        <v>0.258924791759129</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>42.38047784368912</v>
+        <v>42.06445840098355</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -8726,23 +8726,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'linear', 'gamma': 0.0001, 'C': 1000}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>0.0582936778651273</v>
+        <v>0.05487126749116299</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.1910171656092151</v>
+        <v>0.1797092701204524</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>22336169364572.84</v>
+        <v>29530656290652.37</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>0.2414408371943887</v>
+        <v>0.2342461685730697</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>40.45111416192763</v>
+        <v>38.47308191157114</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -8762,10 +8762,10 @@
         </is>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0.0696707191003918</v>
+        <v>0.06967071910039184</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>0.2088153244282614</v>
+        <v>0.2088153244282615</v>
       </c>
       <c r="F9" s="5" t="n">
         <v>30045609963251.31</v>
@@ -8792,10 +8792,10 @@
         </is>
       </c>
       <c r="L9" s="8" t="n">
-        <v>0.0696707191003918</v>
+        <v>0.06967071910039184</v>
       </c>
       <c r="M9" s="8" t="n">
-        <v>0.2088153244282614</v>
+        <v>0.2088153244282615</v>
       </c>
       <c r="N9" s="8" t="n">
         <v>30045609963251.31</v>
@@ -8820,23 +8820,23 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
+          <t>{'weights': 'distance', 'n_neighbors': 7}</t>
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0.05012742623792553</v>
+        <v>0.04743587008132614</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.1679549008529361</v>
+        <v>0.1642666532192697</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>28340733437481.82</v>
+        <v>33674201299287.03</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.2238915501708931</v>
+        <v>0.2177977733617269</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>36.82330665674328</v>
+        <v>35.52921186487665</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -8850,23 +8850,23 @@
       </c>
       <c r="K10" s="8" t="inlineStr">
         <is>
-          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
+          <t>{'weights': 'distance', 'n_neighbors': 7}</t>
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>0.06138722119394868</v>
+        <v>0.05107444334368347</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.1924685832458924</v>
+        <v>0.1693561175681612</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>19537774692403.85</v>
+        <v>32466282389128.17</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>0.2477644469934068</v>
+        <v>0.2259965560438554</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>43.18584752750821</v>
+        <v>36.72133067892661</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -8882,23 +8882,23 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>{'tol': 0.001, 'power_t': 0.25, 'penalty': 'none', 'max_iter': 1000, 'loss': 'huber', 'learning_rate': 'adaptive', 'l1_ratio': 0.7, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 0.01}</t>
+          <t>{'tol': 1e-05, 'power_t': 0.5, 'penalty': 'l2', 'max_iter': 3000, 'loss': 'squared_epsilon_insensitive', 'learning_rate': 'adaptive', 'l1_ratio': 1, 'fit_intercept': False, 'eta0': 0.1, 'alpha': 1}</t>
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>730349.8081436356</v>
+        <v>0.4231923138628946</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>681.7094335836382</v>
+        <v>0.6140047982513612</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>4.734701726586679e+16</v>
+        <v>2731628772965.815</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>854.6050597461003</v>
+        <v>0.6505323311434218</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>199.632397266838</v>
+        <v>183.1880446036282</v>
       </c>
       <c r="I11" s="9" t="inlineStr">
         <is>
@@ -8912,23 +8912,23 @@
       </c>
       <c r="K11" s="8" t="inlineStr">
         <is>
-          <t>{'tol': 0.0001, 'power_t': 0.25, 'penalty': 'elasticnet', 'max_iter': 3000, 'loss': 'squared_loss', 'learning_rate': 'optimal', 'l1_ratio': 0, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 1}</t>
+          <t>{'tol': 1e-05, 'power_t': 0.5, 'penalty': 'l2', 'max_iter': 3000, 'loss': 'squared_epsilon_insensitive', 'learning_rate': 'adaptive', 'l1_ratio': 1, 'fit_intercept': False, 'eta0': 0.1, 'alpha': 1}</t>
         </is>
       </c>
       <c r="L11" s="8" t="n">
-        <v>0.06859048189762119</v>
+        <v>0.4316053369222674</v>
       </c>
       <c r="M11" s="8" t="n">
-        <v>0.2083342627089458</v>
+        <v>0.6140744084988815</v>
       </c>
       <c r="N11" s="8" t="n">
-        <v>29294926466785.37</v>
+        <v>2554457284660.033</v>
       </c>
       <c r="O11" s="8" t="n">
-        <v>0.2618978463019908</v>
+        <v>0.656966770028947</v>
       </c>
       <c r="P11" s="8" t="n">
-        <v>42.04809603140421</v>
+        <v>189.7113618472891</v>
       </c>
     </row>
     <row r="12" ht="45.75" customHeight="1">
@@ -9030,19 +9030,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0.053018037178272</v>
+        <v>0.0468605237447411</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.1718575105882687</v>
+        <v>0.1558101524906078</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>26666866336220.17</v>
+        <v>30583943510164.24</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.230256459579904</v>
+        <v>0.2164729168850947</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>36.05595238261929</v>
+        <v>32.78446626937581</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -9056,23 +9056,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>0.0561392936502394</v>
+        <v>0.04979560812870166</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.1822884839690082</v>
+        <v>0.1651166510576912</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>24798372381684.57</v>
+        <v>28582582483208.96</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>0.2369373200874852</v>
+        <v>0.2231492956043143</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>38.48662691681865</v>
+        <v>34.73745571593716</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -9088,23 +9088,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>0.0677320180600237</v>
+        <v>0.08372556839419026</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.1973134919130299</v>
+        <v>0.2141661897486528</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>29436768852636.02</v>
+        <v>22453896547452.54</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.2602537570526576</v>
+        <v>0.2893537081051326</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>39.80216203439728</v>
+        <v>42.91773589948916</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -9118,23 +9118,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>0.07161607858115369</v>
+        <v>0.09650325055981622</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.2038704621969823</v>
+        <v>0.2289555700645094</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>30358711936670.34</v>
+        <v>35576690140164.41</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>0.2676118057581798</v>
+        <v>0.3106497232572664</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>40.75632698267508</v>
+        <v>43.87644362441592</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -9154,7 +9154,7 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>0.0688863586187215</v>
+        <v>0.06888635861872158</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>0.2089631462553461</v>
@@ -9163,7 +9163,7 @@
         <v>29368713870653.49</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.2624621089199764</v>
+        <v>0.2624621089199765</v>
       </c>
       <c r="H15" s="5" t="n">
         <v>42.14102180393471</v>
@@ -9184,7 +9184,7 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>0.0688863586187215</v>
+        <v>0.06888635861872158</v>
       </c>
       <c r="M15" s="8" t="n">
         <v>0.2089631462553461</v>
@@ -9193,7 +9193,7 @@
         <v>29368713870653.49</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>0.2624621089199764</v>
+        <v>0.2624621089199765</v>
       </c>
       <c r="P15" s="8" t="n">
         <v>42.14102180393471</v>
@@ -9212,23 +9212,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>0.0547223768996318</v>
+        <v>0.05372098078710089</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0.1693469862770087</v>
+        <v>0.169658922525522</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>27104088709212.8</v>
+        <v>29296468540619.84</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>0.2339281447360105</v>
+        <v>0.2317778694938343</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>35.32086038620331</v>
+        <v>35.84871435896012</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -9246,19 +9246,19 @@
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>0.0692716376738975</v>
+        <v>0.05258458020565428</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>0.2032688901975708</v>
+        <v>0.1629535246811047</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>20735335780538.84</v>
+        <v>29128637423171.66</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>0.2631950563249575</v>
+        <v>0.2293132796103494</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>42.80617841882972</v>
+        <v>34.44805183054446</v>
       </c>
     </row>
     <row r="17" ht="42.75" customHeight="1">
@@ -9340,19 +9340,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0.06095533311690104</v>
+        <v>0.06259939529075842</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.1877044006530547</v>
+        <v>0.1938954248548306</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>28999204350870.47</v>
+        <v>31262472722892.48</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>0.2468913386834399</v>
+        <v>0.2501987116089098</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>38.60368498246481</v>
+        <v>39.65144646862679</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -9370,19 +9370,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>0.05837166771720272</v>
+        <v>0.06271520093992723</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.1846627335219367</v>
+        <v>0.1916630511574544</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>25744526093310.08</v>
+        <v>30672106388461.92</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>0.2416022924502222</v>
+        <v>0.2504300320247698</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>38.35752333782202</v>
+        <v>39.18876888195973</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -9402,19 +9402,19 @@
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0.0579132694697535</v>
+        <v>0.05391762811250559</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0.1884561728833011</v>
+        <v>0.1750322101689191</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>27576870657654.62</v>
+        <v>32205471664137.19</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>0.2406517597478845</v>
+        <v>0.2322016970491508</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>39.17634617851189</v>
+        <v>36.87767777851777</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -9428,23 +9428,23 @@
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>0.0581111354233673</v>
+        <v>0.0553507286207801</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>0.1890629690337563</v>
+        <v>0.1795289623801412</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>25126520633235.46</v>
+        <v>27692360162039.01</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>0.2410625135174844</v>
+        <v>0.2352673556207493</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>39.43563006546778</v>
+        <v>37.97170136342019</v>
       </c>
     </row>
     <row r="20" ht="128.25" customHeight="1">
@@ -9460,23 +9460,23 @@
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>{'subsample': 1.0, 'reg_lambda': 0, 'reg_alpha': 1.0, 'n_estimators': 700, 'min_child_weight': 1, 'max_depth': 9, 'learning_rate': 0.01, 'gamma': 0.3, 'colsample_bytree': 0.8}</t>
+          <t>{'subsample': 0.9, 'reg_lambda': 1.0, 'reg_alpha': 0, 'n_estimators': 100, 'min_child_weight': 5, 'max_depth': 3, 'learning_rate': 0.1, 'gamma': 0.2, 'colsample_bytree': 1.0}</t>
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>0.06888635964331299</v>
+        <v>0.05825766569188812</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>0.2089631459938801</v>
+        <v>0.183244293564624</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>29368715048191.67</v>
+        <v>31444168515497.97</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>0.262462110871861</v>
+        <v>0.2413662480378898</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>42.14102144499365</v>
+        <v>38.90535915958891</v>
       </c>
       <c r="I20" s="9" t="inlineStr">
         <is>
@@ -9490,23 +9490,23 @@
       </c>
       <c r="K20" s="8" t="inlineStr">
         <is>
-          <t>{'subsample': 0.8, 'reg_lambda': 0.5, 'reg_alpha': 1.0, 'n_estimators': 600, 'min_child_weight': 5, 'max_depth': 8, 'learning_rate': 0.2, 'gamma': 0.1, 'colsample_bytree': 0.7}</t>
+          <t>{'subsample': 0.9, 'reg_lambda': 1.0, 'reg_alpha': 0, 'n_estimators': 100, 'min_child_weight': 5, 'max_depth': 3, 'learning_rate': 0.1, 'gamma': 0.2, 'colsample_bytree': 1.0}</t>
         </is>
       </c>
       <c r="L20" s="8" t="n">
-        <v>0.06287334001137609</v>
+        <v>0.0512861605069249</v>
       </c>
       <c r="M20" s="8" t="n">
-        <v>0.1977182830357366</v>
+        <v>0.1709056033181563</v>
       </c>
       <c r="N20" s="8" t="n">
-        <v>25133008487107.09</v>
+        <v>28092962554738.89</v>
       </c>
       <c r="O20" s="8" t="n">
-        <v>0.2507455682786361</v>
+        <v>0.2264644795700308</v>
       </c>
       <c r="P20" s="8" t="n">
-        <v>40.72659394128257</v>
+        <v>36.81607076564591</v>
       </c>
     </row>
     <row r="21" ht="45.75" customHeight="1">
@@ -9608,19 +9608,19 @@
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>0.074048884</v>
+        <v>0.05762747675180435</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0.21209219</v>
+        <v>0.1831900477409363</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>30246050000000</v>
+        <v>33677742440448</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>0.2721192463111911</v>
+        <v>0.2400572364079124</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>43.20311844348908</v>
+        <v>45.95741629600525</v>
       </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
@@ -9634,23 +9634,23 @@
       </c>
       <c r="K22" s="8" t="inlineStr">
         <is>
-          <t>{'module__num_units': 100, 'module__activation_func': Tanh(), 'lr': 0.02}</t>
+          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
         </is>
       </c>
       <c r="L22" s="8" t="n">
-        <v>0.084464945</v>
+        <v>0.08027325570583344</v>
       </c>
       <c r="M22" s="8" t="n">
-        <v>0.22427051</v>
+        <v>0.2256852090358734</v>
       </c>
       <c r="N22" s="8" t="n">
-        <v>34330162000000</v>
+        <v>29063175471104</v>
       </c>
       <c r="O22" s="8" t="n">
-        <v>0.2906285342134908</v>
+        <v>0.2833253530939888</v>
       </c>
       <c r="P22" s="8" t="n">
-        <v>43.00118088722229</v>
+        <v>43.38162541389465</v>
       </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
@@ -9666,23 +9666,23 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 30, 'lr': 0.1, 'batch_size': 16}</t>
         </is>
       </c>
       <c r="D23" s="5" t="n">
-        <v>0.070185415</v>
+        <v>0.08558099716901779</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>0.20961301</v>
+        <v>0.2390698343515396</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>27523033000000</v>
+        <v>37734617972736</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>0.2649253016356842</v>
+        <v>0.2925422997944362</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>45.23964822292328</v>
+        <v>65.1398777961731</v>
       </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
@@ -9700,19 +9700,19 @@
         </is>
       </c>
       <c r="L23" s="8" t="n">
-        <v>0.09160694</v>
+        <v>0.1012963056564331</v>
       </c>
       <c r="M23" s="8" t="n">
-        <v>0.23438388</v>
+        <v>0.256516695022583</v>
       </c>
       <c r="N23" s="8" t="n">
-        <v>39004770000000</v>
+        <v>40491533991936</v>
       </c>
       <c r="O23" s="8" t="n">
-        <v>0.3026663796143249</v>
+        <v>0.318270805535841</v>
       </c>
       <c r="P23" s="8" t="n">
-        <v>40.88883996009827</v>
+        <v>49.41315948963165</v>
       </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
@@ -9732,19 +9732,19 @@
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>1335200.375</v>
+        <v>42.55430603027344</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>884.6502075195312</v>
+        <v>5.148109436035156</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>6.286405333208269e+16</v>
+        <v>65027553886208</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>1155.508708318548</v>
+        <v>6.523366157918275</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>197.805392742157</v>
+        <v>175.0324249267578</v>
       </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
@@ -9762,19 +9762,19 @@
         </is>
       </c>
       <c r="L24" s="8" t="n">
-        <v>0.08269235491752625</v>
+        <v>3.761208534240723</v>
       </c>
       <c r="M24" s="8" t="n">
-        <v>0.2210704982280731</v>
+        <v>1.52149760723114</v>
       </c>
       <c r="N24" s="8" t="n">
-        <v>32996390338560</v>
+        <v>50492298231808</v>
       </c>
       <c r="O24" s="8" t="n">
-        <v>0.2875627843054908</v>
+        <v>1.939383544903051</v>
       </c>
       <c r="P24" s="8" t="n">
-        <v>42.59116053581238</v>
+        <v>133.0767273902893</v>
       </c>
     </row>
   </sheetData>
@@ -9948,19 +9948,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.9972854966527085</v>
+        <v>0.9194269403573401</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.6083726915747472</v>
+        <v>0.5383628792847953</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.5965976040668238</v>
+        <v>0.5647023831877299</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.9986418260080581</v>
+        <v>0.95886753014029</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>29.23314770596295</v>
+        <v>26.22294867436287</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -9978,19 +9978,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.9994900133592056</v>
+        <v>0.9683984210187196</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.6103894270354667</v>
+        <v>0.5892843202372989</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.5971204879126394</v>
+        <v>0.5895237546798932</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.9997449741605134</v>
+        <v>0.984072365742845</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>29.3415993157885</v>
+        <v>28.49509937476473</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -10006,23 +10006,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.1, 'C': 1}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>1.032091006402447</v>
+        <v>1.079276913727102</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.5551633240713884</v>
+        <v>0.4935958142958398</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.6259952131185363</v>
+        <v>0.6379869684025011</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>1.015918799118535</v>
+        <v>1.038882531245521</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>26.10774278357824</v>
+        <v>23.38468871119256</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -10036,23 +10036,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.1, 'C': 1}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>1.031792349966598</v>
+        <v>1.07855316565132</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.5543735047963029</v>
+        <v>0.4950291909323166</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>0.6256536221081712</v>
+        <v>0.638125590778008</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>1.015771800143417</v>
+        <v>1.038534142747035</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>26.07620330121429</v>
+        <v>23.44482046139927</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -10130,53 +10130,53 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 1}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>1.531138405963538</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.7109995349113094</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.7447450674280748</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>1.237391775454944</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>35.17355430444191</v>
+      </c>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>K-Neighbors Regressor</t>
+        </is>
+      </c>
+      <c r="J10" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="8" t="inlineStr">
+        <is>
           <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
         </is>
       </c>
-      <c r="D10" s="5" t="n">
-        <v>1.158382051647328</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>0.6922138135041773</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0.6196159498714593</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>1.076281585667676</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <v>32.4700119912636</v>
-      </c>
-      <c r="I10" s="9" t="inlineStr">
-        <is>
-          <t>K-Neighbors Regressor</t>
-        </is>
-      </c>
-      <c r="J10" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K10" s="8" t="inlineStr">
-        <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
-        </is>
-      </c>
       <c r="L10" s="8" t="n">
-        <v>1.182920766676242</v>
+        <v>1.074245791890105</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.708013651200836</v>
+        <v>0.541216202245284</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>0.627563266945484</v>
+        <v>0.6440339915812889</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>1.087621610063096</v>
+        <v>1.036458292402596</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>33.2728859319046</v>
+        <v>25.55614841810936</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -10192,23 +10192,23 @@
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>{'tol': 0.001, 'power_t': 0.25, 'penalty': 'none', 'max_iter': 1000, 'loss': 'huber', 'learning_rate': 'adaptive', 'l1_ratio': 0.7, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 0.01}</t>
+          <t>{'tol': 1e-05, 'power_t': 0.75, 'penalty': 'l1', 'max_iter': 1000, 'loss': 'huber', 'learning_rate': 'invscaling', 'l1_ratio': 0, 'fit_intercept': True, 'eta0': 0.01, 'alpha': 0.01}</t>
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>94.80538782729508</v>
+        <v>6.148127879984507</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>5.96419649846825</v>
+        <v>2.37262241246973</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>2.95172437478444</v>
+        <v>0.9819838836410703</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>9.736805832884574</v>
+        <v>2.479541868971868</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>104.1690558396283</v>
+        <v>169.0044790183496</v>
       </c>
       <c r="I11" s="9" t="inlineStr">
         <is>
@@ -10222,23 +10222,23 @@
       </c>
       <c r="K11" s="8" t="inlineStr">
         <is>
-          <t>{'tol': 1e-05, 'power_t': 0.5, 'penalty': 'l2', 'max_iter': 3000, 'loss': 'squared_epsilon_insensitive', 'learning_rate': 'adaptive', 'l1_ratio': 1, 'fit_intercept': False, 'eta0': 0.1, 'alpha': 1}</t>
+          <t>{'tol': 1e-05, 'power_t': 0.75, 'penalty': 'l1', 'max_iter': 1000, 'loss': 'huber', 'learning_rate': 'invscaling', 'l1_ratio': 0, 'fit_intercept': True, 'eta0': 0.01, 'alpha': 0.01}</t>
         </is>
       </c>
       <c r="L11" s="8" t="n">
-        <v>6.967913733791798</v>
+        <v>6.134129848611734</v>
       </c>
       <c r="M11" s="8" t="n">
-        <v>2.549813070140972</v>
+        <v>2.365829135746786</v>
       </c>
       <c r="N11" s="8" t="n">
-        <v>1.028567070930362</v>
+        <v>0.9783641008392818</v>
       </c>
       <c r="O11" s="8" t="n">
-        <v>2.639680612080143</v>
+        <v>2.476717555275881</v>
       </c>
       <c r="P11" s="8" t="n">
-        <v>191.6210392451946</v>
+        <v>167.8698202106268</v>
       </c>
     </row>
     <row r="12" ht="45.75" customHeight="1">
@@ -10340,19 +10340,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1.006256552565073</v>
+        <v>0.9822839712010852</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.5714872078782586</v>
+        <v>0.5372820748374191</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.6313389459841966</v>
+        <v>0.6063166017463596</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>1.003123398473524</v>
+        <v>0.9911024019752375</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>27.07755080149915</v>
+        <v>25.84849974780389</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -10370,19 +10370,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>1.005360021323149</v>
+        <v>0.9769116340465059</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.5705341061234438</v>
+        <v>0.5359726451675894</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.6218016373956101</v>
+        <v>0.607774171266702</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>1.002676429025411</v>
+        <v>0.9883884024241208</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>27.19562944503461</v>
+        <v>25.7470900182771</v>
       </c>
     </row>
     <row r="14">
@@ -10402,19 +10402,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>1.256826375983269</v>
+        <v>1.219126266334688</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.6429766602114758</v>
+        <v>0.7749186377216453</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.6218116574574047</v>
+        <v>0.6632359679561859</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>1.121082680261928</v>
+        <v>1.104140510231686</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>29.94749219581298</v>
+        <v>36.27082798417992</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -10432,19 +10432,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>1.270770284215343</v>
+        <v>1.076652719563624</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.6272480567603567</v>
+        <v>0.6438525474024651</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.7011658491385377</v>
+        <v>0.6656176292587356</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>1.12728447350939</v>
+        <v>1.037618773713941</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>28.52067744735229</v>
+        <v>30.71988560141656</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -10464,19 +10464,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>1.003647459209448</v>
+        <v>1.007045781728249</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.5953621951870194</v>
+        <v>0.5899788345217452</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.6144378053755243</v>
+        <v>0.6064216442579166</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>1.001822069635845</v>
+        <v>1.003516707249186</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>28.04296367380638</v>
+        <v>27.81423862925155</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -10490,23 +10490,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>1.002209130620602</v>
+        <v>1.111964204400459</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.5975587259052827</v>
+        <v>0.6040401244688824</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.6097729893217377</v>
+        <v>0.5970262886600607</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>1.00110395595093</v>
+        <v>1.054497133424487</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>28.17485650445494</v>
+        <v>28.4207043465556</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -10522,53 +10522,53 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>1.017230231166633</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0.531895071320063</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0.6116338299799076</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>1.008578321781027</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>25.28181894434736</v>
+      </c>
+      <c r="I16" s="9" t="inlineStr">
+        <is>
+          <t>Random Forest Regressor</t>
+        </is>
+      </c>
+      <c r="J16" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K16" s="8" t="inlineStr">
+        <is>
           <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
         </is>
       </c>
-      <c r="D16" s="5" t="n">
-        <v>0.989089260249661</v>
-      </c>
-      <c r="E16" s="5" t="n">
-        <v>0.5585190223316671</v>
-      </c>
-      <c r="F16" s="5" t="n">
-        <v>0.640931989511882</v>
-      </c>
-      <c r="G16" s="5" t="n">
-        <v>0.9945296678579584</v>
-      </c>
-      <c r="H16" s="5" t="n">
-        <v>26.56365392705266</v>
-      </c>
-      <c r="I16" s="9" t="inlineStr">
-        <is>
-          <t>Random Forest Regressor</t>
-        </is>
-      </c>
-      <c r="J16" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K16" s="8" t="inlineStr">
-        <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
-        </is>
-      </c>
       <c r="L16" s="8" t="n">
-        <v>0.9843609792494068</v>
+        <v>1.057020148560591</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>0.5495537989010105</v>
+        <v>0.5479015305078407</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>0.6222881711705995</v>
+        <v>0.619594904228431</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>0.9921496758299158</v>
+        <v>1.028114851833486</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>26.27066502443631</v>
+        <v>25.84471473144074</v>
       </c>
     </row>
     <row r="17">
@@ -10650,19 +10650,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>1.093452047945584</v>
+        <v>1.050523040847129</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.6361689830427744</v>
+        <v>0.6121164599926127</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.6664259075810685</v>
+        <v>0.6283086792051542</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>1.045682575137209</v>
+        <v>1.024950262621133</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>29.86441526711482</v>
+        <v>28.90847036330616</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -10676,23 +10676,23 @@
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 60, 'max_samples': 1.0, 'max_features': 0.6}</t>
+          <t>{'n_estimators': 80, 'max_samples': 0.7000000000000001, 'max_features': 0.1}</t>
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>1.169445093130892</v>
+        <v>1.029793628643595</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.6973877099584853</v>
+        <v>0.5809364263512919</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.6603644640771158</v>
+        <v>0.6255629841793567</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>1.081408846427147</v>
+        <v>1.014787479546134</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>33.23284875501203</v>
+        <v>27.4810967987101</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -10712,19 +10712,19 @@
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>0.9863392271619424</v>
+        <v>0.989042110317038</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0.5967102898082517</v>
+        <v>0.5443832342669384</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>0.6124985499001064</v>
+        <v>0.6027571740720253</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>0.9931461257850944</v>
+        <v>0.9945059629368936</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>28.21979116324216</v>
+        <v>25.90964437316486</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -10742,19 +10742,19 @@
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>0.9860534896212408</v>
+        <v>1.027430653013953</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>0.6061559384362026</v>
+        <v>0.5566206974670663</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>0.6202990203703371</v>
+        <v>0.6257190283577884</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>0.9930022606324926</v>
+        <v>1.013622539712862</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>28.67627776316378</v>
+        <v>26.22729616712379</v>
       </c>
     </row>
     <row r="20">
@@ -10770,23 +10770,23 @@
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
-          <t>{'subsample': 0.9, 'reg_lambda': 1.0, 'reg_alpha': 0, 'n_estimators': 100, 'min_child_weight': 5, 'max_depth': 3, 'learning_rate': 0.1, 'gamma': 0.2, 'colsample_bytree': 1.0}</t>
+          <t>{'subsample': 0.7, 'reg_lambda': 0.1, 'reg_alpha': 0.1, 'n_estimators': 100, 'min_child_weight': 1, 'max_depth': 9, 'learning_rate': 0.3, 'gamma': 0.3, 'colsample_bytree': 0.8}</t>
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>1.19681845723505</v>
+        <v>1.159666327996474</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>0.7183386589077786</v>
+        <v>0.5550756115087627</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>0.6809973380577451</v>
+        <v>0.6619265481266038</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>1.093991982253549</v>
+        <v>1.076878046947041</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>34.67311154621802</v>
+        <v>25.63781479230106</v>
       </c>
       <c r="I20" s="9" t="inlineStr">
         <is>
@@ -10804,19 +10804,19 @@
         </is>
       </c>
       <c r="L20" s="8" t="n">
-        <v>1.145439011917652</v>
+        <v>1.046239900737698</v>
       </c>
       <c r="M20" s="8" t="n">
-        <v>0.7031106206294501</v>
+        <v>0.5827023239068863</v>
       </c>
       <c r="N20" s="8" t="n">
-        <v>0.6310067525714141</v>
+        <v>0.6212578615265136</v>
       </c>
       <c r="O20" s="8" t="n">
-        <v>1.070251845089581</v>
+        <v>1.022858690503091</v>
       </c>
       <c r="P20" s="8" t="n">
-        <v>33.91402803123471</v>
+        <v>27.88920175189286</v>
       </c>
     </row>
     <row r="21" ht="45.75" customHeight="1">
@@ -10914,23 +10914,23 @@
       </c>
       <c r="C22" s="5" t="inlineStr">
         <is>
-          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>1.1615616</v>
+        <v>2.032901287078857</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0.6071076399999999</v>
+        <v>0.9466550946235657</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>0.7252728000000001</v>
+        <v>0.8024421334266663</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>1.077757676063833</v>
+        <v>1.425798473515404</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>27.61473059654236</v>
+        <v>34.85642373561859</v>
       </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
@@ -10944,23 +10944,23 @@
       </c>
       <c r="K22" s="8" t="inlineStr">
         <is>
-          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+          <t>{'module__num_units': 10, 'module__activation_func': ReLU(), 'lr': 0.1}</t>
         </is>
       </c>
       <c r="L22" s="8" t="n">
-        <v>1.3508712</v>
+        <v>1.15458345413208</v>
       </c>
       <c r="M22" s="8" t="n">
-        <v>0.74966383</v>
+        <v>0.6348726749420166</v>
       </c>
       <c r="N22" s="8" t="n">
-        <v>0.70720756</v>
+        <v>0.6587494611740112</v>
       </c>
       <c r="O22" s="8" t="n">
-        <v>1.162269850477889</v>
+        <v>1.074515450857771</v>
       </c>
       <c r="P22" s="8" t="n">
-        <v>31.905797123909</v>
+        <v>28.71542572975159</v>
       </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
@@ -10976,53 +10976,53 @@
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
+          <t>{'module__num_layers': 1, 'module__hidden_size': 75, 'max_epochs': 10, 'lr': 0.1, 'batch_size': 32}</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="n">
+        <v>1.082300901412964</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>0.7571414113044739</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0.4756202101707458</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <v>1.040336917259483</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>38.65192830562592</v>
+      </c>
+      <c r="I23" s="9" t="inlineStr">
+        <is>
+          <t>Long Short-Term Memory Network</t>
+        </is>
+      </c>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
           <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
         </is>
       </c>
-      <c r="D23" s="5" t="n">
-        <v>0.96529603</v>
-      </c>
-      <c r="E23" s="5" t="n">
-        <v>0.6026895</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>0.55783266</v>
-      </c>
-      <c r="G23" s="5" t="n">
-        <v>0.9824947989910968</v>
-      </c>
-      <c r="H23" s="5" t="n">
-        <v>27.04626619815826</v>
-      </c>
-      <c r="I23" s="9" t="inlineStr">
-        <is>
-          <t>Long Short-Term Memory Network</t>
-        </is>
-      </c>
-      <c r="J23" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K23" s="8" t="inlineStr">
-        <is>
-          <t>{'module__num_layers': 1, 'module__hidden_size': 25, 'max_epochs': 20, 'lr': 0.1, 'batch_size': 16}</t>
-        </is>
-      </c>
       <c r="L23" s="8" t="n">
-        <v>1.3641423</v>
+        <v>0.9280839562416077</v>
       </c>
       <c r="M23" s="8" t="n">
-        <v>0.76541257</v>
+        <v>0.5547460913658142</v>
       </c>
       <c r="N23" s="8" t="n">
-        <v>0.46450892</v>
+        <v>0.5543962121009827</v>
       </c>
       <c r="O23" s="8" t="n">
-        <v>1.167965024604087</v>
+        <v>0.9633711414826622</v>
       </c>
       <c r="P23" s="8" t="n">
-        <v>38.79449665546417</v>
+        <v>28.01969945430756</v>
       </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
@@ -11042,19 +11042,19 @@
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>3.017023324966431</v>
+        <v>2.970662832260132</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>1.413211822509766</v>
+        <v>1.264397501945496</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>0.7693153023719788</v>
+        <v>0.7948250770568848</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>1.736958066553833</v>
+        <v>1.723561090376588</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>68.37573051452637</v>
+        <v>51.14279389381409</v>
       </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
@@ -11072,19 +11072,19 @@
         </is>
       </c>
       <c r="L24" s="8" t="n">
-        <v>4.010422229766846</v>
+        <v>1.911144614219666</v>
       </c>
       <c r="M24" s="8" t="n">
-        <v>1.706381797790527</v>
+        <v>1.039782047271729</v>
       </c>
       <c r="N24" s="8" t="n">
-        <v>0.956902027130127</v>
+        <v>0.6874441504478455</v>
       </c>
       <c r="O24" s="8" t="n">
-        <v>2.00260386241684</v>
+        <v>1.382441540977291</v>
       </c>
       <c r="P24" s="8" t="n">
-        <v>84.01063680648804</v>
+        <v>47.27357029914856</v>
       </c>
     </row>
   </sheetData>
@@ -11258,19 +11258,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.025726045133048</v>
+        <v>0.9736012325831581</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.5965767843143749</v>
+        <v>0.5489843625788092</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.6125056140382089</v>
+        <v>0.5790037458731481</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.012781341224772</v>
+        <v>0.9867123352746524</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>28.03458784180085</v>
+        <v>26.26884889509476</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -11288,19 +11288,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>1.025726045133048</v>
+        <v>1.018420590302328</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.5965767843143749</v>
+        <v>0.5826218317915872</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.6125056140382089</v>
+        <v>0.5894666982864859</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>1.012781341224772</v>
+        <v>1.009168266594985</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>28.03458784180085</v>
+        <v>27.57038782826354</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -11320,19 +11320,19 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>1.060034020968848</v>
+        <v>1.060034030771953</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.5651037116684536</v>
+        <v>0.5651037034072864</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.6414090661709061</v>
+        <v>0.6414090694288643</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>1.029579536009166</v>
+        <v>1.029579540769898</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>26.35518383915157</v>
+        <v>26.35518344253772</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -11350,19 +11350,19 @@
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>1.060034020968848</v>
+        <v>1.060034030771953</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.5651037116684536</v>
+        <v>0.5651037034072864</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>0.6414090661709061</v>
+        <v>0.6414090694288643</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>1.029579536009166</v>
+        <v>1.029579540769898</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>26.35518383915157</v>
+        <v>26.35518344253772</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -11444,19 +11444,19 @@
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>1.075319051888163</v>
+        <v>1.053168352102168</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.602855473381276</v>
+        <v>0.5531810291393571</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.6030227846725604</v>
+        <v>0.612605577290814</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>1.036975916734889</v>
+        <v>1.026239909622583</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>28.10352604017888</v>
+        <v>26.13504818997771</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -11474,19 +11474,19 @@
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>1.075319051888163</v>
+        <v>1.018168915369256</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.602855473381276</v>
+        <v>0.5574248839651169</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>0.6030227846725604</v>
+        <v>0.5793078342146595</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>1.036975916734889</v>
+        <v>1.009043564653805</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>28.10352604017888</v>
+        <v>26.44569814879439</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -11506,19 +11506,19 @@
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>6.743962481646168</v>
+        <v>6.559853998591093</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>2.517434895983286</v>
+        <v>2.483013887243377</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>1.024009251381629</v>
+        <v>1.024795411510833</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>2.596914030468889</v>
+        <v>2.561221192827963</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>194.1033335874064</v>
+        <v>180.9128544666521</v>
       </c>
       <c r="I11" s="9" t="inlineStr">
         <is>
@@ -11532,23 +11532,23 @@
       </c>
       <c r="K11" s="8" t="inlineStr">
         <is>
-          <t>{'tol': 1e-05, 'power_t': 0.5, 'penalty': 'l2', 'max_iter': 3000, 'loss': 'squared_epsilon_insensitive', 'learning_rate': 'adaptive', 'l1_ratio': 1, 'fit_intercept': False, 'eta0': 0.1, 'alpha': 1}</t>
+          <t>{'tol': 0.001, 'power_t': 0.25, 'penalty': 'none', 'max_iter': 1000, 'loss': 'huber', 'learning_rate': 'adaptive', 'l1_ratio': 0.7, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 0.01}</t>
         </is>
       </c>
       <c r="L11" s="8" t="n">
-        <v>6.743962481646168</v>
+        <v>586.5189793736753</v>
       </c>
       <c r="M11" s="8" t="n">
-        <v>2.517434895983286</v>
+        <v>18.32625131794528</v>
       </c>
       <c r="N11" s="8" t="n">
-        <v>1.024009251381629</v>
+        <v>11.0758304963702</v>
       </c>
       <c r="O11" s="8" t="n">
-        <v>2.596914030468889</v>
+        <v>24.21815392166949</v>
       </c>
       <c r="P11" s="8" t="n">
-        <v>194.1033335874064</v>
+        <v>171.3420902993867</v>
       </c>
     </row>
     <row r="12" ht="45.75" customHeight="1">
@@ -11650,19 +11650,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1.047588904092994</v>
+        <v>1.040268266220368</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.5859830227709439</v>
+        <v>0.5548291554822417</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.6585066244636306</v>
+        <v>0.6061233116299222</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>1.023517906092998</v>
+        <v>1.01993542257359</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>27.52132700130401</v>
+        <v>26.96712196960937</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -11676,23 +11676,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>1.047588904092994</v>
+        <v>1.109233620423083</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.5859830227709439</v>
+        <v>0.5898880035351725</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.6585066244636306</v>
+        <v>0.6395178790276631</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>1.023517906092998</v>
+        <v>1.053201604833131</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>27.52132700130401</v>
+        <v>28.07704192042915</v>
       </c>
     </row>
     <row r="14" ht="28.5" customHeight="1">
@@ -11708,23 +11708,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearRegression()}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>1.136575428094937</v>
+        <v>1.1769259212962</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.7008268560793711</v>
+        <v>0.5877747571529005</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.6701065975371003</v>
+        <v>0.6919099098758194</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>1.066102916277287</v>
+        <v>1.08486216695772</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>32.52689390998577</v>
+        <v>27.15637474037209</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -11738,23 +11738,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearRegression()}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>1.136575428094937</v>
+        <v>2.022141593713858</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.7008268560793711</v>
+        <v>0.8422791303845842</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.6701065975371003</v>
+        <v>0.8028824666594404</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>1.066102916277287</v>
+        <v>1.422020250810043</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>32.52689390998577</v>
+        <v>41.9538774405393</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -11774,19 +11774,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>1.034466283655863</v>
+        <v>1.010120939935155</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.6021847499277053</v>
+        <v>0.5767256487940705</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.6300232566230564</v>
+        <v>0.6215778294035064</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>1.017087156371499</v>
+        <v>1.005047730177605</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>28.13447459432926</v>
+        <v>27.13651987754176</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -11804,19 +11804,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>1.034466283655863</v>
+        <v>1.03741661222156</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.6021847499277053</v>
+        <v>0.5931372606676891</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.6300232566230564</v>
+        <v>0.6300407798478277</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>1.017087156371499</v>
+        <v>1.018536505100117</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>28.13447459432926</v>
+        <v>27.71258786204551</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -11832,23 +11832,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>1.030946374067976</v>
+        <v>1.07414346069204</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0.6078280774686551</v>
+        <v>0.5677112515211038</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>0.6199727596796715</v>
+        <v>0.6250815088296179</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>1.015355294499406</v>
+        <v>1.036408925420869</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>28.58251409067705</v>
+        <v>27.79896257402924</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -11862,23 +11862,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>1.030946374067976</v>
+        <v>1.135181949259563</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>0.6078280774686551</v>
+        <v>0.5887117744368797</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>0.6199727596796715</v>
+        <v>0.6642101052221003</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>1.015355294499406</v>
+        <v>1.065449177229756</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>28.58251409067705</v>
+        <v>27.94129462687777</v>
       </c>
     </row>
     <row r="17" ht="42.75" customHeight="1">
@@ -11960,19 +11960,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>1.043685085308359</v>
+        <v>1.025892948560254</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.5615557165325861</v>
+        <v>0.538473219344597</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.6375099768271617</v>
+        <v>0.6274779002484193</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>1.021609066770827</v>
+        <v>1.01286373642275</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>26.29899214984019</v>
+        <v>25.37042890111345</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -11990,19 +11990,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>1.043685085308359</v>
+        <v>1.051257849417802</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.5615557165325861</v>
+        <v>0.5561267780791738</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.6375099768271617</v>
+        <v>0.63287680711157</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>1.021609066770827</v>
+        <v>1.02530866055925</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>26.29899214984019</v>
+        <v>26.09186215045203</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -12018,23 +12018,23 @@
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>1.031743326240754</v>
+        <v>1.020733071692</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0.5928400678205478</v>
+        <v>0.5502542821922468</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>0.6187083388812457</v>
+        <v>0.6151058001714512</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>1.015747668587407</v>
+        <v>1.010313353218693</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>27.80600298161085</v>
+        <v>26.14966469189263</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -12048,23 +12048,23 @@
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>1.031743326240754</v>
+        <v>1.024708184972271</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>0.5928400678205478</v>
+        <v>0.5823955546254931</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>0.6187083388812457</v>
+        <v>0.6041139856345472</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>1.015747668587407</v>
+        <v>1.012278709137099</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>27.80600298161085</v>
+        <v>27.49624674143175</v>
       </c>
     </row>
     <row r="20" ht="128.25" customHeight="1">
@@ -12084,19 +12084,19 @@
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>1.063166724010315</v>
+        <v>1.115295984650523</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>0.5983700003322728</v>
+        <v>0.5847681958224508</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>0.6573269351491706</v>
+        <v>0.614622670373734</v>
       </c>
       <c r="G20" s="5" t="n">
-        <v>1.031099764334332</v>
+        <v>1.0560757475913</v>
       </c>
       <c r="H20" s="5" t="n">
-        <v>28.1191476402138</v>
+        <v>28.45299074049245</v>
       </c>
       <c r="I20" s="9" t="inlineStr">
         <is>
@@ -12114,19 +12114,19 @@
         </is>
       </c>
       <c r="L20" s="8" t="n">
-        <v>1.063166724010315</v>
+        <v>1.137157753245467</v>
       </c>
       <c r="M20" s="8" t="n">
-        <v>0.5983700003322728</v>
+        <v>0.6157236752474506</v>
       </c>
       <c r="N20" s="8" t="n">
-        <v>0.6573269351491706</v>
+        <v>0.57728985502758</v>
       </c>
       <c r="O20" s="8" t="n">
-        <v>1.031099764334332</v>
+        <v>1.06637599056124</v>
       </c>
       <c r="P20" s="8" t="n">
-        <v>28.1191476402138</v>
+        <v>29.44404001851152</v>
       </c>
     </row>
     <row r="21" ht="45.75" customHeight="1">
@@ -12228,19 +12228,19 @@
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>1.2090324</v>
+        <v>1.082682728767395</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0.5945903</v>
+        <v>0.6360761523246765</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>0.71568507</v>
+        <v>0.6357178688049316</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>1.099560101287642</v>
+        <v>1.040520412470315</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>26.51034593582153</v>
+        <v>28.82529497146606</v>
       </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
@@ -12258,19 +12258,19 @@
         </is>
       </c>
       <c r="L22" s="8" t="n">
-        <v>1.1692282</v>
+        <v>1.222469210624695</v>
       </c>
       <c r="M22" s="8" t="n">
-        <v>0.6135646</v>
+        <v>0.5939397215843201</v>
       </c>
       <c r="N22" s="8" t="n">
-        <v>0.70662445</v>
+        <v>0.7130594849586487</v>
       </c>
       <c r="O22" s="8" t="n">
-        <v>1.081308557324922</v>
+        <v>1.105653295850329</v>
       </c>
       <c r="P22" s="8" t="n">
-        <v>30.0974428653717</v>
+        <v>26.98169648647308</v>
       </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
@@ -12290,19 +12290,19 @@
         </is>
       </c>
       <c r="D23" s="5" t="n">
-        <v>0.8050272000000001</v>
+        <v>0.7134822607040405</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>0.55315566</v>
+        <v>0.4952762126922607</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>0.5167402</v>
+        <v>0.4335200786590576</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>0.8972330727690409</v>
+        <v>0.8446787914373372</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>28.88316214084625</v>
+        <v>28.40691208839417</v>
       </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
@@ -12320,19 +12320,19 @@
         </is>
       </c>
       <c r="L23" s="8" t="n">
-        <v>1.0132549</v>
+        <v>0.8945280909538269</v>
       </c>
       <c r="M23" s="8" t="n">
-        <v>0.6069928999999999</v>
+        <v>0.6118949055671692</v>
       </c>
       <c r="N23" s="8" t="n">
-        <v>0.5900847299999999</v>
+        <v>0.5418525338172913</v>
       </c>
       <c r="O23" s="8" t="n">
-        <v>1.006605623322834</v>
+        <v>0.9457949518546961</v>
       </c>
       <c r="P23" s="8" t="n">
-        <v>26.80328786373138</v>
+        <v>29.57078218460083</v>
       </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
@@ -12352,19 +12352,19 @@
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>4.31737232208252</v>
+        <v>3.68079948425293</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>1.782651305198669</v>
+        <v>1.475096940994263</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>0.9417372941970825</v>
+        <v>1.009523153305054</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>2.077828751866361</v>
+        <v>1.918540977996803</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>102.4152159690857</v>
+        <v>61.71240210533142</v>
       </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
@@ -12382,19 +12382,19 @@
         </is>
       </c>
       <c r="L24" s="8" t="n">
-        <v>3.605465650558472</v>
+        <v>44637.8359375</v>
       </c>
       <c r="M24" s="8" t="n">
-        <v>1.441632509231567</v>
+        <v>171.7847290039062</v>
       </c>
       <c r="N24" s="8" t="n">
-        <v>0.7818022966384888</v>
+        <v>89.68280029296875</v>
       </c>
       <c r="O24" s="8" t="n">
-        <v>1.898806375215354</v>
+        <v>211.2766810073937</v>
       </c>
       <c r="P24" s="8" t="n">
-        <v>60.18291711807251</v>
+        <v>196.4690685272217</v>
       </c>
     </row>
   </sheetData>
@@ -12568,19 +12568,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>1.098046403166383</v>
+        <v>1.041253928731707</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.6181445844567487</v>
+        <v>0.5475614629460549</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.6208096847378437</v>
+        <v>0.5675048653940714</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>1.04787709354026</v>
+        <v>1.020418506658767</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>28.94298347310742</v>
+        <v>26.41716277788088</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -12598,19 +12598,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>1.098046403166383</v>
+        <v>1.045672234533757</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.6181445844567487</v>
+        <v>0.5510165770322789</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.6208096847378437</v>
+        <v>0.5687744388881267</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>1.04787709354026</v>
+        <v>1.022581162809954</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>28.94298347310742</v>
+        <v>26.56672762088602</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -12630,19 +12630,19 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>1.122942864452199</v>
+        <v>1.123288480431352</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.593715812424585</v>
+        <v>0.5707841448904577</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.6629066209150166</v>
+        <v>0.655990168891905</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>1.059689985067425</v>
+        <v>1.059853046620781</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>27.58166446030737</v>
+        <v>26.42253522320975</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -12656,23 +12656,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.001, 'C': 1}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>1.122942864452199</v>
+        <v>1.125339283373666</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>0.593715812424585</v>
+        <v>0.4723494324330565</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>0.6629066209150166</v>
+        <v>0.6548862081645898</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>1.059689985067425</v>
+        <v>1.060820099438951</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>27.58166446030737</v>
+        <v>22.38580003301633</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -12750,23 +12750,23 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
+          <t>{'weights': 'distance', 'n_neighbors': 7}</t>
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>1.177798866659963</v>
+        <v>1.157695917726301</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>0.6278494973701707</v>
+        <v>0.5655979349190648</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.6555188032412358</v>
+        <v>0.651973630036186</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>1.085264422461163</v>
+        <v>1.075962786404019</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>29.44530935326389</v>
+        <v>26.45212343667282</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -12780,23 +12780,23 @@
       </c>
       <c r="K10" s="8" t="inlineStr">
         <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
+          <t>{'weights': 'distance', 'n_neighbors': 8}</t>
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>1.177798866659963</v>
+        <v>1.140702425245243</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>0.6278494973701707</v>
+        <v>0.5756341313248385</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>0.6555188032412358</v>
+        <v>0.6634191615387093</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>1.085264422461163</v>
+        <v>1.068036715307692</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>29.44530935326389</v>
+        <v>26.98792562889476</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -12816,19 +12816,19 @@
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>7.236455296443212</v>
+        <v>6.995195038312325</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>2.609190362967563</v>
+        <v>2.573316858690849</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>1.073744799484691</v>
+        <v>1.087039138698569</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>2.690066039420447</v>
+        <v>2.644843102777994</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>191.1252118958552</v>
+        <v>184.8434017299801</v>
       </c>
       <c r="I11" s="9" t="inlineStr">
         <is>
@@ -12842,23 +12842,23 @@
       </c>
       <c r="K11" s="8" t="inlineStr">
         <is>
-          <t>{'tol': 1e-05, 'power_t': 0.5, 'penalty': 'l2', 'max_iter': 3000, 'loss': 'squared_epsilon_insensitive', 'learning_rate': 'adaptive', 'l1_ratio': 1, 'fit_intercept': False, 'eta0': 0.1, 'alpha': 1}</t>
+          <t>{'tol': 0.0001, 'power_t': 0.5, 'penalty': 'l1', 'max_iter': 1000, 'loss': 'squared_loss', 'learning_rate': 'adaptive', 'l1_ratio': 0.15, 'fit_intercept': True, 'eta0': 0.001, 'alpha': 0.001}</t>
         </is>
       </c>
       <c r="L11" s="8" t="n">
-        <v>7.236455296443212</v>
+        <v>1.097877982691</v>
       </c>
       <c r="M11" s="8" t="n">
-        <v>2.609190362967563</v>
+        <v>0.6758176776571112</v>
       </c>
       <c r="N11" s="8" t="n">
-        <v>1.073744799484691</v>
+        <v>0.5733621040745174</v>
       </c>
       <c r="O11" s="8" t="n">
-        <v>2.690066039420447</v>
+        <v>1.047796727753528</v>
       </c>
       <c r="P11" s="8" t="n">
-        <v>191.1252118958552</v>
+        <v>33.02465265882636</v>
       </c>
     </row>
     <row r="12" ht="45.75" customHeight="1">
@@ -12960,19 +12960,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1.130291446677522</v>
+        <v>1.088969028812504</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0.6362958587288017</v>
+        <v>0.5559005001269616</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.6726274351422084</v>
+        <v>0.6044178671261706</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>1.063151657421236</v>
+        <v>1.043536788432734</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>29.87399707714334</v>
+        <v>26.60727621665499</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -12990,19 +12990,19 @@
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>1.130291446677522</v>
+        <v>1.092771479626788</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>0.6362958587288017</v>
+        <v>0.5500207302364959</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.6726274351422084</v>
+        <v>0.612767098780387</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>1.063151657421236</v>
+        <v>1.045357106268852</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>29.87399707714334</v>
+        <v>25.89395813943439</v>
       </c>
     </row>
     <row r="14">
@@ -13022,19 +13022,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>1.289020896641276</v>
+        <v>1.21128884343003</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>0.6073829628379563</v>
+        <v>0.5702450868052904</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.7021619068179302</v>
+        <v>0.6844226822308489</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>1.135350561122545</v>
+        <v>1.10058568200301</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>27.1708380746172</v>
+        <v>26.01632130910535</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -13052,19 +13052,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>1.289020896641276</v>
+        <v>1.212784247855638</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>0.6073829628379563</v>
+        <v>0.5716358037812416</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.7021619068179302</v>
+        <v>0.6893822418366214</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>1.135350561122545</v>
+        <v>1.101264840016078</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>27.1708380746172</v>
+        <v>26.05981908587709</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -13084,19 +13084,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>1.089346933982708</v>
+        <v>1.072985679596806</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>0.6003299653104298</v>
+        <v>0.5791633330471319</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.6464762700508082</v>
+        <v>0.6198231638588708</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>1.043717842131056</v>
+        <v>1.035850220638489</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>27.90166615353255</v>
+        <v>27.08702490042202</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -13114,19 +13114,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>1.089346933982708</v>
+        <v>1.087338231821077</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>0.6003299653104298</v>
+        <v>0.5841529669686842</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.6464762700508082</v>
+        <v>0.6419761302453962</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>1.043717842131056</v>
+        <v>1.042755115940975</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>27.90166615353255</v>
+        <v>27.19214620946957</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -13142,23 +13142,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>1.181673537840794</v>
+        <v>1.151019560498153</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0.6474854169630636</v>
+        <v>0.5724027504608212</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>0.6828013407565848</v>
+        <v>0.6528104803772782</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>1.087048084419817</v>
+        <v>1.072855796693178</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>30.37605436832797</v>
+        <v>27.15921317076523</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -13172,23 +13172,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>1.181673537840794</v>
+        <v>1.132558315661979</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>0.6474854169630636</v>
+        <v>0.5479417351979875</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>0.6828013407565848</v>
+        <v>0.652320085351795</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>1.087048084419817</v>
+        <v>1.064217231425041</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>30.37605436832797</v>
+        <v>25.78779419068347</v>
       </c>
     </row>
     <row r="17">
@@ -13270,19 +13270,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>1.09771648586682</v>
+        <v>1.096792887995961</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>0.575528399983945</v>
+        <v>0.5692966211408218</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.6340956570524396</v>
+        <v>0.6207096773583929</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>1.047719659960058</v>
+        <v>1.047278801464042</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>26.84829866664889</v>
+        <v>26.50425462236871</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -13300,19 +13300,19 @@
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>1.09771648586682</v>
+        <v>1.10463545964621</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>0.575528399983945</v>
+        <v>0.5430178290009289</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.6340956570524396</v>
+        <v>0.6263007274449816</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>1.047719659960058</v>
+        <v>1.051016393614395</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>26.84829866664889</v>
+        <v>25.30313925435647</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -13328,23 +13328,23 @@
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>1.099959059047031</v>
+        <v>1.028654628859145</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>0.6061072619831371</v>
+        <v>0.5528883337387287</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>0.648378544280057</v>
+        <v>0.5799519961634545</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>1.048789330155027</v>
+        <v>1.014226123139779</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>28.21106287945828</v>
+        <v>26.35229813144506</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -13358,23 +13358,23 @@
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 4, 'max_depth': 10}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>1.099959059047031</v>
+        <v>1.035097757476993</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>0.6061072619831371</v>
+        <v>0.5356298580698851</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>0.648378544280057</v>
+        <v>0.5870352854154404</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>1.048789330155027</v>
+        <v>1.017397541513146</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>28.21106287945828</v>
+        <v>25.45853877437434</v>
       </c>
     </row>
     <row r="20">
@@ -13390,53 +13390,53 @@
       </c>
       <c r="C20" s="5" t="inlineStr">
         <is>
+          <t>{'subsample': 0.7, 'reg_lambda': 1.0, 'reg_alpha': 1.0, 'n_estimators': 300, 'min_child_weight': 1, 'max_depth': 6, 'learning_rate': 0.1, 'gamma': 0.1, 'colsample_bytree': 0.7}</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>1.077467508582459</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>0.5727081163620181</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <v>0.5552985815875268</v>
+      </c>
+      <c r="G20" s="5" t="n">
+        <v>1.038011323918222</v>
+      </c>
+      <c r="H20" s="5" t="n">
+        <v>27.7526604169288</v>
+      </c>
+      <c r="I20" s="9" t="inlineStr">
+        <is>
+          <t>XGBoost Regressor</t>
+        </is>
+      </c>
+      <c r="J20" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K20" s="8" t="inlineStr">
+        <is>
           <t>{'subsample': 1.0, 'reg_lambda': 0, 'reg_alpha': 1.0, 'n_estimators': 700, 'min_child_weight': 1, 'max_depth': 9, 'learning_rate': 0.01, 'gamma': 0.3, 'colsample_bytree': 0.8}</t>
         </is>
       </c>
-      <c r="D20" s="5" t="n">
-        <v>1.136074277951527</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>0.6125240873805112</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>0.6747420707343883</v>
-      </c>
-      <c r="G20" s="5" t="n">
-        <v>1.065867852011462</v>
-      </c>
-      <c r="H20" s="5" t="n">
-        <v>28.63576423507064</v>
-      </c>
-      <c r="I20" s="9" t="inlineStr">
-        <is>
-          <t>XGBoost Regressor</t>
-        </is>
-      </c>
-      <c r="J20" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K20" s="8" t="inlineStr">
-        <is>
-          <t>{'subsample': 1.0, 'reg_lambda': 0, 'reg_alpha': 1.0, 'n_estimators': 700, 'min_child_weight': 1, 'max_depth': 9, 'learning_rate': 0.01, 'gamma': 0.3, 'colsample_bytree': 0.8}</t>
-        </is>
-      </c>
       <c r="L20" s="8" t="n">
-        <v>1.136074277951527</v>
+        <v>1.10840366500667</v>
       </c>
       <c r="M20" s="8" t="n">
-        <v>0.6125240873805112</v>
+        <v>0.5720284059441874</v>
       </c>
       <c r="N20" s="8" t="n">
-        <v>0.6747420707343883</v>
+        <v>0.6327334289762769</v>
       </c>
       <c r="O20" s="8" t="n">
-        <v>1.065867852011462</v>
+        <v>1.052807515648834</v>
       </c>
       <c r="P20" s="8" t="n">
-        <v>28.63576423507064</v>
+        <v>27.11166049953769</v>
       </c>
     </row>
     <row r="21" ht="45.75" customHeight="1">
@@ -13538,19 +13538,19 @@
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>1.3791548</v>
+        <v>1.249694585800171</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>0.69096446</v>
+        <v>0.60197514295578</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>0.78399706</v>
+        <v>0.7005113363265991</v>
       </c>
       <c r="G22" s="5" t="n">
-        <v>1.174374216920958</v>
+        <v>1.11789739502343</v>
       </c>
       <c r="H22" s="5" t="n">
-        <v>29.50025200843811</v>
+        <v>26.68356895446777</v>
       </c>
       <c r="I22" s="9" t="inlineStr">
         <is>
@@ -13564,23 +13564,23 @@
       </c>
       <c r="K22" s="8" t="inlineStr">
         <is>
-          <t>{'module__num_units': 20, 'module__activation_func': Tanh(), 'lr': 0.1}</t>
+          <t>{'module__num_units': 20, 'module__activation_func': ReLU(), 'lr': 0.05}</t>
         </is>
       </c>
       <c r="L22" s="8" t="n">
-        <v>1.2951268</v>
+        <v>1.177631497383118</v>
       </c>
       <c r="M22" s="8" t="n">
-        <v>0.59583354</v>
+        <v>0.8063110709190369</v>
       </c>
       <c r="N22" s="8" t="n">
-        <v>0.70594573</v>
+        <v>0.6464831233024597</v>
       </c>
       <c r="O22" s="8" t="n">
-        <v>1.138036377172864</v>
+        <v>1.085187309814816</v>
       </c>
       <c r="P22" s="8" t="n">
-        <v>26.69007778167725</v>
+        <v>38.00889849662781</v>
       </c>
     </row>
     <row r="23" ht="30.75" customHeight="1">
@@ -13600,19 +13600,19 @@
         </is>
       </c>
       <c r="D23" s="5" t="n">
-        <v>0.98069865</v>
+        <v>0.8102315068244934</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>0.5671819</v>
+        <v>0.4905827045440674</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>0.6448235</v>
+        <v>0.5509503483772278</v>
       </c>
       <c r="G23" s="5" t="n">
-        <v>0.9903022998634804</v>
+        <v>0.9001286057139243</v>
       </c>
       <c r="H23" s="5" t="n">
-        <v>24.46592301130295</v>
+        <v>24.57649260759354</v>
       </c>
       <c r="I23" s="9" t="inlineStr">
         <is>
@@ -13630,19 +13630,19 @@
         </is>
       </c>
       <c r="L23" s="8" t="n">
-        <v>0.8306941</v>
+        <v>0.7599387168884277</v>
       </c>
       <c r="M23" s="8" t="n">
-        <v>0.5118711</v>
+        <v>0.4732000529766083</v>
       </c>
       <c r="N23" s="8" t="n">
-        <v>0.5871014</v>
+        <v>0.5083568096160889</v>
       </c>
       <c r="O23" s="8" t="n">
-        <v>0.9114242038694764</v>
+        <v>0.8717446397245169</v>
       </c>
       <c r="P23" s="8" t="n">
-        <v>24.40357655286789</v>
+        <v>23.43792170286179</v>
       </c>
     </row>
     <row r="24" ht="30.75" customHeight="1">
@@ -13662,19 +13662,19 @@
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>24.74347305297852</v>
+        <v>2.30403208732605</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>3.979507207870483</v>
+        <v>1.159618139266968</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>2.548369169235229</v>
+        <v>0.7518531084060669</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>4.974281159421783</v>
+        <v>1.517903846535099</v>
       </c>
       <c r="H24" s="5" t="n">
-        <v>137.6319408416748</v>
+        <v>62.13180422782898</v>
       </c>
       <c r="I24" s="9" t="inlineStr">
         <is>
@@ -13692,19 +13692,19 @@
         </is>
       </c>
       <c r="L24" s="8" t="n">
-        <v>3.568130970001221</v>
+        <v>1.690353393554688</v>
       </c>
       <c r="M24" s="8" t="n">
-        <v>1.415134429931641</v>
+        <v>0.8335720300674438</v>
       </c>
       <c r="N24" s="8" t="n">
-        <v>1.059643030166626</v>
+        <v>0.7529817819595337</v>
       </c>
       <c r="O24" s="8" t="n">
-        <v>1.888949700230586</v>
+        <v>1.300135913493158</v>
       </c>
       <c r="P24" s="8" t="n">
-        <v>56.30818605422974</v>
+        <v>35.10884642601013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-run opt 1 on fixed ICA data
</commit_message>
<xml_diff>
--- a/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
+++ b/data/performance_sheets/BA11 Overall Model Peformance Results.xlsx
@@ -2085,19 +2085,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>213.8163390130718</v>
+        <v>1.769232701541864</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>13.56103739683302</v>
+        <v>1.02230986261075</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>30.08261470719345</v>
+        <v>1.00898893568755</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>14.6224600875869</v>
+        <v>1.330125069886988</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>181.1983650998126</v>
+        <v>43.86104748747221</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -2115,19 +2115,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>239.5708087408467</v>
+        <v>1.454476084646399</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>14.19397400665806</v>
+        <v>0.9354470705453805</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>31.87488055473336</v>
+        <v>0.9033627821656172</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>15.47807509804907</v>
+        <v>1.206016618727287</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>181.7957328526647</v>
+        <v>40.61210329651929</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -2143,23 +2143,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>185.0771947395382</v>
+        <v>0.5354111383148584</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>13.60278433289607</v>
+        <v>0.4491184414289403</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>38.58250450416094</v>
+        <v>0.9098627937609209</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>13.60430794783543</v>
+        <v>0.7317179363080137</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>182.9487359152741</v>
+        <v>22.30282807451723</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -2173,23 +2173,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>184.4836028368815</v>
+        <v>0.5354209564944966</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>13.58083500245154</v>
+        <v>0.449125360112092</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>38.51911855118092</v>
+        <v>0.9098660631438041</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>13.58247410587929</v>
+        <v>0.7317246452693094</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>182.928595813403</v>
+        <v>22.30308172779294</v>
       </c>
     </row>
     <row r="9" ht="45.75" customHeight="1">
@@ -2267,53 +2267,53 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
+          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.8559409972065409</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.5963268560920627</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.8882263445244392</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.9251707935330324</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>29.8393981630295</v>
+      </c>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>K-Neighbors Regressor</t>
+        </is>
+      </c>
+      <c r="J10" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="8" t="inlineStr">
+        <is>
           <t>{'weights': 'uniform', 'n_neighbors': 1}</t>
         </is>
       </c>
-      <c r="D10" s="5" t="n">
-        <v>161.507027826113</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>11.31730409828494</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>27.65927538975735</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>12.70854153025095</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <v>167.1556434975956</v>
-      </c>
-      <c r="I10" s="9" t="inlineStr">
-        <is>
-          <t>K-Neighbors Regressor</t>
-        </is>
-      </c>
-      <c r="J10" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K10" s="8" t="inlineStr">
-        <is>
-          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
-        </is>
-      </c>
       <c r="L10" s="8" t="n">
-        <v>165.4377330238757</v>
+        <v>1.435310837684936</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>12.51640933612325</v>
+        <v>0.7010335884573395</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>35.43340557312825</v>
+        <v>0.89733538391769</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>12.86226002784408</v>
+        <v>1.198044589188956</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>180.2612454608483</v>
+        <v>39.60039431611219</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -2473,23 +2473,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>135.5221357784295</v>
+        <v>0.6488811329960428</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>11.33121791348492</v>
+        <v>0.5989970692348564</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>27.79834007091864</v>
+        <v>0.8067711497696463</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>11.64139750109193</v>
+        <v>0.8055315841083097</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>179.771417240013</v>
+        <v>29.9149724850222</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -2503,23 +2503,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>148.7139732792945</v>
+        <v>0.858212165481929</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>11.91738444442772</v>
+        <v>0.7540729513054227</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>30.15646213820498</v>
+        <v>0.6872331645761827</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>12.19483387665836</v>
+        <v>0.9263974122815375</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>180.7845496936478</v>
+        <v>37.18871789739021</v>
       </c>
     </row>
     <row r="14">
@@ -2539,19 +2539,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>141.0358617660922</v>
+        <v>0.4718473999419967</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>11.80077608074444</v>
+        <v>0.4133690088579485</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>31.4525795694083</v>
+        <v>0.8767948646495074</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>11.87585204379426</v>
+        <v>0.6869114935288219</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>180.786421688723</v>
+        <v>21.24117369036682</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -2569,19 +2569,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>151.5220099846828</v>
+        <v>0.4630258966564034</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>11.71759720410413</v>
+        <v>0.4423815243245858</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>29.39273384494233</v>
+        <v>0.8628642489380264</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>12.30942768713001</v>
+        <v>0.6804600624991913</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>179.534511988419</v>
+        <v>22.36283226403948</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -2597,23 +2597,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>141.7043864106675</v>
+        <v>0.6008169963231103</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>11.81576463736849</v>
+        <v>0.627872637555876</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>34.08609011183047</v>
+        <v>0.8934960082630922</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>11.90396515496696</v>
+        <v>0.7751238586981504</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>180.2945352160393</v>
+        <v>30.16446747970215</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -2627,23 +2627,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 5, 'min_impurity_decrease': 1, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 10, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>164.8897447299939</v>
+        <v>0.9388529150563099</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>12.82737260300344</v>
+        <v>0.9034383327231343</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>36.49368406089806</v>
+        <v>0.9068228875901293</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>12.8409401809211</v>
+        <v>0.9689442270101566</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>181.9352268286076</v>
+        <v>43.96336513139732</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -2663,19 +2663,19 @@
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>106.1750624465927</v>
+        <v>1.23130023875285</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>10.21495150339187</v>
+        <v>0.9753180194444772</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>27.81091788784975</v>
+        <v>0.8709861592358131</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>10.30412841760975</v>
+        <v>1.109639688706586</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>177.8483815914194</v>
+        <v>49.09506984518232</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -2689,23 +2689,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>119.7957814552441</v>
+        <v>2.113900544465133</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>10.89442732128727</v>
+        <v>1.300066664303352</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>29.49289694605525</v>
+        <v>0.7121756278967802</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>10.945125922311</v>
+        <v>1.453925907488113</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>179.2844079557333</v>
+        <v>70.73259938775509</v>
       </c>
     </row>
     <row r="17">
@@ -2721,23 +2721,23 @@
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>140.934877760399</v>
+        <v>1.024117707669397</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>11.66901865255594</v>
+        <v>0.7109636682753624</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>32.97529066072916</v>
+        <v>0.9179528046593174</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>11.87159962938437</v>
+        <v>1.011987009634707</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>179.7444706316188</v>
+        <v>40.67579859222572</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -2751,23 +2751,23 @@
       </c>
       <c r="K17" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'loss': 'square', 'learning_rate': 0.01}</t>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>145.0307762207937</v>
+        <v>0.5542382996023565</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>11.96097410073012</v>
+        <v>0.5781278298896819</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>33.21734443768007</v>
+        <v>0.8550784265152902</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>12.04287242400224</v>
+        <v>0.7444718259291996</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>180.7185421901526</v>
+        <v>27.52170643676115</v>
       </c>
     </row>
     <row r="18" ht="27.95" customHeight="1">
@@ -2783,53 +2783,53 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
+          <t>{'n_estimators': 50, 'max_samples': 0.7000000000000001, 'max_features': 0.9}</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>1.431472544992964</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>1.082515978490064</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0.8753364572936239</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <v>1.196441617879019</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>54.78406336146282</v>
+      </c>
+      <c r="I18" s="9" t="inlineStr">
+        <is>
+          <t>BaggingRegressor</t>
+        </is>
+      </c>
+      <c r="J18" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K18" s="8" t="inlineStr">
+        <is>
           <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
         </is>
       </c>
-      <c r="D18" s="5" t="n">
-        <v>141.7146966534518</v>
-      </c>
-      <c r="E18" s="5" t="n">
-        <v>11.8923210622738</v>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>33.85736517888689</v>
-      </c>
-      <c r="G18" s="5" t="n">
-        <v>11.90439820627031</v>
-      </c>
-      <c r="H18" s="5" t="n">
-        <v>180.7371108914126</v>
-      </c>
-      <c r="I18" s="9" t="inlineStr">
-        <is>
-          <t>BaggingRegressor</t>
-        </is>
-      </c>
-      <c r="J18" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K18" s="8" t="inlineStr">
-        <is>
-          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
-        </is>
-      </c>
       <c r="L18" s="8" t="n">
-        <v>133.5188783536586</v>
+        <v>1.047830739546428</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>11.53584619261317</v>
+        <v>0.9843985316817765</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>32.22712430902885</v>
+        <v>0.7595414157531426</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>11.55503692567266</v>
+        <v>1.023636038612567</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>180.1994978012069</v>
+        <v>48.73250361186899</v>
       </c>
     </row>
     <row r="19" ht="27.95" customHeight="1">
@@ -2849,19 +2849,19 @@
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>95.89740018828086</v>
+        <v>1.540484131543442</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>9.645942860468804</v>
+        <v>1.074220522769573</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>27.61455336742408</v>
+        <v>0.885703561990854</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>9.792721796736638</v>
+        <v>1.241162411428675</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>176.159016666245</v>
+        <v>57.39760669372957</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -2875,23 +2875,23 @@
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>89.95393324877827</v>
+        <v>1.393132975402805</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>9.258686531792584</v>
+        <v>1.024300859750056</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>26.02390230032488</v>
+        <v>0.9282612942656259</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>9.484404738768704</v>
+        <v>1.180310541934962</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>174.5726954783764</v>
+        <v>52.51273754345118</v>
       </c>
     </row>
     <row r="20" ht="42.75" customHeight="1">
@@ -3397,19 +3397,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>158.9744102796962</v>
+        <v>1.443177585675457</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>11.22754077236819</v>
+        <v>0.9596520279243288</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>4.777805672492045</v>
+        <v>0.4575946204779743</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>12.60850547367515</v>
+        <v>1.20132326443612</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>130.0977315084083</v>
+        <v>40.52912424177863</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -3427,19 +3427,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>183.438910199954</v>
+        <v>1.198252523016234</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>12.0645583056421</v>
+        <v>0.8543265053434743</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>5.167369451284474</v>
+        <v>0.3978033107629965</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>13.5439621307782</v>
+        <v>1.094647213953534</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>131.7310410134532</v>
+        <v>39.17638434807445</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -3455,23 +3455,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>138.3341656852436</v>
+        <v>0.4700525441291818</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>11.74623284290611</v>
+        <v>0.4234313562215242</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>5.982344866082618</v>
+        <v>0.4023499853044116</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>11.76155456073914</v>
+        <v>0.6856037807138915</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>140.2990198154174</v>
+        <v>20.30674979644189</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -3485,23 +3485,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>138.3599004373704</v>
+        <v>0.4700580982366084</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>11.74755181800329</v>
+        <v>0.4234284324734668</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>5.981165572301412</v>
+        <v>0.4023511300861887</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>11.762648529875</v>
+        <v>0.6856078312246794</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>140.3089376995914</v>
+        <v>20.30661577910789</v>
       </c>
     </row>
     <row r="9" ht="183" customHeight="1">
@@ -3579,23 +3579,23 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 2}</t>
+          <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>123.9541149554842</v>
+        <v>0.6154295084234465</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>10.39187042072695</v>
+        <v>0.54974246183925</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>4.902755019275828</v>
+        <v>0.3988007499354917</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>11.13346823570644</v>
+        <v>0.7844931538410304</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>130.1404591714005</v>
+        <v>26.68833903779967</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -3609,23 +3609,23 @@
       </c>
       <c r="K10" s="8" t="inlineStr">
         <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
+          <t>{'weights': 'distance', 'n_neighbors': 6}</t>
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>130.0021526356227</v>
+        <v>0.5369682634272699</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>11.13525292039445</v>
+        <v>0.5248078770963078</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>5.609722899776675</v>
+        <v>0.3715318465888818</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>11.40184864991738</v>
+        <v>0.7327811838654633</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>136.6463077980497</v>
+        <v>25.29541425197888</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -3785,23 +3785,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>100.8923633974045</v>
+        <v>0.8464520639398175</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>9.762969052326142</v>
+        <v>0.7311504864325359</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>4.55581794491934</v>
+        <v>0.3492544752211116</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>10.0445190724795</v>
+        <v>0.9200282951843479</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>131.6843980149396</v>
+        <v>36.60504784833064</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -3815,23 +3815,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 50}</t>
+          <t>{'rf__n_estimators': 200, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>123.3751802203941</v>
+        <v>0.746042471161584</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>10.82252228056753</v>
+        <v>0.7108766557934925</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>5.03864456295055</v>
+        <v>0.3357585642194387</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>11.10743805836405</v>
+        <v>0.8637375013055668</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>136.3540466346784</v>
+        <v>34.49018278160485</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -3847,23 +3847,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>149.6623750343091</v>
+        <v>0.627915878536274</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>11.59522034423923</v>
+        <v>0.4934616741972525</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>6.471001271863921</v>
+        <v>0.4708113357667477</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>12.23365746758953</v>
+        <v>0.7924114326133073</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>135.93042942859</v>
+        <v>22.22213473770726</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -3881,19 +3881,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>117.767003379292</v>
+        <v>0.5018713459605403</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>10.67695983742053</v>
+        <v>0.3980635171176031</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>5.23330558693812</v>
+        <v>0.4101960138657624</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>10.85205065318496</v>
+        <v>0.7084287867954974</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>135.8840069436641</v>
+        <v>19.23382721475109</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -3909,23 +3909,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>118.5150363593</v>
+        <v>0.5527599280954707</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>10.85589292202144</v>
+        <v>0.6136309601425133</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>5.540789335674413</v>
+        <v>0.4206626399318599</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>10.88646114948747</v>
+        <v>0.7434782633644851</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>136.9369168195906</v>
+        <v>28.62807090113444</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -3939,23 +3939,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': None, 'max_depth': 15, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>111.4516430337855</v>
+        <v>0.6209700678170409</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>10.49971981948138</v>
+        <v>0.660683635214852</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>5.25060248475229</v>
+        <v>0.420953942535312</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>10.55706602393797</v>
+        <v>0.7880165403194535</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>135.5312020824626</v>
+        <v>31.20632109076831</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -3971,23 +3971,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>76.34711966397535</v>
+        <v>2.23833831607516</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>8.570980618387528</v>
+        <v>1.362099442895907</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>4.159753250952243</v>
+        <v>0.5660019156074769</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>8.737683884415558</v>
+        <v>1.496107722082591</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>126.1216069019241</v>
+        <v>74.09468874848125</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -4005,19 +4005,19 @@
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>101.9747930288503</v>
+        <v>2.036686802195669</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>10.02371662522081</v>
+        <v>1.269211342571213</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>4.954295503441731</v>
+        <v>0.5249270327736971</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>10.09825693022565</v>
+        <v>1.427125363167395</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>133.5259555379661</v>
+        <v>68.70518391116607</v>
       </c>
     </row>
     <row r="17" ht="42.75" customHeight="1">
@@ -4033,53 +4033,53 @@
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>0.507846194096621</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.5091754028367175</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0.4056806992639247</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <v>0.7126332816369307</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <v>24.10101384773738</v>
+      </c>
+      <c r="I17" s="9" t="inlineStr">
+        <is>
+          <t>AdaBoostRegressor</t>
+        </is>
+      </c>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="inlineStr">
+        <is>
           <t>{'n_estimators': 50, 'loss': 'linear', 'learning_rate': 0.01}</t>
         </is>
       </c>
-      <c r="D17" s="5" t="n">
-        <v>109.145251888653</v>
-      </c>
-      <c r="E17" s="5" t="n">
-        <v>10.37533867555989</v>
-      </c>
-      <c r="F17" s="5" t="n">
-        <v>5.215174276767614</v>
-      </c>
-      <c r="G17" s="5" t="n">
-        <v>10.44726049683136</v>
-      </c>
-      <c r="H17" s="5" t="n">
-        <v>134.9070487286027</v>
-      </c>
-      <c r="I17" s="9" t="inlineStr">
-        <is>
-          <t>AdaBoostRegressor</t>
-        </is>
-      </c>
-      <c r="J17" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K17" s="8" t="inlineStr">
-        <is>
-          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
-        </is>
-      </c>
       <c r="L17" s="8" t="n">
-        <v>122.8537381435135</v>
+        <v>0.8764326845026739</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>10.94393352078239</v>
+        <v>0.6396903835521888</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>5.320438810088163</v>
+        <v>0.346665997505735</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>11.08394055124411</v>
+        <v>0.9361798355565419</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>137.0899645124008</v>
+        <v>32.28071407598027</v>
       </c>
     </row>
     <row r="18" ht="42" customHeight="1">
@@ -4095,23 +4095,23 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 80, 'max_samples': 0.7000000000000001, 'max_features': 0.1}</t>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>105.9560890218211</v>
+        <v>1.122958451463104</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>10.23630572891851</v>
+        <v>0.9993826542595892</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>5.24019759136548</v>
+        <v>0.4944358551210494</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>10.29349741447586</v>
+        <v>1.05969733955649</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>134.2473976438846</v>
+        <v>48.11527237037399</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -4125,23 +4125,23 @@
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 80, 'max_samples': 0.7000000000000001, 'max_features': 0.1}</t>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>115.7606929888626</v>
+        <v>1.198105754328884</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>10.72357129397382</v>
+        <v>1.040215895071614</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>5.468411518950822</v>
+        <v>0.4931903644977592</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>10.7592143295346</v>
+        <v>1.09458017263647</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>136.3653671807099</v>
+        <v>50.37082563242917</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -4161,19 +4161,19 @@
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>101.0218550177319</v>
+        <v>1.154057600911361</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>9.679620979108662</v>
+        <v>0.9140027000188681</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>4.87099129145491</v>
+        <v>0.4630255458682873</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>10.05096289007834</v>
+        <v>1.074270729802949</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>129.7013227647717</v>
+        <v>45.53642856111317</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -4187,23 +4187,23 @@
       </c>
       <c r="K19" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>105.0024649518852</v>
+        <v>0.8183543122685908</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>10.08607359498114</v>
+        <v>0.7283061969012877</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>5.215994667081008</v>
+        <v>0.4382065922750457</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>10.24707104258994</v>
+        <v>0.9046293784023327</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>132.9398125979116</v>
+        <v>35.3656838028893</v>
       </c>
     </row>
     <row r="20" ht="128.25" customHeight="1">
@@ -4709,19 +4709,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>240.6562662892612</v>
+        <v>0.5804310525865963</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>14.37630458250666</v>
+        <v>0.5948923478381558</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.9554887903667054</v>
+        <v>0.2488588521082821</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>15.5130998285082</v>
+        <v>0.7618602579125625</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>183.0646534649585</v>
+        <v>23.58702784933934</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -4739,19 +4739,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>241.0115602001964</v>
+        <v>0.507305681784554</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>14.38805807341825</v>
+        <v>0.5383454824504699</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.9568560289846385</v>
+        <v>0.22715147822155</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>15.52454702077315</v>
+        <v>0.712253944730778</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>183.5288978668657</v>
+        <v>21.16884484095739</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -4767,23 +4767,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>243.1531786336676</v>
+        <v>0.4857192089930711</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>14.38846317876686</v>
+        <v>0.4278962984523826</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.9337394734508088</v>
+        <v>0.3868131122913781</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>15.59336970105139</v>
+        <v>0.6969355845363839</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>176.8746333491799</v>
+        <v>20.52554387072879</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -4797,23 +4797,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>243.1383311843655</v>
+        <v>0.485729719806678</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>14.38790515642364</v>
+        <v>0.4278926157414357</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>0.9336842169244747</v>
+        <v>0.3868179179807086</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>15.59289361165417</v>
+        <v>0.6969431252309459</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>176.8567681982798</v>
+        <v>20.52534178099097</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -4891,23 +4891,23 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>{'weights': 'distance', 'n_neighbors': 7}</t>
+          <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>242.4696725781817</v>
+        <v>0.5260819421271655</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>14.36829886097157</v>
+        <v>0.5465775861011675</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.9322850323108952</v>
+        <v>0.3860397311064874</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>15.5714377171211</v>
+        <v>0.7253150640426307</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>176.3903402733384</v>
+        <v>25.9213566665146</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -4925,19 +4925,19 @@
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>242.9411750574015</v>
+        <v>0.4381387257472351</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>14.38205359053171</v>
+        <v>0.483926078482028</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>0.9333616862819741</v>
+        <v>0.3641263583106026</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>15.58657034300367</v>
+        <v>0.6619204829488472</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>176.8034437208556</v>
+        <v>23.18374159098116</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -5101,19 +5101,19 @@
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>243.378010708805</v>
+        <v>0.4078913521835428</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>14.42132238171461</v>
+        <v>0.5549573881232133</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.9448158152503722</v>
+        <v>0.2772505349915751</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>15.6005772556276</v>
+        <v>0.6386637238669054</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>179.925308929443</v>
+        <v>26.628117688169</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -5127,23 +5127,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>243.4188084477343</v>
+        <v>0.2527719733142195</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>14.42966226651145</v>
+        <v>0.4332281470334858</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.9481878958087796</v>
+        <v>0.2398930822333896</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>15.60188477228743</v>
+        <v>0.5027643317840074</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>180.857972629812</v>
+        <v>20.79213270769238</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -5163,19 +5163,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>243.0347437834212</v>
+        <v>0.5467814814061386</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>14.36700250429444</v>
+        <v>0.426320826543279</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.925017352627632</v>
+        <v>0.4131063878748897</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>15.58957163566149</v>
+        <v>0.7394467400740493</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>174.8004727845133</v>
+        <v>20.20242213493225</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -5189,23 +5189,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
+          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>241.2257081814366</v>
+        <v>0.5185524376169465</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>14.29831689658993</v>
+        <v>0.4000087281950603</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.9200285868485021</v>
+        <v>0.3955689970634569</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>15.53144256601545</v>
+        <v>0.7201058516752564</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>172.9913853578928</v>
+        <v>19.33836587729197</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -5221,23 +5221,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>243.8484839956338</v>
+        <v>0.527053744479462</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>14.40810403410933</v>
+        <v>0.6063648449891953</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.9346618716484465</v>
+        <v>0.4076488159042245</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>15.61564868955606</v>
+        <v>0.7259846723447142</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>177.2495940599183</v>
+        <v>28.2517256319913</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -5251,23 +5251,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 10, 'min_impurity_decrease': 0, 'max_leaf_nodes': 20, 'max_features': 'log2', 'max_depth': 20, 'learning_rate': 0.05}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>243.8484839956338</v>
+        <v>0.5855659610844781</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>14.40810403410933</v>
+        <v>0.645263524480183</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.9346618716484465</v>
+        <v>0.4193624233324351</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>15.61564868955606</v>
+        <v>0.7652228179324491</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>177.2495940599183</v>
+        <v>29.98960464611356</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -5287,19 +5287,19 @@
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>245.2861600129148</v>
+        <v>0.971049581455485</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>14.45843776837312</v>
+        <v>0.9402550875162459</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>0.9414628971292403</v>
+        <v>0.4587832776558165</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>15.66161422117512</v>
+        <v>0.9854184803703882</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>179.2755015230341</v>
+        <v>44.91306170349021</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -5313,23 +5313,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 2, 'max_depth': None}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>246.8648254388376</v>
+        <v>0.6615054800025688</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>14.52364294767868</v>
+        <v>0.71146978333397</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>0.951973977521001</v>
+        <v>0.3976463411936382</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>15.71193258128476</v>
+        <v>0.8133298715789116</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>182.4515822069793</v>
+        <v>33.62019534324767</v>
       </c>
     </row>
     <row r="17" ht="42.75" customHeight="1">
@@ -5349,19 +5349,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>242.7200169602142</v>
+        <v>0.5715496429581376</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>14.37845326993526</v>
+        <v>0.4924876746568833</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.9331707265390033</v>
+        <v>0.3895187692457379</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>15.57947421963316</v>
+        <v>0.756009023066615</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>176.6885040886813</v>
+        <v>23.82757115408248</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -5379,19 +5379,19 @@
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>243.726554722449</v>
+        <v>0.4663624575586709</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>14.41681046388761</v>
+        <v>0.4609998840738848</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>0.9399803032433556</v>
+        <v>0.3835767847249791</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>15.61174412813793</v>
+        <v>0.6829073564976957</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>178.616409169586</v>
+        <v>22.00177111322367</v>
       </c>
     </row>
     <row r="18" ht="56.1" customHeight="1">
@@ -5411,19 +5411,19 @@
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>245.4070516631837</v>
+        <v>0.9395529721262826</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>14.45985306638602</v>
+        <v>0.9355505665714938</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.9394054797724328</v>
+        <v>0.468505422642724</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>15.66547323457493</v>
+        <v>0.9693054070447986</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>178.8258190181574</v>
+        <v>44.33856880496145</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -5437,23 +5437,23 @@
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 80, 'max_samples': 0.7000000000000001, 'max_features': 0.1}</t>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>244.1488669892477</v>
+        <v>0.95786492569499</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>14.42211859604409</v>
+        <v>0.9389889748784206</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.9375538273604467</v>
+        <v>0.4894802943493622</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>15.62526374143002</v>
+        <v>0.9787057400950452</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>178.0370206836091</v>
+        <v>44.31106315065421</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -5473,19 +5473,19 @@
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>244.4208790964909</v>
+        <v>0.6790554263039367</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>14.43876698069344</v>
+        <v>0.7187632826453487</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>0.9417406590708228</v>
+        <v>0.3931252623569603</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>15.63396555888783</v>
+        <v>0.8240481941633855</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>179.2453100445157</v>
+        <v>34.29006167301126</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -5503,19 +5503,19 @@
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>244.439013742642</v>
+        <v>0.5629968415477786</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>14.45139190103333</v>
+        <v>0.6365169630900936</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>0.9453873906249366</v>
+        <v>0.388238723216196</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>15.63454552401962</v>
+        <v>0.750331154589611</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>180.2444991077866</v>
+        <v>30.15054714015765</v>
       </c>
     </row>
     <row r="20" ht="128.25" customHeight="1">
@@ -26566,19 +26566,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>240.8759668677221</v>
+        <v>0.03315056222995385</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>14.38492014482672</v>
+        <v>0.1476600338299492</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.9559510267913478</v>
+        <v>0.3343543601020191</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>15.52017934392905</v>
+        <v>0.1820729585357305</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>183.1887413129058</v>
+        <v>31.45267805898039</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -26596,19 +26596,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>241.0887246160163</v>
+        <v>0.02418280517125763</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>14.3889158067735</v>
+        <v>0.1244585526796847</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.9559300224874552</v>
+        <v>0.311597459303614</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>15.52703206076474</v>
+        <v>0.1555082157677131</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>183.0820377721972</v>
+        <v>30.20593206599377</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -26628,19 +26628,19 @@
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>243.0390034136249</v>
+        <v>0.06391746905278159</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>14.38486779631906</v>
+        <v>0.1963585720647092</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.9333431384773434</v>
+        <v>0.8209663255622688</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>15.58970825299899</v>
+        <v>0.2528190440864406</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>176.7571616967685</v>
+        <v>36.51598115602491</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -26658,19 +26658,19 @@
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>243.0968427014847</v>
+        <v>0.06333046724204258</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>14.38672587399908</v>
+        <v>0.1951620105631108</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>0.933498147624193</v>
+        <v>0.8199944884028048</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>15.59156318979866</v>
+        <v>0.2516554534319544</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>176.8101489648907</v>
+        <v>36.32649302535467</v>
       </c>
     </row>
     <row r="9" ht="30.75" customHeight="1">
@@ -26748,53 +26748,53 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.0731357616844846</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.2134835529385756</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.8201068471083037</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.270436243289402</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>39.94742835395629</v>
+      </c>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>K-Neighbors Regressor</t>
+        </is>
+      </c>
+      <c r="J10" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="8" t="inlineStr">
+        <is>
           <t>{'weights': 'uniform', 'n_neighbors': 9}</t>
         </is>
       </c>
-      <c r="D10" s="5" t="n">
-        <v>243.5370308577884</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>14.40620875193379</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0.9360799889862575</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>15.6056730344381</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <v>177.6463255926339</v>
-      </c>
-      <c r="I10" s="9" t="inlineStr">
-        <is>
-          <t>K-Neighbors Regressor</t>
-        </is>
-      </c>
-      <c r="J10" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K10" s="8" t="inlineStr">
-        <is>
-          <t>{'weights': 'distance', 'n_neighbors': 3}</t>
-        </is>
-      </c>
       <c r="L10" s="8" t="n">
-        <v>242.457463673753</v>
+        <v>0.06755142078278834</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>14.37539542850807</v>
+        <v>0.2039277841972753</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>0.9367706468895632</v>
+        <v>0.7926528588029638</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>15.57104568337506</v>
+        <v>0.2599065616385787</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>177.5406600529724</v>
+        <v>38.1419866611859</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -26954,23 +26954,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>243.244138318315</v>
+        <v>0.05166675673210638</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>14.41947100932368</v>
+        <v>0.1840373406246086</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.9454275601679715</v>
+        <v>0.572982789818138</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>15.59628604246264</v>
+        <v>0.2273032264005647</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>180.0976723879394</v>
+        <v>35.57074358712617</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -26984,23 +26984,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 100}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>243.5158706994976</v>
+        <v>0.04790033476850457</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>14.43270215747562</v>
+        <v>0.1618684099403406</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>0.9467628913017915</v>
+        <v>0.498168537927996</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>15.60499505605489</v>
+        <v>0.2188614510792263</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>180.5734249992165</v>
+        <v>31.85824670039957</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -27020,19 +27020,19 @@
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>239.8692687989359</v>
+        <v>0.101628748133242</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>14.26507355702452</v>
+        <v>0.2395949568166445</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.9186045033392765</v>
+        <v>1.219152930298395</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>15.48771347872035</v>
+        <v>0.318792641278374</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>172.4393798664549</v>
+        <v>39.63267714965917</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -27050,19 +27050,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>240.6412530290474</v>
+        <v>0.1341502786014555</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>14.27027233132535</v>
+        <v>0.2752798081324091</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>0.9137167134928713</v>
+        <v>1.261233145293909</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>15.5126159312041</v>
+        <v>0.3662653117638299</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>171.5276103963667</v>
+        <v>48.32175316244035</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -27082,19 +27082,19 @@
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>243.8484839956338</v>
+        <v>0.07159066282081683</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>14.40810403410933</v>
+        <v>0.2128146409749657</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.9346618716484465</v>
+        <v>0.8407144707345121</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>15.61564868955606</v>
+        <v>0.2675643152978678</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>177.2495940599183</v>
+        <v>39.16633162853304</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -27112,19 +27112,19 @@
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>243.8484839956338</v>
+        <v>0.07159066282081683</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>14.40810403410933</v>
+        <v>0.2128146409749657</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>0.9346618716484465</v>
+        <v>0.8407144707345121</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>15.61564868955606</v>
+        <v>0.2675643152978678</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>177.2495940599183</v>
+        <v>39.16633162853304</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -27140,23 +27140,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 30}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 2, 'max_depth': 10}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>244.1072021869969</v>
+        <v>0.07869640901856262</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>14.42823186538505</v>
+        <v>0.2379152121396042</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>0.9417259793049334</v>
+        <v>0.7306855549079274</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>15.62393043337677</v>
+        <v>0.2805288024759002</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>179.0878900330491</v>
+        <v>45.7270760113422</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -27174,19 +27174,19 @@
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>244.5524988954338</v>
+        <v>0.08145873611560754</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>14.45825619338385</v>
+        <v>0.2121982297962995</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>0.9446105664496006</v>
+        <v>0.7230123009399867</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>15.63817441057088</v>
+        <v>0.2854097687809714</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>180.2656773729982</v>
+        <v>40.17942123076487</v>
       </c>
     </row>
     <row r="17" ht="42.75" customHeight="1">
@@ -27202,23 +27202,23 @@
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'loss': 'exponential', 'learning_rate': 0.01}</t>
+          <t>{'n_estimators': 250, 'loss': 'exponential', 'learning_rate': 0.01}</t>
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>243.2135001645385</v>
+        <v>0.06499820783617426</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>14.39540737980159</v>
+        <v>0.2103171763419817</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>0.9362688686081541</v>
+        <v>0.7478066826054257</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>15.5953037855804</v>
+        <v>0.2549474609329818</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>177.5345642927484</v>
+        <v>39.57524338653875</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -27236,19 +27236,19 @@
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>243.4137090455806</v>
+        <v>0.04658276588573607</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>14.41202193946667</v>
+        <v>0.1779718230358435</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>0.9420313460482426</v>
+        <v>0.7174890083786107</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>15.60172134879932</v>
+        <v>0.215830410011509</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>179.1054020511808</v>
+        <v>34.46715592375804</v>
       </c>
     </row>
     <row r="18" ht="42" customHeight="1">
@@ -27264,23 +27264,23 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
+          <t>{'n_estimators': 50, 'max_samples': 0.7000000000000001, 'max_features': 0.9}</t>
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>244.8341665405792</v>
+        <v>0.07461774278854551</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>14.44677784062994</v>
+        <v>0.2239750833301102</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>0.9406047156683017</v>
+        <v>0.7511479492432943</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>15.64717759024225</v>
+        <v>0.2731624842260472</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>178.9606220088916</v>
+        <v>41.95069882333044</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -27294,23 +27294,23 @@
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 130, 'max_samples': 0.8, 'max_features': 0.6}</t>
+          <t>{'n_estimators': 80, 'max_samples': 0.7000000000000001, 'max_features': 0.1}</t>
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>245.5753838656393</v>
+        <v>0.072129706906121</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>14.47396789815944</v>
+        <v>0.2127470047834389</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>0.9442491666524354</v>
+        <v>0.7725352384833154</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>15.67084502717193</v>
+        <v>0.2685697430950125</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>180.0888922440634</v>
+        <v>39.7552940899879</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -27326,53 +27326,53 @@
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
+          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>0.06952300739878484</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>0.2070012627623057</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>0.6648519731671538</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>0.2636721589375428</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>39.64639839064865</v>
+      </c>
+      <c r="I19" s="9" t="inlineStr">
+        <is>
+          <t>ExtraTreesRegressor</t>
+        </is>
+      </c>
+      <c r="J19" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K19" s="8" t="inlineStr">
+        <is>
           <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
         </is>
       </c>
-      <c r="D19" s="5" t="n">
-        <v>244.9838871861681</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <v>14.45522173901107</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>0.9426351416918962</v>
-      </c>
-      <c r="G19" s="5" t="n">
-        <v>15.65196112907798</v>
-      </c>
-      <c r="H19" s="5" t="n">
-        <v>179.5404927374476</v>
-      </c>
-      <c r="I19" s="9" t="inlineStr">
-        <is>
-          <t>ExtraTreesRegressor</t>
-        </is>
-      </c>
-      <c r="J19" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K19" s="8" t="inlineStr">
-        <is>
-          <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
-        </is>
-      </c>
       <c r="L19" s="8" t="n">
-        <v>245.2252610721424</v>
+        <v>0.06525338315817054</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>14.46829584556836</v>
+        <v>0.1995262350212016</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>0.9451437691337127</v>
+        <v>0.6993532293178434</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>15.65966989026724</v>
+        <v>0.2554474175993379</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>180.3128007315614</v>
+        <v>37.86595455425887</v>
       </c>
     </row>
     <row r="20" ht="128.25" customHeight="1">
@@ -27880,19 +27880,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>200.172372057822</v>
+        <v>0.05367575929621722</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>13.2637107499197</v>
+        <v>0.1804193489533207</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>28.56874489632778</v>
+        <v>0.6388930342504122</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>14.14822858374228</v>
+        <v>0.2316802954422694</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>182.282186075038</v>
+        <v>36.15785340575221</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -27910,19 +27910,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>211.8990775066814</v>
+        <v>0.04615325272703776</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>13.54041881387108</v>
+        <v>0.1692240456006783</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>29.39807095438232</v>
+        <v>0.585345857429775</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>14.55675367335318</v>
+        <v>0.2148330810816569</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>181.9896724673766</v>
+        <v>33.80879160082123</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -27938,23 +27938,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>185.0012271958868</v>
+        <v>0.06715432607692697</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>13.6000915404775</v>
+        <v>0.2049415301936128</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>38.56654573375957</v>
+        <v>0.9413512156694218</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>13.60151562127864</v>
+        <v>0.2591415174705261</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>182.9502945942912</v>
+        <v>38.35610951144575</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -27968,23 +27968,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 100}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>184.102532485005</v>
+        <v>0.06721253525522927</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>13.56686856983595</v>
+        <v>0.2049261476654589</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>38.47910214626955</v>
+        <v>0.9405178565272493</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>13.56843883742728</v>
+        <v>0.2592538047073356</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>182.9121275253395</v>
+        <v>38.3554598534757</v>
       </c>
     </row>
     <row r="9" ht="45.75" customHeight="1">
@@ -28062,53 +28062,53 @@
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
+          <t>{'weights': 'uniform', 'n_neighbors': 1}</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>0.1191687281007852</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0.2725588763396568</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>1.084936911565008</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>0.3452082387498671</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>53.39784823080357</v>
+      </c>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>K-Neighbors Regressor</t>
+        </is>
+      </c>
+      <c r="J10" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K10" s="8" t="inlineStr">
+        <is>
           <t>{'weights': 'uniform', 'n_neighbors': 5}</t>
         </is>
       </c>
-      <c r="D10" s="5" t="n">
-        <v>159.8097048765044</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>12.38205052806046</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>35.04035251951674</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <v>12.64158632753439</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <v>180.7622274228935</v>
-      </c>
-      <c r="I10" s="9" t="inlineStr">
-        <is>
-          <t>K-Neighbors Regressor</t>
-        </is>
-      </c>
-      <c r="J10" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K10" s="8" t="inlineStr">
-        <is>
-          <t>{'weights': 'uniform', 'n_neighbors': 1}</t>
-        </is>
-      </c>
       <c r="L10" s="8" t="n">
-        <v>195.6905887850585</v>
+        <v>0.08405274052389124</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>12.87902460393052</v>
+        <v>0.2297373510391769</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>37.47515040245671</v>
+        <v>0.9270374120824035</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>13.98894523490097</v>
+        <v>0.2899185066943661</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>174.8494786778928</v>
+        <v>43.36209737293908</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -28268,23 +28268,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>146.2212179146187</v>
+        <v>0.06128108179095727</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>11.82554040996049</v>
+        <v>0.1978164270836612</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>29.74240601214563</v>
+        <v>0.7131082485883615</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>12.09219657112051</v>
+        <v>0.2475501601513465</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>180.853476998894</v>
+        <v>38.48139893743166</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -28298,23 +28298,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 50, 'gb__n_estimators': 100}</t>
+          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>103.2094818990566</v>
+        <v>0.06100114903964915</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>9.620544777690368</v>
+        <v>0.2037714975606461</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>23.0864848943774</v>
+        <v>0.7310302114760669</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>10.15920675540451</v>
+        <v>0.246984106856391</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>175.9444547048871</v>
+        <v>39.44731154605231</v>
       </c>
     </row>
     <row r="14">
@@ -28330,23 +28330,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearSVR(random_state=42)}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>141.5199688449433</v>
+        <v>0.09753232520919694</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>11.8611188389942</v>
+        <v>0.2466834280916166</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>32.17762950924512</v>
+        <v>1.244822303279174</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>11.8962165769182</v>
+        <v>0.3123016573910503</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>180.8680827255007</v>
+        <v>42.13035515956254</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -28360,23 +28360,23 @@
       </c>
       <c r="K14" s="8" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearRegression()}</t>
+          <t>{'final_estimator': RandomForestRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>211.4180798188557</v>
+        <v>0.1018524476729634</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>13.80479179587894</v>
+        <v>0.2375961067655805</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>46.90734393893289</v>
+        <v>1.330216146713711</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>14.54022282562601</v>
+        <v>0.3191433027230298</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>180.3560819988877</v>
+        <v>40.42996014686523</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -28392,23 +28392,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>149.9371943528563</v>
+        <v>0.07420607255353387</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>12.22092795204828</v>
+        <v>0.2201516487670297</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>34.87100738104628</v>
+        <v>0.9513086449421472</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>12.24488441565931</v>
+        <v>0.2724079157321495</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>181.1298265762092</v>
+        <v>40.85233230389441</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -28422,23 +28422,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 200, 'min_samples_split': 10, 'min_samples_leaf': 2, 'min_impurity_decrease': 2, 'max_leaf_nodes': 20, 'max_features': None, 'max_depth': 20, 'learning_rate': 0.5}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>36.61515844817541</v>
+        <v>0.07420607255353387</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>4.819848867612599</v>
+        <v>0.2201516487670297</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>11.23798855580279</v>
+        <v>0.9513086449421472</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>6.051046062308187</v>
+        <v>0.2724079157321495</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>152.5493140191423</v>
+        <v>40.85233230389441</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -28454,23 +28454,23 @@
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 2, 'min_samples_leaf': 4, 'max_depth': 20}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>124.1237488817685</v>
+        <v>0.09712440047506488</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>11.03640010255528</v>
+        <v>0.2663036174247009</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>30.42428919489855</v>
+        <v>0.7664745924399317</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>11.14108382886371</v>
+        <v>0.3116478789837416</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>179.1739336362004</v>
+        <v>51.45065429099458</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -28484,23 +28484,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
+          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 2, 'max_depth': None}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>81.30849102310461</v>
+        <v>0.09905584872456591</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>8.891483968835596</v>
+        <v>0.2733843410453902</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>24.50570207971522</v>
+        <v>0.8126347132151012</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>9.017122103149353</v>
+        <v>0.3147313913872684</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>174.9140180215303</v>
+        <v>52.84315958843664</v>
       </c>
     </row>
     <row r="17">
@@ -28516,23 +28516,23 @@
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 100, 'loss': 'square', 'learning_rate': 0.01}</t>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>136.1613760406751</v>
+        <v>0.06051702901464881</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>11.54249283909001</v>
+        <v>0.2065222823214725</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>32.21106975221335</v>
+        <v>0.6412103983206281</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>11.66882067908643</v>
+        <v>0.2460020914842978</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>179.7925981725</v>
+        <v>40.40457655119</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -28546,23 +28546,23 @@
       </c>
       <c r="K17" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'loss': 'linear', 'learning_rate': 0.01}</t>
+          <t>{'n_estimators': 250, 'loss': 'linear', 'learning_rate': 0.01}</t>
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>109.9020590706382</v>
+        <v>0.07534030226728958</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>10.31399259250103</v>
+        <v>0.2225643466682358</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>28.98467186553974</v>
+        <v>0.8365806399737594</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>10.48341829131311</v>
+        <v>0.2744818796702063</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>177.6608653759161</v>
+        <v>42.17420769212681</v>
       </c>
     </row>
     <row r="18" ht="27.95" customHeight="1">
@@ -28578,23 +28578,23 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 60, 'max_samples': 1.0, 'max_features': 0.6}</t>
+          <t>{'n_estimators': 50, 'max_samples': 0.7000000000000001, 'max_features': 0.9}</t>
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>112.023845316687</v>
+        <v>0.08878245854614478</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>10.52478780306895</v>
+        <v>0.2556660582340358</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>29.35948826132876</v>
+        <v>0.817895096627811</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>10.58413176962036</v>
+        <v>0.2979638544289303</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>178.4830013689954</v>
+        <v>49.01828496189521</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -28608,23 +28608,23 @@
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 30, 'max_samples': 0.9, 'max_features': 0.7000000000000001}</t>
+          <t>{'n_estimators': 150, 'max_samples': 0.1, 'max_features': 1.0}</t>
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>80.07217359611666</v>
+        <v>0.07872922611542961</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>8.818307163122725</v>
+        <v>0.2326435853959143</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>23.84604105635131</v>
+        <v>0.867172050887019</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>8.948305627107104</v>
+        <v>0.2805872878721158</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>174.7904077185312</v>
+        <v>43.68587403446259</v>
       </c>
     </row>
     <row r="19" ht="27.95" customHeight="1">
@@ -28644,19 +28644,19 @@
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>144.1541823516042</v>
+        <v>0.133299907837532</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>11.90957129816272</v>
+        <v>0.3144979632448218</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>33.64187296414384</v>
+        <v>0.7746504426583641</v>
       </c>
       <c r="G19" s="5" t="n">
-        <v>12.00642254593783</v>
+        <v>0.3651025990561174</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>180.5124458108438</v>
+        <v>62.29948512425475</v>
       </c>
       <c r="I19" s="9" t="inlineStr">
         <is>
@@ -28674,19 +28674,19 @@
         </is>
       </c>
       <c r="L19" s="8" t="n">
-        <v>103.3896386410472</v>
+        <v>0.1013571446180372</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>10.02875836869834</v>
+        <v>0.2582551654834584</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>27.49828350791259</v>
+        <v>0.7895140971981672</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>10.1680695631495</v>
+        <v>0.3183663685410838</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>177.2844447080663</v>
+        <v>49.64492908923234</v>
       </c>
     </row>
     <row r="20" ht="42.75" customHeight="1">
@@ -29192,19 +29192,19 @@
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>156.9310339823946</v>
+        <v>0.05155044070519678</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>11.46040140654099</v>
+        <v>0.1853826313835207</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>4.716610564153942</v>
+        <v>0.4415188348668875</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>12.52721174014372</v>
+        <v>0.2270472213113316</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>132.3910770820619</v>
+        <v>32.64372814346199</v>
       </c>
       <c r="I7" s="9" t="inlineStr">
         <is>
@@ -29222,19 +29222,19 @@
         </is>
       </c>
       <c r="L7" s="8" t="n">
-        <v>163.0399925593417</v>
+        <v>0.04643063824787421</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>11.61331782367148</v>
+        <v>0.1765283236742786</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>4.827015865443597</v>
+        <v>0.4093779268321637</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>12.76871146824697</v>
+        <v>0.2154776977969512</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>132.0061906926455</v>
+        <v>31.71347222002588</v>
       </c>
     </row>
     <row r="8" ht="30.75" customHeight="1">
@@ -29250,23 +29250,23 @@
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>138.7062991209416</v>
+        <v>0.06624643068685879</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>11.76266494367776</v>
+        <v>0.2029658127467085</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>5.985634253145435</v>
+        <v>0.8587371309959917</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>11.77736384429646</v>
+        <v>0.2573838197844977</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>140.3662369569724</v>
+        <v>37.3711416026947</v>
       </c>
       <c r="I8" s="9" t="inlineStr">
         <is>
@@ -29280,23 +29280,23 @@
       </c>
       <c r="K8" s="8" t="inlineStr">
         <is>
-          <t>{'kernel': 'rbf', 'gamma': 0.01, 'C': 10}</t>
+          <t>{'kernel': 'rbf', 'gamma': 0.0001, 'C': 1}</t>
         </is>
       </c>
       <c r="L8" s="8" t="n">
-        <v>138.6018168633331</v>
+        <v>0.06624704651493001</v>
       </c>
       <c r="M8" s="8" t="n">
-        <v>11.75846213506279</v>
+        <v>0.2029664116637251</v>
       </c>
       <c r="N8" s="8" t="n">
-        <v>5.981374272414147</v>
+        <v>0.8587176347558545</v>
       </c>
       <c r="O8" s="8" t="n">
-        <v>11.77292728523085</v>
+        <v>0.2573850161041431</v>
       </c>
       <c r="P8" s="8" t="n">
-        <v>140.3553565984228</v>
+        <v>37.37135968624489</v>
       </c>
     </row>
     <row r="9" ht="45.75" customHeight="1">
@@ -29378,19 +29378,19 @@
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>155.6185727928138</v>
+        <v>0.09511229788042685</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>11.86925922495594</v>
+        <v>0.2300615051521568</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>6.047810407144868</v>
+        <v>0.7761718536437537</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>12.47471734320316</v>
+        <v>0.3084028175623998</v>
       </c>
       <c r="H10" s="5" t="n">
-        <v>136.7662086894867</v>
+        <v>44.83258393225377</v>
       </c>
       <c r="I10" s="9" t="inlineStr">
         <is>
@@ -29408,19 +29408,19 @@
         </is>
       </c>
       <c r="L10" s="8" t="n">
-        <v>130.690323130537</v>
+        <v>0.08732102881708742</v>
       </c>
       <c r="M10" s="8" t="n">
-        <v>10.74551359761878</v>
+        <v>0.2179568694532526</v>
       </c>
       <c r="N10" s="8" t="n">
-        <v>5.374159174764705</v>
+        <v>0.8803691511349324</v>
       </c>
       <c r="O10" s="8" t="n">
-        <v>11.43198684090115</v>
+        <v>0.2955013177924718</v>
       </c>
       <c r="P10" s="8" t="n">
-        <v>134.6633027056991</v>
+        <v>41.53159842237443</v>
       </c>
     </row>
     <row r="11" ht="30.75" customHeight="1">
@@ -29580,23 +29580,23 @@
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 200}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>122.3912347795116</v>
+        <v>0.05096389998989885</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>10.84332124867506</v>
+        <v>0.1855110937418041</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>5.118537474464082</v>
+        <v>0.5730349387598093</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>11.06305720763983</v>
+        <v>0.2257518548980248</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>136.776942963376</v>
+        <v>36.31733992050076</v>
       </c>
       <c r="I13" s="9" t="inlineStr">
         <is>
@@ -29610,23 +29610,23 @@
       </c>
       <c r="K13" s="8" t="inlineStr">
         <is>
-          <t>{'rf__n_estimators': 10, 'gb__n_estimators': 10}</t>
+          <t>{'rf__n_estimators': 100, 'gb__n_estimators': 10}</t>
         </is>
       </c>
       <c r="L13" s="8" t="n">
-        <v>117.5965402189461</v>
+        <v>0.05243414714328576</v>
       </c>
       <c r="M13" s="8" t="n">
-        <v>10.67417597753739</v>
+        <v>0.1845187937035802</v>
       </c>
       <c r="N13" s="8" t="n">
-        <v>5.102114388179131</v>
+        <v>0.6090120453438939</v>
       </c>
       <c r="O13" s="8" t="n">
-        <v>10.84419384827411</v>
+        <v>0.2289850369419054</v>
       </c>
       <c r="P13" s="8" t="n">
-        <v>136.1745667529457</v>
+        <v>35.98225962375968</v>
       </c>
     </row>
     <row r="14" ht="42.75" customHeight="1">
@@ -29642,23 +29642,23 @@
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>{'final_estimator': LinearRegression()}</t>
+          <t>{'final_estimator': GradientBoostingRegressor(random_state=42)}</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>103.7355154864981</v>
+        <v>0.1013301830588594</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>9.634886466953253</v>
+        <v>0.2419820842612799</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>5.581687243596258</v>
+        <v>1.041202304976041</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>10.18506335211019</v>
+        <v>0.3183240221203222</v>
       </c>
       <c r="H14" s="5" t="n">
-        <v>127.7186705053837</v>
+        <v>42.48120521982573</v>
       </c>
       <c r="I14" s="9" t="inlineStr">
         <is>
@@ -29676,19 +29676,19 @@
         </is>
       </c>
       <c r="L14" s="8" t="n">
-        <v>119.3644624972574</v>
+        <v>0.1152895303457057</v>
       </c>
       <c r="M14" s="8" t="n">
-        <v>10.1908949640637</v>
+        <v>0.2668029343219719</v>
       </c>
       <c r="N14" s="8" t="n">
-        <v>6.115775390646502</v>
+        <v>1.023768895742058</v>
       </c>
       <c r="O14" s="8" t="n">
-        <v>10.92540445463038</v>
+        <v>0.3395431200093821</v>
       </c>
       <c r="P14" s="8" t="n">
-        <v>129.6054412443564</v>
+        <v>49.47355524717001</v>
       </c>
     </row>
     <row r="15" ht="30.75" customHeight="1">
@@ -29704,23 +29704,23 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 5, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 5, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': None, 'max_features': 'sqrt', 'max_depth': 20, 'learning_rate': 1}</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>131.5956391383839</v>
+        <v>0.06894907611059664</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>11.40412117264977</v>
+        <v>0.211207802924734</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>5.777620175463793</v>
+        <v>0.8270258804249856</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>11.47151424783947</v>
+        <v>0.2625815608731821</v>
       </c>
       <c r="H15" s="5" t="n">
-        <v>138.8427146219531</v>
+        <v>39.01446122961597</v>
       </c>
       <c r="I15" s="9" t="inlineStr">
         <is>
@@ -29734,23 +29734,23 @@
       </c>
       <c r="K15" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 10, 'min_samples_leaf': 10, 'min_impurity_decrease': 2, 'max_leaf_nodes': 10, 'max_features': 'sqrt', 'max_depth': None, 'learning_rate': 0.05}</t>
+          <t>{'n_estimators': 100, 'min_samples_split': 2, 'min_samples_leaf': 2, 'min_impurity_decrease': 0, 'max_leaf_nodes': 15, 'max_features': 'sqrt', 'max_depth': 15, 'learning_rate': 0.1}</t>
         </is>
       </c>
       <c r="L15" s="8" t="n">
-        <v>125.0412777698951</v>
+        <v>0.06593423918368013</v>
       </c>
       <c r="M15" s="8" t="n">
-        <v>11.15550919225125</v>
+        <v>0.2029469697934521</v>
       </c>
       <c r="N15" s="8" t="n">
-        <v>5.674051238447214</v>
+        <v>0.8071121761284088</v>
       </c>
       <c r="O15" s="8" t="n">
-        <v>11.18218573311565</v>
+        <v>0.2567766328614816</v>
       </c>
       <c r="P15" s="8" t="n">
-        <v>138.113618916513</v>
+        <v>37.75032686991108</v>
       </c>
     </row>
     <row r="16" ht="30.75" customHeight="1">
@@ -29770,19 +29770,19 @@
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>109.1725391956389</v>
+        <v>0.07056890923587042</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>10.39693994585653</v>
+        <v>0.2181000866722641</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>5.283541521441565</v>
+        <v>0.7097864391122888</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>10.44856637035143</v>
+        <v>0.2656480928519352</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>135.0955686430214</v>
+        <v>41.17932541202556</v>
       </c>
       <c r="I16" s="9" t="inlineStr">
         <is>
@@ -29796,23 +29796,23 @@
       </c>
       <c r="K16" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 10, 'min_samples_split': 2, 'min_samples_leaf': 2, 'max_depth': None}</t>
+          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
         </is>
       </c>
       <c r="L16" s="8" t="n">
-        <v>105.9755394164171</v>
+        <v>0.07535454121409982</v>
       </c>
       <c r="M16" s="8" t="n">
-        <v>10.03452346293774</v>
+        <v>0.2244982121897985</v>
       </c>
       <c r="N16" s="8" t="n">
-        <v>5.314220084863426</v>
+        <v>0.74104614791838</v>
       </c>
       <c r="O16" s="8" t="n">
-        <v>10.29444216149749</v>
+        <v>0.2745078163078418</v>
       </c>
       <c r="P16" s="8" t="n">
-        <v>132.0196569172437</v>
+        <v>42.21994855984672</v>
       </c>
     </row>
     <row r="17" ht="42.75" customHeight="1">
@@ -29832,19 +29832,19 @@
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>141.6020948381482</v>
+        <v>0.06361744246180578</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>11.77528817415153</v>
+        <v>0.202306488808366</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>5.884378466367019</v>
+        <v>0.7217691129036868</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>11.8996678457068</v>
+        <v>0.2522249838176341</v>
       </c>
       <c r="H17" s="5" t="n">
-        <v>140.2131074073046</v>
+        <v>38.84135412708952</v>
       </c>
       <c r="I17" s="9" t="inlineStr">
         <is>
@@ -29858,23 +29858,23 @@
       </c>
       <c r="K17" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 50, 'loss': 'linear', 'learning_rate': 0.01}</t>
+          <t>{'n_estimators': 400, 'loss': 'square', 'learning_rate': 1.0}</t>
         </is>
       </c>
       <c r="L17" s="8" t="n">
-        <v>108.9731930830271</v>
+        <v>0.06641719904069573</v>
       </c>
       <c r="M17" s="8" t="n">
-        <v>10.34382192575833</v>
+        <v>0.1963903831657134</v>
       </c>
       <c r="N17" s="8" t="n">
-        <v>5.153726670093267</v>
+        <v>0.7812883960630148</v>
       </c>
       <c r="O17" s="8" t="n">
-        <v>10.43902261148174</v>
+        <v>0.2577153449849188</v>
       </c>
       <c r="P17" s="8" t="n">
-        <v>134.6742585846141</v>
+        <v>37.05617947898697</v>
       </c>
     </row>
     <row r="18" ht="56.1" customHeight="1">
@@ -29890,23 +29890,23 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>{'n_estimators': 80, 'max_samples': 0.7000000000000001, 'max_features': 0.1}</t>
+          <t>{'n_estimators': 100, 'max_samples': 1.0, 'max_features': 0.6}</t>
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>121.7490999529044</v>
+        <v>0.07762142494936972</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>10.99774026393382</v>
+        <v>0.2293397488546227</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>5.536953291759263</v>
+        <v>0.7345036496814984</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>11.03399746025458</v>
+        <v>0.2786062184327007</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>137.6002635944041</v>
+        <v>43.16979624942318</v>
       </c>
       <c r="I18" s="9" t="inlineStr">
         <is>
@@ -29920,23 +29920,23 @@
       </c>
       <c r="K18" s="8" t="inlineStr">
         <is>
-          <t>{'n_estimators': 80, 'max_samples': 0.7000000000000001, 'max_features': 0.1}</t>
+          <t>{'n_estimators': 60, 'max_samples': 1.0, 'max_features': 0.6}</t>
         </is>
       </c>
       <c r="L18" s="8" t="n">
-        <v>95.67567646403457</v>
+        <v>0.07290159252935727</v>
       </c>
       <c r="M18" s="8" t="n">
-        <v>9.729039135866635</v>
+        <v>0.220982940647136</v>
       </c>
       <c r="N18" s="8" t="n">
-        <v>4.983886694393921</v>
+        <v>0.7995539360673345</v>
       </c>
       <c r="O18" s="8" t="n">
-        <v>9.781394402846384</v>
+        <v>0.2700029491123334</v>
       </c>
       <c r="P18" s="8" t="n">
-        <v>132.0543669308058</v>
+        <v>41.11892940809664</v>
       </c>
     </row>
     <row r="19" ht="56.1" customHeight="1">
@@ -29952,53 +29952,53 @@
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
+          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>0.09271513661187851</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>0.2497451873717317</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>0.6547716900794268</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <v>0.3044916035162193</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>47.93763839752529</v>
+      </c>
+      <c r="I19" s="9" t="inlineStr">
+        <is>
+          <t>ExtraTreesRegressor</t>
+        </is>
+      </c>
+      <c r="J19" s="8" t="inlineStr">
+        <is>
+          <t>Random</t>
+        </is>
+      </c>
+      <c r="K19" s="8" t="inlineStr">
+        <is>
           <t>{'n_estimators': 100, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 20}</t>
         </is>
       </c>
-      <c r="D19" s="5" t="n">
-        <v>106.1226183818705</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <v>10.18877368548426</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>5.186947881112723</v>
-      </c>
-      <c r="G19" s="5" t="n">
-        <v>10.30158329490523</v>
-      </c>
-      <c r="H19" s="5" t="n">
-        <v>133.8100432884893</v>
-      </c>
-      <c r="I19" s="9" t="inlineStr">
-        <is>
-          <t>ExtraTreesRegressor</t>
-        </is>
-      </c>
-      <c r="J19" s="8" t="inlineStr">
-        <is>
-          <t>Random</t>
-        </is>
-      </c>
-      <c r="K19" s="8" t="inlineStr">
-        <is>
-          <t>{'n_estimators': 50, 'min_samples_split': 10, 'min_samples_leaf': 1, 'max_depth': 30}</t>
-        </is>
-      </c>
       <c r="L19" s="8" t="n">
-        <v>88.75030023591843</v>
+        <v>0.06836955627939649</v>
       </c>
       <c r="M19" s="8" t="n">
-        <v>9.330594799432527</v>
+        <v>0.2030279833838825</v>
       </c>
       <c r="N19" s="8" t="n">
-        <v>4.626579439623181</v>
+        <v>0.7853607895862844</v>
       </c>
       <c r="O19" s="8" t="n">
-        <v>9.420737775562932</v>
+        <v>0.2614757278972495</v>
       </c>
       <c r="P19" s="8" t="n">
-        <v>130.2820707047342</v>
+        <v>37.89521001414831</v>
       </c>
     </row>
     <row r="20" ht="128.25" customHeight="1">

</xml_diff>